<commit_message>
format color +Red -Green
</commit_message>
<xml_diff>
--- a/stock.xlsx
+++ b/stock.xlsx
@@ -111,9 +111,11 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <numFmts count="2">
-    <numFmt numFmtId="164" formatCode="0.000%"/>
+  <numFmts count="4">
     <numFmt numFmtId="165" formatCode="#,##0.00;[Red]#,##0.00"/>
+    <numFmt numFmtId="167" formatCode="[Red]0.00;[Green]\-0.00"/>
+    <numFmt numFmtId="169" formatCode="[Red]0.0000000;[Green]\-0.0000000"/>
+    <numFmt numFmtId="170" formatCode="[Red]0.000%;[Green]\-0.000%"/>
   </numFmts>
   <fonts count="7" x14ac:knownFonts="1">
     <font>
@@ -219,12 +221,12 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="164" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="165" fontId="6" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="167" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="167" fontId="5" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="169" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="170" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
   </cellXfs>
   <cellStyles count="31">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
@@ -589,11 +591,12 @@
   <dimension ref="A2:H8"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="125" zoomScaleNormal="125" zoomScalePageLayoutView="125" workbookViewId="0">
-      <selection activeCell="E2" sqref="E2:F2"/>
+      <selection activeCell="D12" sqref="D12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
   <cols>
+    <col min="2" max="2" width="11.83203125" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="15.1640625" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="14.1640625" customWidth="1"/>
   </cols>
@@ -645,19 +648,19 @@
       <c r="C6" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="D6" s="3">
+      <c r="D6" s="5">
         <v>716.65</v>
       </c>
-      <c r="E6" s="3">
+      <c r="E6" s="6">
         <v>3356.54</v>
       </c>
-      <c r="F6" s="3">
+      <c r="F6" s="5">
         <v>1618.98</v>
       </c>
-      <c r="G6" s="3">
+      <c r="G6" s="6">
         <v>534.94000000000005</v>
       </c>
-      <c r="H6" s="3">
+      <c r="H6" s="5">
         <v>3517.1</v>
       </c>
     </row>
@@ -682,11 +685,11 @@
       </c>
     </row>
     <row r="8" spans="1:8">
-      <c r="A8" s="4">
+      <c r="A8" s="8">
         <f>B8/F2</f>
         <v>9.783390411306268E-3</v>
       </c>
-      <c r="B8" s="3">
+      <c r="B8" s="7">
         <f>SUM(D8:M8)</f>
         <v>560.58827056784924</v>
       </c>
@@ -730,7 +733,7 @@
   <dimension ref="A2:H8"/>
   <sheetViews>
     <sheetView zoomScale="125" zoomScaleNormal="125" zoomScalePageLayoutView="125" workbookViewId="0">
-      <selection activeCell="C3" sqref="C3"/>
+      <selection activeCell="A8" sqref="A8:B8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -785,19 +788,19 @@
       <c r="C6" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="D6" s="3">
+      <c r="D6" s="5">
         <v>203.1</v>
       </c>
-      <c r="E6" s="5">
+      <c r="E6" s="6">
         <v>130.58000000000001</v>
       </c>
-      <c r="F6" s="3">
+      <c r="F6" s="5">
         <v>-82.17</v>
       </c>
-      <c r="G6" s="5">
+      <c r="G6" s="6">
         <v>537.89</v>
       </c>
-      <c r="H6" s="3">
+      <c r="H6" s="5">
         <v>34.83</v>
       </c>
     </row>
@@ -805,28 +808,28 @@
       <c r="C7" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="D7" s="8">
+      <c r="D7" s="4">
         <v>8.0500000000000007</v>
       </c>
-      <c r="E7" s="7">
+      <c r="E7" s="3">
         <v>8.2100000000000009</v>
       </c>
-      <c r="F7" s="7">
+      <c r="F7" s="3">
         <v>8.2200000000000006</v>
       </c>
-      <c r="G7" s="7">
+      <c r="G7" s="3">
         <v>8.32</v>
       </c>
-      <c r="H7" s="7">
+      <c r="H7" s="3">
         <v>8.4</v>
       </c>
     </row>
     <row r="8" spans="1:8">
-      <c r="A8" s="4">
+      <c r="A8" s="8">
         <f>B8/F2</f>
         <v>2.5690263795769344E-3</v>
       </c>
-      <c r="B8" s="3">
+      <c r="B8" s="7">
         <f>SUM(D8:M8)</f>
         <v>99.935126165542741</v>
       </c>
@@ -869,11 +872,12 @@
   <dimension ref="A2:H8"/>
   <sheetViews>
     <sheetView zoomScale="125" zoomScaleNormal="125" zoomScalePageLayoutView="125" workbookViewId="0">
-      <selection activeCell="C3" sqref="C3"/>
+      <selection activeCell="A8" sqref="A8:B8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
   <cols>
+    <col min="2" max="2" width="12.83203125" bestFit="1" customWidth="1"/>
     <col min="3" max="4" width="15.1640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
@@ -924,19 +928,19 @@
       <c r="C6" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="D6" s="3">
+      <c r="D6" s="5">
         <v>6669.91</v>
       </c>
-      <c r="E6" s="5">
+      <c r="E6" s="6">
         <v>622.99</v>
       </c>
-      <c r="F6" s="3">
+      <c r="F6" s="5">
         <v>1046.03</v>
       </c>
-      <c r="G6" s="5">
+      <c r="G6" s="6">
         <v>216.6</v>
       </c>
-      <c r="H6" s="3">
+      <c r="H6" s="5">
         <v>6596.98</v>
       </c>
     </row>
@@ -944,28 +948,28 @@
       <c r="C7" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="D7" s="8">
+      <c r="D7" s="4">
         <v>5.04</v>
       </c>
-      <c r="E7" s="7">
+      <c r="E7" s="3">
         <v>5.04</v>
       </c>
-      <c r="F7" s="7">
+      <c r="F7" s="3">
         <v>5.03</v>
       </c>
-      <c r="G7" s="7">
+      <c r="G7" s="3">
         <v>5.01</v>
       </c>
-      <c r="H7" s="7">
+      <c r="H7" s="3">
         <v>5.08</v>
       </c>
     </row>
     <row r="8" spans="1:8">
-      <c r="A8" s="4">
+      <c r="A8" s="8">
         <f>B8/F2</f>
         <v>1.845442368323997E-3</v>
       </c>
-      <c r="B8" s="3">
+      <c r="B8" s="7">
         <f>SUM(D8:M8)</f>
         <v>2996.8138619213382</v>
       </c>
@@ -1008,11 +1012,12 @@
   <dimension ref="A2:H8"/>
   <sheetViews>
     <sheetView zoomScale="125" zoomScaleNormal="125" zoomScalePageLayoutView="125" workbookViewId="0">
-      <selection activeCell="D2" sqref="D2"/>
+      <selection activeCell="A8" sqref="A8:B8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
   <cols>
+    <col min="2" max="2" width="12.83203125" bestFit="1" customWidth="1"/>
     <col min="3" max="4" width="15.1640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
@@ -1063,19 +1068,19 @@
       <c r="C6" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="D6" s="3">
+      <c r="D6" s="5">
         <v>-6879.03</v>
       </c>
-      <c r="E6" s="5">
+      <c r="E6" s="6">
         <v>2267.5500000000002</v>
       </c>
-      <c r="F6" s="3">
+      <c r="F6" s="5">
         <v>7197.26</v>
       </c>
-      <c r="G6" s="5">
+      <c r="G6" s="6">
         <v>5988.2</v>
       </c>
-      <c r="H6" s="3">
+      <c r="H6" s="5">
         <v>4570.2</v>
       </c>
     </row>
@@ -1083,28 +1088,28 @@
       <c r="C7" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="D7" s="8">
+      <c r="D7" s="4">
         <v>7.71</v>
       </c>
-      <c r="E7" s="7">
+      <c r="E7" s="3">
         <v>7.79</v>
       </c>
-      <c r="F7" s="7">
+      <c r="F7" s="3">
         <v>7.82</v>
       </c>
-      <c r="G7" s="7">
+      <c r="G7" s="3">
         <v>7.84</v>
       </c>
-      <c r="H7" s="7">
+      <c r="H7" s="3">
         <v>7.96</v>
       </c>
     </row>
     <row r="8" spans="1:8">
-      <c r="A8" s="4">
+      <c r="A8" s="8">
         <f>B8/F2</f>
         <v>7.5019258129176158E-4</v>
       </c>
-      <c r="B8" s="3">
+      <c r="B8" s="7">
         <f>SUM(D8:M8)</f>
         <v>1657.1754120735013</v>
       </c>
@@ -1147,11 +1152,12 @@
   <dimension ref="A2:H8"/>
   <sheetViews>
     <sheetView zoomScale="125" zoomScaleNormal="125" zoomScalePageLayoutView="125" workbookViewId="0">
-      <selection activeCell="C2" sqref="C2"/>
+      <selection activeCell="A8" sqref="A8:B8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
   <cols>
+    <col min="2" max="2" width="13.5" bestFit="1" customWidth="1"/>
     <col min="3" max="4" width="15.1640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
@@ -1202,19 +1208,19 @@
       <c r="C6" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="D6" s="3">
+      <c r="D6" s="5">
         <v>-3240.47</v>
       </c>
-      <c r="E6" s="5">
+      <c r="E6" s="6">
         <v>-9894.83</v>
       </c>
-      <c r="F6" s="3">
+      <c r="F6" s="5">
         <v>295.26</v>
       </c>
-      <c r="G6" s="5">
+      <c r="G6" s="6">
         <v>-10161.91</v>
       </c>
-      <c r="H6" s="3">
+      <c r="H6" s="5">
         <v>-2626</v>
       </c>
     </row>
@@ -1222,28 +1228,28 @@
       <c r="C7" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="D7" s="8">
+      <c r="D7" s="4">
         <v>8.18</v>
       </c>
-      <c r="E7" s="7">
+      <c r="E7" s="3">
         <v>8.18</v>
       </c>
-      <c r="F7" s="7">
+      <c r="F7" s="3">
         <v>8.23</v>
       </c>
-      <c r="G7" s="7">
+      <c r="G7" s="3">
         <v>8.17</v>
       </c>
-      <c r="H7" s="7">
+      <c r="H7" s="3">
         <v>8.2200000000000006</v>
       </c>
     </row>
     <row r="8" spans="1:8">
-      <c r="A8" s="4">
+      <c r="A8" s="8">
         <f>B8/F2</f>
         <v>-1.0602256654833931E-3</v>
       </c>
-      <c r="B8" s="3">
+      <c r="B8" s="7">
         <f>SUM(D8:M8)</f>
         <v>-3133.1788866365232</v>
       </c>
@@ -1286,11 +1292,12 @@
   <dimension ref="A2:H8"/>
   <sheetViews>
     <sheetView zoomScale="125" zoomScaleNormal="125" zoomScalePageLayoutView="125" workbookViewId="0">
-      <selection activeCell="C3" sqref="C3"/>
+      <selection activeCell="A8" sqref="A8:B8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
   <cols>
+    <col min="2" max="2" width="12.83203125" bestFit="1" customWidth="1"/>
     <col min="3" max="4" width="15.1640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
@@ -1341,19 +1348,19 @@
       <c r="C6" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="D6" s="3">
+      <c r="D6" s="5">
         <v>-1260.6400000000001</v>
       </c>
-      <c r="E6" s="5">
+      <c r="E6" s="6">
         <v>814.23</v>
       </c>
-      <c r="F6" s="3">
+      <c r="F6" s="5">
         <v>544.08000000000004</v>
       </c>
-      <c r="G6" s="5">
+      <c r="G6" s="6">
         <v>92.02</v>
       </c>
-      <c r="H6" s="3">
+      <c r="H6" s="5">
         <v>4107.3900000000003</v>
       </c>
     </row>
@@ -1361,28 +1368,28 @@
       <c r="C7" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="D7" s="8">
+      <c r="D7" s="4">
         <v>3.04</v>
       </c>
-      <c r="E7" s="7">
+      <c r="E7" s="3">
         <v>3.09</v>
       </c>
-      <c r="F7" s="7">
+      <c r="F7" s="3">
         <v>3.12</v>
       </c>
-      <c r="G7" s="7">
+      <c r="G7" s="3">
         <v>3.15</v>
       </c>
-      <c r="H7" s="7">
+      <c r="H7" s="3">
         <v>3.25</v>
       </c>
     </row>
     <row r="8" spans="1:8">
-      <c r="A8" s="4">
+      <c r="A8" s="8">
         <f>B8/F2</f>
         <v>7.0311445797662268E-3</v>
       </c>
-      <c r="B8" s="3">
+      <c r="B8" s="7">
         <f>SUM(D8:M8)</f>
         <v>1316.2302653322377</v>
       </c>
@@ -1425,11 +1432,12 @@
   <dimension ref="A2:H8"/>
   <sheetViews>
     <sheetView zoomScale="125" zoomScaleNormal="125" zoomScalePageLayoutView="125" workbookViewId="0">
-      <selection activeCell="C3" sqref="C3"/>
+      <selection activeCell="A8" sqref="A8:B8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
   <cols>
+    <col min="2" max="2" width="11.83203125" bestFit="1" customWidth="1"/>
     <col min="3" max="4" width="15.1640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
@@ -1480,19 +1488,19 @@
       <c r="C6" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="D6" s="3">
+      <c r="D6" s="5">
         <v>-296.07</v>
       </c>
-      <c r="E6" s="5">
+      <c r="E6" s="6">
         <v>191.78</v>
       </c>
-      <c r="F6" s="3">
+      <c r="F6" s="5">
         <v>355.5</v>
       </c>
-      <c r="G6" s="5">
+      <c r="G6" s="6">
         <v>1391.63</v>
       </c>
-      <c r="H6" s="3">
+      <c r="H6" s="5">
         <v>1681.46</v>
       </c>
     </row>
@@ -1500,28 +1508,28 @@
       <c r="C7" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="D7" s="8">
+      <c r="D7" s="4">
         <v>4.37</v>
       </c>
-      <c r="E7" s="7">
+      <c r="E7" s="3">
         <v>4.4400000000000004</v>
       </c>
-      <c r="F7" s="7">
+      <c r="F7" s="3">
         <v>4.43</v>
       </c>
-      <c r="G7" s="7">
+      <c r="G7" s="3">
         <v>4.49</v>
       </c>
-      <c r="H7" s="7">
+      <c r="H7" s="3">
         <v>4.51</v>
       </c>
     </row>
     <row r="8" spans="1:8">
-      <c r="A8" s="4">
+      <c r="A8" s="8">
         <f>B8/F2</f>
         <v>4.413990216804841E-3</v>
       </c>
-      <c r="B8" s="3">
+      <c r="B8" s="7">
         <f>SUM(D8:M8)</f>
         <v>738.46056327144993</v>
       </c>
@@ -1564,7 +1572,7 @@
   <dimension ref="A2:H8"/>
   <sheetViews>
     <sheetView zoomScale="125" zoomScaleNormal="125" zoomScalePageLayoutView="125" workbookViewId="0">
-      <selection activeCell="C3" sqref="C3"/>
+      <selection activeCell="A8" sqref="A8:B8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -1619,19 +1627,19 @@
       <c r="C6" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="D6" s="3">
+      <c r="D6" s="5">
         <v>77.569999999999993</v>
       </c>
-      <c r="E6" s="5">
+      <c r="E6" s="6">
         <v>214.59</v>
       </c>
-      <c r="F6" s="3">
+      <c r="F6" s="5">
         <v>79.16</v>
       </c>
-      <c r="G6" s="5">
+      <c r="G6" s="6">
         <v>44.29</v>
       </c>
-      <c r="H6" s="3">
+      <c r="H6" s="5">
         <v>75.2</v>
       </c>
     </row>
@@ -1639,28 +1647,28 @@
       <c r="C7" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="D7" s="8">
+      <c r="D7" s="4">
         <v>5.72</v>
       </c>
-      <c r="E7" s="7">
+      <c r="E7" s="3">
         <v>5.86</v>
       </c>
-      <c r="F7" s="7">
+      <c r="F7" s="3">
         <v>5.9</v>
       </c>
-      <c r="G7" s="7">
+      <c r="G7" s="3">
         <v>5.93</v>
       </c>
-      <c r="H7" s="7">
+      <c r="H7" s="3">
         <v>5.95</v>
       </c>
     </row>
     <row r="8" spans="1:8">
-      <c r="A8" s="4">
+      <c r="A8" s="8">
         <f>B8/F2</f>
         <v>1.5500935194254768E-3</v>
       </c>
-      <c r="B8" s="3">
+      <c r="B8" s="7">
         <f>SUM(D8:M8)</f>
         <v>83.70505004897575</v>
       </c>
@@ -1703,7 +1711,7 @@
   <dimension ref="A2:H8"/>
   <sheetViews>
     <sheetView zoomScale="125" zoomScaleNormal="125" zoomScalePageLayoutView="125" workbookViewId="0">
-      <selection activeCell="C3" sqref="C3"/>
+      <selection activeCell="A8" sqref="A8:B8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -1758,19 +1766,19 @@
       <c r="C6" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="D6" s="3">
+      <c r="D6" s="5">
         <v>-420.05</v>
       </c>
-      <c r="E6" s="5">
+      <c r="E6" s="6">
         <v>103.51</v>
       </c>
-      <c r="F6" s="3">
+      <c r="F6" s="5">
         <v>1590.33</v>
       </c>
-      <c r="G6" s="5">
+      <c r="G6" s="6">
         <v>-1058.44</v>
       </c>
-      <c r="H6" s="3">
+      <c r="H6" s="5">
         <v>0</v>
       </c>
     </row>
@@ -1778,28 +1786,28 @@
       <c r="C7" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="D7" s="8">
+      <c r="D7" s="4">
         <v>12.31</v>
       </c>
-      <c r="E7" s="7">
+      <c r="E7" s="3">
         <v>12.09</v>
       </c>
-      <c r="F7" s="7">
+      <c r="F7" s="3">
         <v>12.17</v>
       </c>
-      <c r="G7" s="7">
+      <c r="G7" s="3">
         <v>11.14</v>
       </c>
-      <c r="H7" s="7">
+      <c r="H7" s="3">
         <v>12.22</v>
       </c>
     </row>
     <row r="8" spans="1:8">
-      <c r="A8" s="4">
+      <c r="A8" s="8">
         <f>B8/F2</f>
         <v>3.269463569744558E-4</v>
       </c>
-      <c r="B8" s="3">
+      <c r="B8" s="7">
         <f>SUM(D8:M8)</f>
         <v>10.102642430510684</v>
       </c>
@@ -1842,11 +1850,12 @@
   <dimension ref="A2:H8"/>
   <sheetViews>
     <sheetView zoomScale="125" zoomScaleNormal="125" zoomScalePageLayoutView="125" workbookViewId="0">
-      <selection activeCell="E3" sqref="E3"/>
+      <selection activeCell="A8" sqref="A8:B8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
   <cols>
+    <col min="2" max="2" width="13" customWidth="1"/>
     <col min="3" max="4" width="15.1640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
@@ -1897,19 +1906,19 @@
       <c r="C6" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="D6" s="3">
+      <c r="D6" s="5">
         <v>-1286.24</v>
       </c>
-      <c r="E6" s="5">
+      <c r="E6" s="6">
         <v>786.76</v>
       </c>
-      <c r="F6" s="3">
+      <c r="F6" s="5">
         <v>584.53</v>
       </c>
-      <c r="G6" s="5">
+      <c r="G6" s="6">
         <v>860.62</v>
       </c>
-      <c r="H6" s="3">
+      <c r="H6" s="5">
         <v>0</v>
       </c>
     </row>
@@ -1917,28 +1926,28 @@
       <c r="C7" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="D7" s="8">
+      <c r="D7" s="4">
         <v>5.41</v>
       </c>
-      <c r="E7" s="7">
+      <c r="E7" s="3">
         <v>5.41</v>
       </c>
-      <c r="F7" s="7">
+      <c r="F7" s="3">
         <v>5.45</v>
       </c>
-      <c r="G7" s="7">
+      <c r="G7" s="3">
         <v>5.49</v>
       </c>
-      <c r="H7" s="7">
+      <c r="H7" s="3">
         <v>12.22</v>
       </c>
     </row>
     <row r="8" spans="1:8">
-      <c r="A8" s="4">
+      <c r="A8" s="8">
         <f>B8/F2</f>
         <v>1.4624299137076912E-3</v>
       </c>
-      <c r="B8" s="3">
+      <c r="B8" s="7">
         <f>SUM(D8:M8)</f>
         <v>171.68927186928295</v>
       </c>
@@ -1981,11 +1990,12 @@
   <dimension ref="A2:H8"/>
   <sheetViews>
     <sheetView zoomScale="125" zoomScaleNormal="125" zoomScalePageLayoutView="125" workbookViewId="0">
-      <selection sqref="A1:XFD1048576"/>
+      <selection activeCell="A8" sqref="A8:B8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
   <cols>
+    <col min="2" max="2" width="13.5" bestFit="1" customWidth="1"/>
     <col min="3" max="4" width="15.1640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
@@ -2039,16 +2049,16 @@
       <c r="D6" s="5">
         <v>-14643.97</v>
       </c>
-      <c r="E6" s="5">
+      <c r="E6" s="6">
         <v>-261.02</v>
       </c>
       <c r="F6" s="5">
         <v>-3748.62</v>
       </c>
-      <c r="G6" s="5">
+      <c r="G6" s="6">
         <v>-3807.77</v>
       </c>
-      <c r="H6" s="3">
+      <c r="H6" s="5">
         <v>1312.78</v>
       </c>
     </row>
@@ -2073,11 +2083,11 @@
       </c>
     </row>
     <row r="8" spans="1:8">
-      <c r="A8" s="6">
+      <c r="A8" s="8">
         <f>B8/F2</f>
         <v>-6.5831381327964636E-3</v>
       </c>
-      <c r="B8" s="5">
+      <c r="B8" s="7">
         <f>SUM(D8:M8)</f>
         <v>-5221.7451669341544</v>
       </c>
@@ -2121,11 +2131,12 @@
   <dimension ref="A2:H8"/>
   <sheetViews>
     <sheetView zoomScale="125" zoomScaleNormal="125" zoomScalePageLayoutView="125" workbookViewId="0">
-      <selection sqref="A1:XFD1048576"/>
+      <selection activeCell="A8" sqref="A8:B8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
   <cols>
+    <col min="2" max="2" width="13.5" bestFit="1" customWidth="1"/>
     <col min="3" max="4" width="15.1640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
@@ -2179,13 +2190,13 @@
       <c r="D6" s="5">
         <v>-21881.24</v>
       </c>
-      <c r="E6" s="3">
+      <c r="E6" s="6">
         <v>9170.2999999999993</v>
       </c>
-      <c r="F6" s="3">
+      <c r="F6" s="5">
         <v>357.95</v>
       </c>
-      <c r="G6" s="3">
+      <c r="G6" s="6">
         <v>5057.8599999999997</v>
       </c>
       <c r="H6" s="5">
@@ -2213,11 +2224,11 @@
       </c>
     </row>
     <row r="8" spans="1:8">
-      <c r="A8" s="6">
+      <c r="A8" s="8">
         <f>B8/F2</f>
         <v>-1.5238955333729573E-3</v>
       </c>
-      <c r="B8" s="5">
+      <c r="B8" s="7">
         <f>SUM(D8:M8)</f>
         <v>-3358.5133660006604</v>
       </c>
@@ -2261,11 +2272,12 @@
   <dimension ref="A2:H8"/>
   <sheetViews>
     <sheetView zoomScale="125" zoomScaleNormal="125" zoomScalePageLayoutView="125" workbookViewId="0">
-      <selection sqref="A1:XFD1048576"/>
+      <selection activeCell="A8" sqref="A8:B8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
   <cols>
+    <col min="2" max="2" width="12.5" bestFit="1" customWidth="1"/>
     <col min="3" max="4" width="15.1640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
@@ -2319,13 +2331,13 @@
       <c r="D6" s="5">
         <v>-2926.17</v>
       </c>
-      <c r="E6" s="5">
+      <c r="E6" s="6">
         <v>-729.21</v>
       </c>
-      <c r="F6" s="3">
+      <c r="F6" s="5">
         <v>571.54</v>
       </c>
-      <c r="G6" s="5">
+      <c r="G6" s="6">
         <v>-70.55</v>
       </c>
       <c r="H6" s="5">
@@ -2353,11 +2365,11 @@
       </c>
     </row>
     <row r="8" spans="1:8">
-      <c r="A8" s="6">
+      <c r="A8" s="8">
         <f>B8/F2</f>
         <v>-5.920097179474954E-3</v>
       </c>
-      <c r="B8" s="5">
+      <c r="B8" s="7">
         <f>SUM(D8:M8)</f>
         <v>-568.3293292295956</v>
       </c>
@@ -2401,11 +2413,12 @@
   <dimension ref="A2:H8"/>
   <sheetViews>
     <sheetView zoomScale="125" zoomScaleNormal="125" zoomScalePageLayoutView="125" workbookViewId="0">
-      <selection sqref="A1:XFD1048576"/>
+      <selection activeCell="A8" sqref="A8:B8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
   <cols>
+    <col min="2" max="2" width="12.83203125" bestFit="1" customWidth="1"/>
     <col min="3" max="4" width="15.1640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
@@ -2456,16 +2469,16 @@
       <c r="C6" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="D6" s="3">
+      <c r="D6" s="5">
         <v>12051.06</v>
       </c>
-      <c r="E6" s="3">
+      <c r="E6" s="6">
         <v>4064.21</v>
       </c>
       <c r="F6" s="5">
         <v>-5780.02</v>
       </c>
-      <c r="G6" s="3">
+      <c r="G6" s="6">
         <v>5066.84</v>
       </c>
       <c r="H6" s="5">
@@ -2476,28 +2489,28 @@
       <c r="C7" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="D7" s="8">
+      <c r="D7" s="4">
         <v>6</v>
       </c>
-      <c r="E7" s="7">
+      <c r="E7" s="3">
         <v>5.98</v>
       </c>
-      <c r="F7" s="7">
+      <c r="F7" s="3">
         <v>5.97</v>
       </c>
-      <c r="G7" s="7">
+      <c r="G7" s="3">
         <v>5.92</v>
       </c>
-      <c r="H7" s="7">
+      <c r="H7" s="3">
         <v>5.94</v>
       </c>
     </row>
     <row r="8" spans="1:8">
-      <c r="A8" s="4">
+      <c r="A8" s="8">
         <f>B8/F2</f>
         <v>1.2990818272522878E-4</v>
       </c>
-      <c r="B8" s="3">
+      <c r="B8" s="7">
         <f>SUM(D8:M8)</f>
         <v>1241.3766124857411</v>
       </c>
@@ -2541,11 +2554,12 @@
   <dimension ref="A2:H8"/>
   <sheetViews>
     <sheetView zoomScale="125" zoomScaleNormal="125" zoomScalePageLayoutView="125" workbookViewId="0">
-      <selection sqref="A1:XFD1048576"/>
+      <selection activeCell="A8" sqref="A8:B8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
   <cols>
+    <col min="2" max="2" width="11.83203125" bestFit="1" customWidth="1"/>
     <col min="3" max="4" width="15.1640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
@@ -2596,16 +2610,16 @@
       <c r="C6" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="D6" s="3">
+      <c r="D6" s="5">
         <v>47.13</v>
       </c>
-      <c r="E6" s="3">
+      <c r="E6" s="6">
         <v>340.97</v>
       </c>
       <c r="F6" s="5">
         <v>-32.82</v>
       </c>
-      <c r="G6" s="3">
+      <c r="G6" s="6">
         <v>3671.71</v>
       </c>
       <c r="H6" s="5">
@@ -2616,28 +2630,28 @@
       <c r="C7" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="D7" s="8">
+      <c r="D7" s="4">
         <v>16.45</v>
       </c>
-      <c r="E7" s="7">
+      <c r="E7" s="3">
         <v>16.61</v>
       </c>
-      <c r="F7" s="7">
+      <c r="F7" s="3">
         <v>16.690000000000001</v>
       </c>
-      <c r="G7" s="7">
+      <c r="G7" s="3">
         <v>18.36</v>
       </c>
-      <c r="H7" s="7">
+      <c r="H7" s="3">
         <v>18.41</v>
       </c>
     </row>
     <row r="8" spans="1:8">
-      <c r="A8" s="4">
+      <c r="A8" s="8">
         <f>B8/F2</f>
         <v>5.1096127334663687E-3</v>
       </c>
-      <c r="B8" s="3">
+      <c r="B8" s="7">
         <f>SUM(D8:M8)</f>
         <v>206.93931570538794</v>
       </c>
@@ -2681,11 +2695,12 @@
   <dimension ref="A2:H8"/>
   <sheetViews>
     <sheetView zoomScale="125" zoomScaleNormal="125" zoomScalePageLayoutView="125" workbookViewId="0">
-      <selection sqref="A1:XFD1048576"/>
+      <selection activeCell="A8" sqref="A8:B8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
   <cols>
+    <col min="2" max="2" width="11.5" bestFit="1" customWidth="1"/>
     <col min="3" max="4" width="15.1640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
@@ -2736,19 +2751,19 @@
       <c r="C6" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="D6" s="3">
+      <c r="D6" s="5">
         <v>1074.42</v>
       </c>
-      <c r="E6" s="5">
+      <c r="E6" s="6">
         <v>-3820.16</v>
       </c>
-      <c r="F6" s="3">
+      <c r="F6" s="5">
         <v>1339.85</v>
       </c>
-      <c r="G6" s="5">
+      <c r="G6" s="6">
         <v>-1621.19</v>
       </c>
-      <c r="H6" s="3">
+      <c r="H6" s="5">
         <v>2580.94</v>
       </c>
     </row>
@@ -2756,28 +2771,28 @@
       <c r="C7" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="D7" s="8">
+      <c r="D7" s="4">
         <v>10.61</v>
       </c>
-      <c r="E7" s="7">
+      <c r="E7" s="3">
         <v>10.5</v>
       </c>
-      <c r="F7" s="7">
+      <c r="F7" s="3">
         <v>10.58</v>
       </c>
-      <c r="G7" s="7">
+      <c r="G7" s="3">
         <v>10.39</v>
       </c>
-      <c r="H7" s="7">
+      <c r="H7" s="3">
         <v>10.55</v>
       </c>
     </row>
     <row r="8" spans="1:8">
-      <c r="A8" s="6">
+      <c r="A8" s="8">
         <f>B8/F2</f>
         <v>-5.0550058245195264E-4</v>
       </c>
-      <c r="B8" s="5">
+      <c r="B8" s="7">
         <f>SUM(D8:M8)</f>
         <v>-47.314854517502766</v>
       </c>
@@ -2821,7 +2836,7 @@
   <dimension ref="A2:H8"/>
   <sheetViews>
     <sheetView zoomScale="125" zoomScaleNormal="125" zoomScalePageLayoutView="125" workbookViewId="0">
-      <selection activeCell="D7" sqref="D7"/>
+      <selection activeCell="A8" sqref="A8:B8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -2876,19 +2891,19 @@
       <c r="C6" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="D6" s="3">
+      <c r="D6" s="5">
         <v>-5587.2</v>
       </c>
-      <c r="E6" s="5">
+      <c r="E6" s="6">
         <v>321.14999999999998</v>
       </c>
-      <c r="F6" s="3">
+      <c r="F6" s="5">
         <v>451.41</v>
       </c>
-      <c r="G6" s="5">
+      <c r="G6" s="6">
         <v>7513.55</v>
       </c>
-      <c r="H6" s="3">
+      <c r="H6" s="5">
         <v>-1473.72</v>
       </c>
     </row>
@@ -2896,28 +2911,28 @@
       <c r="C7" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="D7" s="8">
+      <c r="D7" s="4">
         <v>11.5</v>
       </c>
-      <c r="E7" s="7">
+      <c r="E7" s="3">
         <v>11.5</v>
       </c>
-      <c r="F7" s="7">
+      <c r="F7" s="3">
         <v>11.7</v>
       </c>
-      <c r="G7" s="7">
+      <c r="G7" s="3">
         <v>12.33</v>
       </c>
-      <c r="H7" s="7">
+      <c r="H7" s="3">
         <v>12.22</v>
       </c>
     </row>
     <row r="8" spans="1:8">
-      <c r="A8" s="4">
+      <c r="A8" s="8">
         <f>B8/F2</f>
         <v>9.9480076960092542E-4</v>
       </c>
-      <c r="B8" s="3">
+      <c r="B8" s="7">
         <f>SUM(D8:M8)</f>
         <v>69.437093718144595</v>
       </c>
@@ -2961,11 +2976,12 @@
   <dimension ref="A2:H8"/>
   <sheetViews>
     <sheetView zoomScale="125" zoomScaleNormal="125" zoomScalePageLayoutView="125" workbookViewId="0">
-      <selection activeCell="E3" sqref="E3"/>
+      <selection activeCell="A8" sqref="A8:B8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
   <cols>
+    <col min="2" max="2" width="11.83203125" bestFit="1" customWidth="1"/>
     <col min="3" max="4" width="15.1640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
@@ -3016,19 +3032,19 @@
       <c r="C6" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="D6" s="3">
+      <c r="D6" s="5">
         <v>1560.66</v>
       </c>
-      <c r="E6" s="5">
+      <c r="E6" s="6">
         <v>640.62</v>
       </c>
-      <c r="F6" s="3">
+      <c r="F6" s="5">
         <v>-863.63</v>
       </c>
-      <c r="G6" s="5">
+      <c r="G6" s="6">
         <v>400.78</v>
       </c>
-      <c r="H6" s="3">
+      <c r="H6" s="5">
         <v>-144.65</v>
       </c>
     </row>
@@ -3036,28 +3052,28 @@
       <c r="C7" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="D7" s="8">
+      <c r="D7" s="4">
         <v>4.28</v>
       </c>
-      <c r="E7" s="7">
+      <c r="E7" s="3">
         <v>4.3899999999999997</v>
       </c>
-      <c r="F7" s="7">
+      <c r="F7" s="3">
         <v>4.3</v>
       </c>
-      <c r="G7" s="7">
+      <c r="G7" s="3">
         <v>4.34</v>
       </c>
-      <c r="H7" s="7">
+      <c r="H7" s="3">
         <v>4.3499999999999996</v>
       </c>
     </row>
     <row r="8" spans="1:8">
-      <c r="A8" s="4">
+      <c r="A8" s="8">
         <f>B8/F2</f>
         <v>1.8552105457116546E-3</v>
       </c>
-      <c r="B8" s="3">
+      <c r="B8" s="7">
         <f>SUM(D8:M8)</f>
         <v>368.81585648747694</v>
       </c>

</xml_diff>

<commit_message>
add sum of pure money
</commit_message>
<xml_diff>
--- a/stock.xlsx
+++ b/stock.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="26405"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="16060" tabRatio="954" activeTab="15"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="16060" tabRatio="954" activeTab="17"/>
   </bookViews>
   <sheets>
     <sheet name="达华智能" sheetId="1" r:id="rId1"/>
@@ -269,7 +269,7 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="15">
+  <cellXfs count="16">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
@@ -285,6 +285,7 @@
     <xf numFmtId="16" fontId="8" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="37">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
@@ -658,7 +659,7 @@
   <dimension ref="A2:K8"/>
   <sheetViews>
     <sheetView zoomScale="125" zoomScaleNormal="125" zoomScalePageLayoutView="125" workbookViewId="0">
-      <selection activeCell="K8" sqref="K8"/>
+      <selection activeCell="C6" sqref="C6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -721,6 +722,10 @@
       </c>
     </row>
     <row r="6" spans="1:11">
+      <c r="B6" s="15">
+        <f>SUM(D6:MI6)</f>
+        <v>13651.52</v>
+      </c>
       <c r="C6" s="1" t="s">
         <v>2</v>
       </c>
@@ -839,7 +844,7 @@
   <dimension ref="A2:K8"/>
   <sheetViews>
     <sheetView zoomScale="125" zoomScaleNormal="125" zoomScalePageLayoutView="125" workbookViewId="0">
-      <selection activeCell="K7" sqref="K7"/>
+      <selection activeCell="B7" sqref="B7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -901,6 +906,10 @@
       </c>
     </row>
     <row r="6" spans="1:11">
+      <c r="B6" s="15">
+        <f>SUM(D6:MI6)</f>
+        <v>481.52</v>
+      </c>
       <c r="C6" s="1" t="s">
         <v>2</v>
       </c>
@@ -1018,7 +1027,7 @@
   <dimension ref="A2:K8"/>
   <sheetViews>
     <sheetView zoomScale="125" zoomScaleNormal="125" zoomScalePageLayoutView="125" workbookViewId="0">
-      <selection activeCell="K7" sqref="K7"/>
+      <selection activeCell="B7" sqref="B7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -1080,6 +1089,10 @@
       </c>
     </row>
     <row r="6" spans="1:11">
+      <c r="B6" s="15">
+        <f>SUM(D6:MI6)</f>
+        <v>12577.31</v>
+      </c>
       <c r="C6" s="1" t="s">
         <v>2</v>
       </c>
@@ -1197,7 +1210,7 @@
   <dimension ref="A2:K8"/>
   <sheetViews>
     <sheetView zoomScale="125" zoomScaleNormal="125" zoomScalePageLayoutView="125" workbookViewId="0">
-      <selection activeCell="K7" sqref="K7"/>
+      <selection activeCell="B7" sqref="B7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -1259,6 +1272,10 @@
       </c>
     </row>
     <row r="6" spans="1:11">
+      <c r="B6" s="15">
+        <f>SUM(D6:MI6)</f>
+        <v>31603.15</v>
+      </c>
       <c r="C6" s="1" t="s">
         <v>2</v>
       </c>
@@ -1376,7 +1393,7 @@
   <dimension ref="A2:K8"/>
   <sheetViews>
     <sheetView zoomScale="125" zoomScaleNormal="125" zoomScalePageLayoutView="125" workbookViewId="0">
-      <selection activeCell="K7" sqref="K7"/>
+      <selection activeCell="B7" sqref="B7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -1438,6 +1455,10 @@
       </c>
     </row>
     <row r="6" spans="1:11">
+      <c r="B6" s="15">
+        <f>SUM(D6:MI6)</f>
+        <v>-30005.739999999998</v>
+      </c>
       <c r="C6" s="1" t="s">
         <v>2</v>
       </c>
@@ -1555,7 +1576,7 @@
   <dimension ref="A2:K8"/>
   <sheetViews>
     <sheetView zoomScale="125" zoomScaleNormal="125" zoomScalePageLayoutView="125" workbookViewId="0">
-      <selection activeCell="K7" sqref="K7"/>
+      <selection activeCell="B7" sqref="B7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -1617,6 +1638,10 @@
       </c>
     </row>
     <row r="6" spans="1:11">
+      <c r="B6" s="15">
+        <f>SUM(D6:MI6)</f>
+        <v>1062.8700000000001</v>
+      </c>
       <c r="C6" s="1" t="s">
         <v>2</v>
       </c>
@@ -1734,7 +1759,7 @@
   <dimension ref="A2:K8"/>
   <sheetViews>
     <sheetView zoomScale="125" zoomScaleNormal="125" zoomScalePageLayoutView="125" workbookViewId="0">
-      <selection activeCell="K7" sqref="K7"/>
+      <selection activeCell="B7" sqref="B7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -1796,6 +1821,10 @@
       </c>
     </row>
     <row r="6" spans="1:11">
+      <c r="B6" s="15">
+        <f>SUM(D6:MI6)</f>
+        <v>6146.6100000000006</v>
+      </c>
       <c r="C6" s="1" t="s">
         <v>2</v>
       </c>
@@ -1912,8 +1941,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A2:K8"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="125" zoomScaleNormal="125" zoomScalePageLayoutView="125" workbookViewId="0">
-      <selection activeCell="K7" sqref="K7"/>
+    <sheetView zoomScale="125" zoomScaleNormal="125" zoomScalePageLayoutView="125" workbookViewId="0">
+      <selection activeCell="B7" sqref="B7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -1975,6 +2004,10 @@
       </c>
     </row>
     <row r="6" spans="1:11">
+      <c r="B6" s="15">
+        <f>SUM(D6:MI6)</f>
+        <v>-88.340000000000032</v>
+      </c>
       <c r="C6" s="1" t="s">
         <v>2</v>
       </c>
@@ -2092,7 +2125,7 @@
   <dimension ref="A2:H8"/>
   <sheetViews>
     <sheetView zoomScale="125" zoomScaleNormal="125" zoomScalePageLayoutView="125" workbookViewId="0">
-      <selection activeCell="A8" sqref="A8:B8"/>
+      <selection activeCell="B7" sqref="B7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -2144,6 +2177,10 @@
       </c>
     </row>
     <row r="6" spans="1:8">
+      <c r="B6" s="15">
+        <f>SUM(D6:MI6)</f>
+        <v>215.34999999999991</v>
+      </c>
       <c r="C6" s="1" t="s">
         <v>2</v>
       </c>
@@ -2230,8 +2267,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A2:H8"/>
   <sheetViews>
-    <sheetView zoomScale="125" zoomScaleNormal="125" zoomScalePageLayoutView="125" workbookViewId="0">
-      <selection activeCell="F31" sqref="F31"/>
+    <sheetView tabSelected="1" zoomScale="125" zoomScaleNormal="125" zoomScalePageLayoutView="125" workbookViewId="0">
+      <selection activeCell="B7" sqref="B7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -2284,6 +2321,10 @@
       </c>
     </row>
     <row r="6" spans="1:8">
+      <c r="B6" s="15">
+        <f>SUM(D6:MI6)</f>
+        <v>945.67</v>
+      </c>
       <c r="C6" s="1" t="s">
         <v>2</v>
       </c>
@@ -2371,7 +2412,7 @@
   <dimension ref="A2:K15"/>
   <sheetViews>
     <sheetView zoomScale="125" zoomScaleNormal="125" zoomScalePageLayoutView="125" workbookViewId="0">
-      <selection activeCell="K7" sqref="K7"/>
+      <selection activeCell="C6" sqref="C6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -2433,6 +2474,10 @@
       </c>
     </row>
     <row r="6" spans="1:11">
+      <c r="B6" s="15">
+        <f>SUM(D6:MI6)</f>
+        <v>-21575.31</v>
+      </c>
       <c r="C6" s="1" t="s">
         <v>2</v>
       </c>
@@ -2567,7 +2612,7 @@
   <dimension ref="A2:K8"/>
   <sheetViews>
     <sheetView zoomScale="125" zoomScaleNormal="125" zoomScalePageLayoutView="125" workbookViewId="0">
-      <selection activeCell="K7" sqref="K7"/>
+      <selection activeCell="B7" sqref="B7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -2629,6 +2674,10 @@
       </c>
     </row>
     <row r="6" spans="1:11">
+      <c r="B6" s="15">
+        <f>SUM(D6:MI6)</f>
+        <v>-10408.580000000002</v>
+      </c>
       <c r="C6" s="1" t="s">
         <v>2</v>
       </c>
@@ -2747,7 +2796,7 @@
   <dimension ref="A2:K15"/>
   <sheetViews>
     <sheetView zoomScale="125" zoomScaleNormal="125" zoomScalePageLayoutView="125" workbookViewId="0">
-      <selection activeCell="K7" sqref="K7"/>
+      <selection activeCell="B7" sqref="B7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -2809,6 +2858,10 @@
       </c>
     </row>
     <row r="6" spans="1:11">
+      <c r="B6" s="15">
+        <f>SUM(D6:MI6)</f>
+        <v>-4272.87</v>
+      </c>
       <c r="C6" s="1" t="s">
         <v>2</v>
       </c>
@@ -2937,7 +2990,7 @@
   <dimension ref="A2:K8"/>
   <sheetViews>
     <sheetView zoomScale="125" zoomScaleNormal="125" zoomScalePageLayoutView="125" workbookViewId="0">
-      <selection activeCell="K7" sqref="K7"/>
+      <selection activeCell="B7" sqref="B7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -2999,6 +3052,10 @@
       </c>
     </row>
     <row r="6" spans="1:11">
+      <c r="B6" s="15">
+        <f>SUM(D6:MI6)</f>
+        <v>31212.69</v>
+      </c>
       <c r="C6" s="1" t="s">
         <v>2</v>
       </c>
@@ -3120,7 +3177,7 @@
   <dimension ref="A2:K8"/>
   <sheetViews>
     <sheetView zoomScale="125" zoomScaleNormal="125" zoomScalePageLayoutView="125" workbookViewId="0">
-      <selection activeCell="K7" sqref="K7"/>
+      <selection activeCell="B7" sqref="B7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -3182,6 +3239,10 @@
       </c>
     </row>
     <row r="6" spans="1:11">
+      <c r="B6" s="15">
+        <f>SUM(D6:MI6)</f>
+        <v>5308.41</v>
+      </c>
       <c r="C6" s="1" t="s">
         <v>2</v>
       </c>
@@ -3300,7 +3361,7 @@
   <dimension ref="A2:K8"/>
   <sheetViews>
     <sheetView zoomScale="125" zoomScaleNormal="125" zoomScalePageLayoutView="125" workbookViewId="0">
-      <selection activeCell="K7" sqref="K7"/>
+      <selection activeCell="B7" sqref="B7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -3362,6 +3423,10 @@
       </c>
     </row>
     <row r="6" spans="1:11">
+      <c r="B6" s="15">
+        <f>SUM(D6:MI6)</f>
+        <v>-2405.5099999999998</v>
+      </c>
       <c r="C6" s="1" t="s">
         <v>2</v>
       </c>
@@ -3483,7 +3548,7 @@
   <dimension ref="A2:K8"/>
   <sheetViews>
     <sheetView zoomScale="125" zoomScaleNormal="125" zoomScalePageLayoutView="125" workbookViewId="0">
-      <selection activeCell="K7" sqref="K7"/>
+      <selection activeCell="B7" sqref="B7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -3545,6 +3610,10 @@
       </c>
     </row>
     <row r="6" spans="1:11">
+      <c r="B6" s="15">
+        <f>SUM(D6:MI6)</f>
+        <v>6827.42</v>
+      </c>
       <c r="C6" s="1" t="s">
         <v>2</v>
       </c>
@@ -3663,7 +3732,7 @@
   <dimension ref="A2:K8"/>
   <sheetViews>
     <sheetView zoomScale="125" zoomScaleNormal="125" zoomScalePageLayoutView="125" workbookViewId="0">
-      <selection activeCell="K7" sqref="K7"/>
+      <selection activeCell="B7" sqref="B7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -3725,6 +3794,10 @@
       </c>
     </row>
     <row r="6" spans="1:11">
+      <c r="B6" s="15">
+        <f>SUM(D6:MI6)</f>
+        <v>-66.799999999999841</v>
+      </c>
       <c r="C6" s="1" t="s">
         <v>2</v>
       </c>

</xml_diff>

<commit_message>
add cost and quantity
</commit_message>
<xml_diff>
--- a/stock.xlsx
+++ b/stock.xlsx
@@ -1,10 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="26405"/>
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="22416"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="1160" yWindow="140" windowWidth="25600" windowHeight="16060" tabRatio="954" activeTab="17"/>
+    <workbookView xWindow="1160" yWindow="140" windowWidth="25600" windowHeight="16060" tabRatio="954" activeTab="15"/>
   </bookViews>
   <sheets>
     <sheet name="达华智能" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="133" uniqueCount="30">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="175" uniqueCount="35">
   <si>
     <t>达华智能</t>
   </si>
@@ -107,6 +107,39 @@
     <t>万方发展</t>
   </si>
   <si>
+    <t>亏646.88</t>
+  </si>
+  <si>
+    <t>走得及时啊</t>
+  </si>
+  <si>
+    <t>亏1179.38</t>
+  </si>
+  <si>
+    <t>亏692.88</t>
+  </si>
+  <si>
+    <t>持仓</t>
+  </si>
+  <si>
+    <t>均价</t>
+  </si>
+  <si>
+    <t>卖</t>
+  </si>
+  <si>
+    <t>买</t>
+  </si>
+  <si>
+    <t>卖价</t>
+  </si>
+  <si>
+    <t>跌得太厉害了，抖动都懒得理</t>
+  </si>
+  <si>
+    <r>
+      <t>md</t>
+    </r>
     <r>
       <rPr>
         <sz val="12"/>
@@ -115,55 +148,11 @@
         <family val="2"/>
         <charset val="134"/>
       </rPr>
-      <t>卖</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>2300</t>
+      <t>戴帽子了，落刀子不能接</t>
     </r>
   </si>
   <si>
-    <t>亏646.88</t>
-  </si>
-  <si>
-    <t>走得及时啊</t>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="宋体"/>
-        <family val="2"/>
-        <charset val="134"/>
-      </rPr>
-      <t>卖</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>500</t>
-    </r>
-  </si>
-  <si>
-    <t>亏1179.38</t>
-  </si>
-  <si>
-    <t>卖500</t>
-  </si>
-  <si>
-    <t>亏692.88</t>
+    <t>普邦股份</t>
   </si>
 </sst>
 </file>
@@ -176,7 +165,7 @@
     <numFmt numFmtId="166" formatCode="[Red]0.0000000;[Green]\-0.0000000"/>
     <numFmt numFmtId="167" formatCode="[Red]0.000%;[Green]\-0.000%"/>
   </numFmts>
-  <fonts count="11" x14ac:knownFonts="1">
+  <fonts count="12" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -253,6 +242,13 @@
       <family val="2"/>
       <charset val="134"/>
     </font>
+    <font>
+      <b/>
+      <sz val="12"/>
+      <color rgb="FF008000"/>
+      <name val="宋体"/>
+      <charset val="134"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -271,7 +267,7 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="39">
+  <cellStyleXfs count="67">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -311,8 +307,36 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="18">
+  <cellXfs count="19">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
@@ -331,8 +355,9 @@
     <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="16" fontId="7" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
-  <cellStyles count="39">
+  <cellStyles count="67">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
@@ -352,6 +377,20 @@
     <cellStyle name="Followed Hyperlink" xfId="34" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="36" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="38" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="40" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="42" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="44" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="46" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="48" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="50" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="52" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="54" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="56" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="58" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="60" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="62" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="64" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="66" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
@@ -371,6 +410,20 @@
     <cellStyle name="Hyperlink" xfId="33" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="35" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="37" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="39" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="41" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="43" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="45" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="47" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="49" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="51" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="53" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="55" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="57" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="59" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="61" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="63" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="65" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -703,10 +756,10 @@
   <sheetPr enableFormatConditionsCalculation="0">
     <tabColor rgb="FFFF0000"/>
   </sheetPr>
-  <dimension ref="A2:N8"/>
+  <dimension ref="A2:N13"/>
   <sheetViews>
-    <sheetView topLeftCell="B1" zoomScale="125" zoomScaleNormal="125" zoomScalePageLayoutView="125" workbookViewId="0">
-      <selection activeCell="N7" sqref="N7"/>
+    <sheetView topLeftCell="A2" zoomScale="125" zoomScaleNormal="125" zoomScalePageLayoutView="125" workbookViewId="0">
+      <selection activeCell="C29" sqref="C29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -912,6 +965,22 @@
       <c r="N8">
         <f t="shared" si="3"/>
         <v>-6.1347393087287641</v>
+      </c>
+    </row>
+    <row r="12" spans="1:14">
+      <c r="C12" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="D12" s="1" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="13" spans="1:14">
+      <c r="C13">
+        <v>1000</v>
+      </c>
+      <c r="D13">
+        <v>17.239999999999998</v>
       </c>
     </row>
   </sheetData>
@@ -933,7 +1002,7 @@
   <dimension ref="A2:N15"/>
   <sheetViews>
     <sheetView zoomScale="125" zoomScaleNormal="125" zoomScalePageLayoutView="125" workbookViewId="0">
-      <selection activeCell="N7" sqref="N7"/>
+      <selection activeCell="F15" sqref="F15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -1141,23 +1210,39 @@
       </c>
     </row>
     <row r="14" spans="1:14">
-      <c r="C14" s="11">
+      <c r="C14" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="D14" s="17" t="s">
+        <v>28</v>
+      </c>
+      <c r="E14" s="1" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="15" spans="1:14">
+      <c r="A15" t="s">
+        <v>29</v>
+      </c>
+      <c r="B15" s="16">
         <v>42972</v>
       </c>
-    </row>
-    <row r="15" spans="1:14">
-      <c r="C15" t="s">
-        <v>26</v>
+      <c r="C15">
+        <v>500</v>
       </c>
       <c r="D15">
+        <v>10.66</v>
+      </c>
+      <c r="E15">
         <v>8.27</v>
       </c>
-      <c r="E15" s="1" t="s">
-        <v>27</v>
+      <c r="F15" s="18" t="s">
+        <v>25</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
       <mx:PLV Mode="0" OnePage="0" WScale="0"/>
@@ -1168,10 +1253,10 @@
 
 <file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A2:N8"/>
+  <dimension ref="A2:N13"/>
   <sheetViews>
-    <sheetView topLeftCell="B1" zoomScale="125" zoomScaleNormal="125" zoomScalePageLayoutView="125" workbookViewId="0">
-      <selection activeCell="N7" sqref="N7"/>
+    <sheetView zoomScale="125" zoomScaleNormal="125" zoomScalePageLayoutView="125" workbookViewId="0">
+      <selection activeCell="D14" sqref="D14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -1376,6 +1461,22 @@
       <c r="N8">
         <f t="shared" si="3"/>
         <v>1699.0019762845852</v>
+      </c>
+    </row>
+    <row r="12" spans="1:14">
+      <c r="C12" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="D12" s="1" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="13" spans="1:14">
+      <c r="C13">
+        <v>800</v>
+      </c>
+      <c r="D13">
+        <v>9.1660000000000004</v>
       </c>
     </row>
   </sheetData>
@@ -1393,10 +1494,10 @@
   <sheetPr enableFormatConditionsCalculation="0">
     <tabColor theme="5" tint="0.39997558519241921"/>
   </sheetPr>
-  <dimension ref="A2:N8"/>
+  <dimension ref="A2:N13"/>
   <sheetViews>
     <sheetView zoomScale="125" zoomScaleNormal="125" zoomScalePageLayoutView="125" workbookViewId="0">
-      <selection activeCell="N7" sqref="N7"/>
+      <selection activeCell="C14" sqref="C14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -1601,6 +1702,22 @@
       <c r="N8">
         <f t="shared" si="3"/>
         <v>-238.4009900990099</v>
+      </c>
+    </row>
+    <row r="12" spans="1:14">
+      <c r="C12" s="17" t="s">
+        <v>27</v>
+      </c>
+      <c r="D12" s="17" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="13" spans="1:14">
+      <c r="C13" s="10">
+        <v>400</v>
+      </c>
+      <c r="D13" s="10">
+        <v>9.0630000000000006</v>
       </c>
     </row>
   </sheetData>
@@ -1615,10 +1732,10 @@
 
 <file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A2:N8"/>
+  <dimension ref="A2:N13"/>
   <sheetViews>
     <sheetView zoomScale="125" zoomScaleNormal="125" zoomScalePageLayoutView="125" workbookViewId="0">
-      <selection activeCell="N7" sqref="N7"/>
+      <selection activeCell="C14" sqref="C14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -1823,6 +1940,22 @@
       <c r="N8">
         <f t="shared" si="3"/>
         <v>1942.0536992840093</v>
+      </c>
+    </row>
+    <row r="12" spans="1:14">
+      <c r="C12" s="17" t="s">
+        <v>27</v>
+      </c>
+      <c r="D12" s="17" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="13" spans="1:14">
+      <c r="C13" s="10">
+        <v>300</v>
+      </c>
+      <c r="D13" s="10">
+        <v>10.034000000000001</v>
       </c>
     </row>
   </sheetData>
@@ -1837,10 +1970,10 @@
 
 <file path=xl/worksheets/sheet14.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A2:N8"/>
+  <dimension ref="A2:N13"/>
   <sheetViews>
     <sheetView zoomScale="125" zoomScaleNormal="125" zoomScalePageLayoutView="125" workbookViewId="0">
-      <selection activeCell="N6" sqref="N6"/>
+      <selection activeCell="C14" sqref="C14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -2045,6 +2178,22 @@
       <c r="N8">
         <f t="shared" si="3"/>
         <v>121.17834394904457</v>
+      </c>
+    </row>
+    <row r="12" spans="1:14">
+      <c r="C12" s="17" t="s">
+        <v>27</v>
+      </c>
+      <c r="D12" s="17" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="13" spans="1:14">
+      <c r="C13" s="10">
+        <v>600</v>
+      </c>
+      <c r="D13" s="10">
+        <v>7.2480000000000002</v>
       </c>
     </row>
   </sheetData>
@@ -2062,10 +2211,10 @@
   <sheetPr enableFormatConditionsCalculation="0">
     <tabColor theme="5" tint="0.39997558519241921"/>
   </sheetPr>
-  <dimension ref="A2:N8"/>
+  <dimension ref="A2:N13"/>
   <sheetViews>
     <sheetView zoomScale="125" zoomScaleNormal="125" zoomScalePageLayoutView="125" workbookViewId="0">
-      <selection activeCell="N7" sqref="N7"/>
+      <selection activeCell="C14" sqref="C14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -2270,6 +2419,22 @@
       <c r="N8">
         <f t="shared" ref="N8" si="3">N6/N7</f>
         <v>46.759299781181618</v>
+      </c>
+    </row>
+    <row r="12" spans="1:14">
+      <c r="C12" s="17" t="s">
+        <v>27</v>
+      </c>
+      <c r="D12" s="17" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="13" spans="1:14">
+      <c r="C13" s="10">
+        <v>400</v>
+      </c>
+      <c r="D13" s="10">
+        <v>8.4030000000000005</v>
       </c>
     </row>
   </sheetData>
@@ -2284,10 +2449,10 @@
 
 <file path=xl/worksheets/sheet16.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A2:N8"/>
+  <dimension ref="A2:N13"/>
   <sheetViews>
-    <sheetView topLeftCell="G1" zoomScale="125" zoomScaleNormal="125" zoomScalePageLayoutView="125" workbookViewId="0">
-      <selection activeCell="N7" sqref="N7"/>
+    <sheetView tabSelected="1" zoomScale="125" zoomScaleNormal="125" zoomScalePageLayoutView="125" workbookViewId="0">
+      <selection activeCell="C14" sqref="C14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -2492,6 +2657,22 @@
       <c r="N8">
         <f t="shared" si="3"/>
         <v>41.627906976744185</v>
+      </c>
+    </row>
+    <row r="12" spans="1:14">
+      <c r="C12" s="17" t="s">
+        <v>27</v>
+      </c>
+      <c r="D12" s="17" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="13" spans="1:14">
+      <c r="C13" s="10">
+        <v>300</v>
+      </c>
+      <c r="D13" s="10">
+        <v>8.4870000000000001</v>
       </c>
     </row>
   </sheetData>
@@ -2506,10 +2687,10 @@
 
 <file path=xl/worksheets/sheet17.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A2:H8"/>
+  <dimension ref="A2:H13"/>
   <sheetViews>
     <sheetView zoomScale="125" zoomScaleNormal="125" zoomScalePageLayoutView="125" workbookViewId="0">
-      <selection activeCell="B9" sqref="B9"/>
+      <selection activeCell="C14" sqref="C14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -2635,6 +2816,22 @@
       <c r="H8">
         <f t="shared" si="0"/>
         <v>0</v>
+      </c>
+    </row>
+    <row r="12" spans="1:8">
+      <c r="C12" s="17" t="s">
+        <v>27</v>
+      </c>
+      <c r="D12" s="17" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="13" spans="1:8">
+      <c r="C13" s="10">
+        <v>300</v>
+      </c>
+      <c r="D13" s="10">
+        <v>16.887</v>
       </c>
     </row>
   </sheetData>
@@ -2649,10 +2846,10 @@
 
 <file path=xl/worksheets/sheet18.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A2:H8"/>
+  <dimension ref="A2:H13"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="125" zoomScaleNormal="125" zoomScalePageLayoutView="125" workbookViewId="0">
-      <selection activeCell="B9" sqref="B9"/>
+    <sheetView zoomScale="125" zoomScaleNormal="125" zoomScalePageLayoutView="125" workbookViewId="0">
+      <selection activeCell="D14" sqref="D14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -2663,7 +2860,7 @@
   <sheetData>
     <row r="2" spans="1:8">
       <c r="C2" s="1" t="s">
-        <v>13</v>
+        <v>34</v>
       </c>
       <c r="D2" s="1" t="s">
         <v>7</v>
@@ -2779,6 +2976,22 @@
       <c r="H8">
         <f t="shared" si="0"/>
         <v>0</v>
+      </c>
+    </row>
+    <row r="12" spans="1:8">
+      <c r="C12" s="17" t="s">
+        <v>27</v>
+      </c>
+      <c r="D12" s="17" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="13" spans="1:8">
+      <c r="C13" s="10">
+        <v>800</v>
+      </c>
+      <c r="D13" s="10">
+        <v>14.318</v>
       </c>
     </row>
   </sheetData>
@@ -2796,10 +3009,10 @@
   <sheetPr enableFormatConditionsCalculation="0">
     <tabColor theme="3" tint="0.39997558519241921"/>
   </sheetPr>
-  <dimension ref="A2:N15"/>
+  <dimension ref="A2:N16"/>
   <sheetViews>
     <sheetView topLeftCell="A2" zoomScale="125" zoomScaleNormal="125" zoomScalePageLayoutView="125" workbookViewId="0">
-      <selection activeCell="N7" sqref="N7"/>
+      <selection activeCell="F15" sqref="F15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -3007,22 +3220,51 @@
       </c>
     </row>
     <row r="14" spans="1:14">
-      <c r="C14" s="11">
+      <c r="C14" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="D14" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="E14" s="1" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="15" spans="1:14">
+      <c r="A15" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="B15" s="11">
         <v>42969</v>
       </c>
-    </row>
-    <row r="15" spans="1:14">
-      <c r="C15" t="s">
+      <c r="C15">
+        <v>2300</v>
+      </c>
+      <c r="D15">
+        <v>4.4000000000000004</v>
+      </c>
+      <c r="E15">
+        <v>4.0999999999999996</v>
+      </c>
+      <c r="F15" s="18" t="s">
         <v>23</v>
       </c>
-      <c r="D15">
-        <v>4.0999999999999996</v>
-      </c>
-      <c r="E15" s="1" t="s">
+      <c r="G15" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="F15" s="1" t="s">
-        <v>25</v>
+    </row>
+    <row r="16" spans="1:14">
+      <c r="A16" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="B16" s="11">
+        <v>42972</v>
+      </c>
+      <c r="C16">
+        <v>300</v>
+      </c>
+      <c r="D16">
+        <v>3.9769999999999999</v>
       </c>
     </row>
   </sheetData>
@@ -3038,10 +3280,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A2:N8"/>
+  <dimension ref="A2:N13"/>
   <sheetViews>
     <sheetView zoomScale="125" zoomScaleNormal="125" zoomScalePageLayoutView="125" workbookViewId="0">
-      <selection activeCell="N7" sqref="N7"/>
+      <selection activeCell="C12" sqref="C12:D13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -3246,6 +3488,22 @@
       <c r="N8">
         <f t="shared" si="3"/>
         <v>2034.7925925925922</v>
+      </c>
+    </row>
+    <row r="12" spans="1:14">
+      <c r="C12" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="D12" s="1" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="13" spans="1:14">
+      <c r="C13">
+        <v>2800</v>
+      </c>
+      <c r="D13">
+        <v>3.8860000000000001</v>
       </c>
     </row>
   </sheetData>
@@ -3264,7 +3522,7 @@
   <dimension ref="A2:N15"/>
   <sheetViews>
     <sheetView zoomScale="125" zoomScaleNormal="125" zoomScalePageLayoutView="125" workbookViewId="0">
-      <selection activeCell="N7" sqref="N7"/>
+      <selection activeCell="C14" sqref="C14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -3469,6 +3727,22 @@
       <c r="N8">
         <f t="shared" si="3"/>
         <v>314.54113924050631</v>
+      </c>
+    </row>
+    <row r="12" spans="1:14">
+      <c r="C12" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="D12" s="1" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="13" spans="1:14">
+      <c r="C13">
+        <v>1000</v>
+      </c>
+      <c r="D13">
+        <v>7.2249999999999996</v>
       </c>
     </row>
     <row r="14" spans="1:14">
@@ -3494,10 +3768,10 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A2:N8"/>
+  <dimension ref="A2:N13"/>
   <sheetViews>
-    <sheetView topLeftCell="B1" zoomScale="125" zoomScaleNormal="125" zoomScalePageLayoutView="125" workbookViewId="0">
-      <selection activeCell="N7" sqref="N7"/>
+    <sheetView zoomScale="125" zoomScaleNormal="125" zoomScalePageLayoutView="125" workbookViewId="0">
+      <selection activeCell="D14" sqref="D14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -3702,6 +3976,22 @@
       <c r="N8">
         <f t="shared" si="3"/>
         <v>1324.8325041459368</v>
+      </c>
+    </row>
+    <row r="12" spans="1:14">
+      <c r="C12" s="17" t="s">
+        <v>27</v>
+      </c>
+      <c r="D12" s="17" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="13" spans="1:14">
+      <c r="C13" s="10">
+        <v>1000</v>
+      </c>
+      <c r="D13" s="10">
+        <v>7.5910000000000002</v>
       </c>
     </row>
   </sheetData>
@@ -3720,10 +4010,10 @@
   <sheetPr enableFormatConditionsCalculation="0">
     <tabColor theme="5" tint="0.39997558519241921"/>
   </sheetPr>
-  <dimension ref="A2:N8"/>
+  <dimension ref="A2:N13"/>
   <sheetViews>
-    <sheetView topLeftCell="B1" zoomScale="125" zoomScaleNormal="125" zoomScalePageLayoutView="125" workbookViewId="0">
-      <selection activeCell="N7" sqref="N7"/>
+    <sheetView zoomScale="125" zoomScaleNormal="125" zoomScalePageLayoutView="125" workbookViewId="0">
+      <selection activeCell="C14" sqref="C14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -3928,6 +4218,22 @@
       <c r="N8">
         <f t="shared" si="3"/>
         <v>23.429752066115704</v>
+      </c>
+    </row>
+    <row r="12" spans="1:14">
+      <c r="C12" s="17" t="s">
+        <v>27</v>
+      </c>
+      <c r="D12" s="17" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="13" spans="1:14">
+      <c r="C13" s="10">
+        <v>300</v>
+      </c>
+      <c r="D13" s="10">
+        <v>27.286999999999999</v>
       </c>
     </row>
   </sheetData>
@@ -3948,8 +4254,8 @@
   </sheetPr>
   <dimension ref="A2:N17"/>
   <sheetViews>
-    <sheetView topLeftCell="B1" zoomScale="125" zoomScaleNormal="125" zoomScalePageLayoutView="125" workbookViewId="0">
-      <selection activeCell="C31" sqref="C31"/>
+    <sheetView zoomScale="125" zoomScaleNormal="125" zoomScalePageLayoutView="125" workbookViewId="0">
+      <selection activeCell="F17" sqref="F17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -4157,21 +4463,34 @@
       </c>
     </row>
     <row r="16" spans="1:14">
-      <c r="C16" s="16">
+      <c r="C16" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="D16" s="17" t="s">
+        <v>28</v>
+      </c>
+      <c r="E16" s="17" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="17" spans="1:6">
+      <c r="A17" t="s">
+        <v>29</v>
+      </c>
+      <c r="B17" s="16">
         <v>42972</v>
       </c>
-      <c r="D16" s="10"/>
-      <c r="E16" s="10"/>
-    </row>
-    <row r="17" spans="3:5">
-      <c r="C17" s="17" t="s">
-        <v>28</v>
-      </c>
-      <c r="D17" s="10">
+      <c r="C17" s="17">
+        <v>500</v>
+      </c>
+      <c r="D17">
+        <v>11.72</v>
+      </c>
+      <c r="E17" s="10">
         <v>10.199999999999999</v>
       </c>
-      <c r="E17" s="17" t="s">
-        <v>29</v>
+      <c r="F17" s="18" t="s">
+        <v>26</v>
       </c>
     </row>
   </sheetData>
@@ -4190,10 +4509,10 @@
   <sheetPr enableFormatConditionsCalculation="0">
     <tabColor theme="5" tint="0.39997558519241921"/>
   </sheetPr>
-  <dimension ref="A2:N8"/>
+  <dimension ref="A2:N13"/>
   <sheetViews>
-    <sheetView topLeftCell="D1" zoomScale="125" zoomScaleNormal="125" zoomScalePageLayoutView="125" workbookViewId="0">
-      <selection activeCell="N7" sqref="N7"/>
+    <sheetView topLeftCell="B1" zoomScale="125" zoomScaleNormal="125" zoomScalePageLayoutView="125" workbookViewId="0">
+      <selection activeCell="G13" sqref="G13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -4398,6 +4717,25 @@
       <c r="N8">
         <f t="shared" si="3"/>
         <v>-404.26353503184714</v>
+      </c>
+    </row>
+    <row r="12" spans="1:14">
+      <c r="C12" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="D12" s="1" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="13" spans="1:14">
+      <c r="C13">
+        <v>400</v>
+      </c>
+      <c r="D13">
+        <v>27.524999999999999</v>
+      </c>
+      <c r="G13" s="1" t="s">
+        <v>32</v>
       </c>
     </row>
   </sheetData>
@@ -4413,10 +4751,10 @@
 
 <file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A2:N8"/>
+  <dimension ref="A2:N13"/>
   <sheetViews>
     <sheetView zoomScale="125" zoomScaleNormal="125" zoomScalePageLayoutView="125" workbookViewId="0">
-      <selection activeCell="N7" sqref="N7"/>
+      <selection activeCell="G14" sqref="G14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -4623,6 +4961,25 @@
         <v>0.19506726457399104</v>
       </c>
     </row>
+    <row r="12" spans="1:14">
+      <c r="C12" s="17" t="s">
+        <v>27</v>
+      </c>
+      <c r="D12" s="17" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="13" spans="1:14">
+      <c r="C13" s="10">
+        <v>1000</v>
+      </c>
+      <c r="D13" s="10">
+        <v>4.46</v>
+      </c>
+      <c r="G13" t="s">
+        <v>33</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <extLst>

</xml_diff>

<commit_message>
change chart data range
</commit_message>
<xml_diff>
--- a/stock.xlsx
+++ b/stock.xlsx
@@ -1,10 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="22416"/>
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="26405"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="3860" yWindow="100" windowWidth="25600" windowHeight="16060" tabRatio="996" activeTab="6"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="16060" tabRatio="996" activeTab="19"/>
   </bookViews>
   <sheets>
     <sheet name="远大控股" sheetId="6" r:id="rId1"/>
@@ -694,10 +694,10 @@
           </c:marker>
           <c:val>
             <c:numRef>
-              <c:f>远大控股!$D$9:$AD$9</c:f>
+              <c:f>远大控股!$D$9:$BD$9</c:f>
               <c:numCache>
                 <c:formatCode>[Red]0.00;[Green]\-0.00</c:formatCode>
-                <c:ptCount val="27"/>
+                <c:ptCount val="53"/>
                 <c:pt idx="0">
                   <c:v>47.13</c:v>
                 </c:pt>
@@ -794,11 +794,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="2142940456"/>
-        <c:axId val="2142714104"/>
+        <c:axId val="-2031941224"/>
+        <c:axId val="-2031938216"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="2142940456"/>
+        <c:axId val="-2031941224"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -807,7 +807,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="2142714104"/>
+        <c:crossAx val="-2031938216"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -815,7 +815,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="2142714104"/>
+        <c:axId val="-2031938216"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -826,7 +826,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="2142940456"/>
+        <c:crossAx val="-2031941224"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -876,10 +876,10 @@
           </c:marker>
           <c:val>
             <c:numRef>
-              <c:f>天宝食品!$D$9:$AD$9</c:f>
+              <c:f>天宝食品!$D$9:$BD$9</c:f>
               <c:numCache>
                 <c:formatCode>[Red]0.00;[Green]\-0.00</c:formatCode>
-                <c:ptCount val="27"/>
+                <c:ptCount val="53"/>
                 <c:pt idx="0">
                   <c:v>203.1</c:v>
                 </c:pt>
@@ -976,11 +976,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="-2115539192"/>
-        <c:axId val="-2115536104"/>
+        <c:axId val="-2031556776"/>
+        <c:axId val="-2031553768"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="-2115539192"/>
+        <c:axId val="-2031556776"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -989,7 +989,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-2115536104"/>
+        <c:crossAx val="-2031553768"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -997,7 +997,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="-2115536104"/>
+        <c:axId val="-2031553768"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1008,7 +1008,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-2115539192"/>
+        <c:crossAx val="-2031556776"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -1058,10 +1058,10 @@
           </c:marker>
           <c:val>
             <c:numRef>
-              <c:f>宝钢股份!$D$9:$AD$9</c:f>
+              <c:f>宝钢股份!$D$9:$BD$9</c:f>
               <c:numCache>
                 <c:formatCode>[Red]0.00;[Green]\-0.00</c:formatCode>
-                <c:ptCount val="27"/>
+                <c:ptCount val="53"/>
                 <c:pt idx="0">
                   <c:v>-6879.03</c:v>
                 </c:pt>
@@ -1158,11 +1158,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="-2113368296"/>
-        <c:axId val="-2115604040"/>
+        <c:axId val="-2031515112"/>
+        <c:axId val="-2031512088"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="-2113368296"/>
+        <c:axId val="-2031515112"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1171,7 +1171,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-2115604040"/>
+        <c:crossAx val="-2031512088"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -1179,7 +1179,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="-2115604040"/>
+        <c:axId val="-2031512088"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1190,7 +1190,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-2113368296"/>
+        <c:crossAx val="-2031515112"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -1240,10 +1240,10 @@
           </c:marker>
           <c:val>
             <c:numRef>
-              <c:f>中国石化!$D$9:$AD$9</c:f>
+              <c:f>中国石化!$D$9:$BD$9</c:f>
               <c:numCache>
                 <c:formatCode>[Red]0.00;[Green]\-0.00</c:formatCode>
-                <c:ptCount val="27"/>
+                <c:ptCount val="53"/>
                 <c:pt idx="0">
                   <c:v>12051.06</c:v>
                 </c:pt>
@@ -1340,11 +1340,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="-2115875496"/>
-        <c:axId val="-2115869480"/>
+        <c:axId val="-2031473192"/>
+        <c:axId val="-2031470168"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="-2115875496"/>
+        <c:axId val="-2031473192"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1353,7 +1353,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-2115869480"/>
+        <c:crossAx val="-2031470168"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -1361,7 +1361,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="-2115869480"/>
+        <c:axId val="-2031470168"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1372,7 +1372,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-2115875496"/>
+        <c:crossAx val="-2031473192"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -1422,10 +1422,10 @@
           </c:marker>
           <c:val>
             <c:numRef>
-              <c:f>中国中冶!$D$9:$AD$9</c:f>
+              <c:f>中国中冶!$D$9:$BD$9</c:f>
               <c:numCache>
                 <c:formatCode>[Red]0.00;[Green]\-0.00</c:formatCode>
-                <c:ptCount val="27"/>
+                <c:ptCount val="53"/>
                 <c:pt idx="0">
                   <c:v>6669.91</c:v>
                 </c:pt>
@@ -1522,11 +1522,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="-2114935208"/>
-        <c:axId val="-2114828152"/>
+        <c:axId val="-2031431352"/>
+        <c:axId val="-2031428328"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="-2114935208"/>
+        <c:axId val="-2031431352"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1535,7 +1535,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-2114828152"/>
+        <c:crossAx val="-2031428328"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -1543,7 +1543,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="-2114828152"/>
+        <c:axId val="-2031428328"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1554,7 +1554,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-2114935208"/>
+        <c:crossAx val="-2031431352"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -1604,10 +1604,10 @@
           </c:marker>
           <c:val>
             <c:numRef>
-              <c:f>远望谷!$D$9:$AD$9</c:f>
+              <c:f>远望谷!$D$9:$BD$9</c:f>
               <c:numCache>
                 <c:formatCode>[Red]0.00;[Green]\-0.00</c:formatCode>
-                <c:ptCount val="27"/>
+                <c:ptCount val="53"/>
                 <c:pt idx="0">
                   <c:v>-5587.2</c:v>
                 </c:pt>
@@ -1704,11 +1704,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="-2113957416"/>
-        <c:axId val="-2113953768"/>
+        <c:axId val="-2031389512"/>
+        <c:axId val="-2031386488"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="-2113957416"/>
+        <c:axId val="-2031389512"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1717,7 +1717,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-2113953768"/>
+        <c:crossAx val="-2031386488"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -1725,7 +1725,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="-2113953768"/>
+        <c:axId val="-2031386488"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1736,7 +1736,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-2113957416"/>
+        <c:crossAx val="-2031389512"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -1786,10 +1786,10 @@
           </c:marker>
           <c:val>
             <c:numRef>
-              <c:f>巨轮智能!$D$9:$AD$9</c:f>
+              <c:f>巨轮智能!$D$9:$BD$9</c:f>
               <c:numCache>
                 <c:formatCode>[Red]0.00;[Green]\-0.00</c:formatCode>
-                <c:ptCount val="27"/>
+                <c:ptCount val="53"/>
                 <c:pt idx="0">
                   <c:v>-1260.64</c:v>
                 </c:pt>
@@ -1886,11 +1886,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="-2111979080"/>
-        <c:axId val="-2111996232"/>
+        <c:axId val="-2031347816"/>
+        <c:axId val="-2031344792"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="-2111979080"/>
+        <c:axId val="-2031347816"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1899,7 +1899,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-2111996232"/>
+        <c:crossAx val="-2031344792"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -1907,7 +1907,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="-2111996232"/>
+        <c:axId val="-2031344792"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1918,7 +1918,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-2111979080"/>
+        <c:crossAx val="-2031347816"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -1968,10 +1968,10 @@
           </c:marker>
           <c:val>
             <c:numRef>
-              <c:f>大金重工!$D$9:$AD$9</c:f>
+              <c:f>大金重工!$D$9:$BD$9</c:f>
               <c:numCache>
                 <c:formatCode>[Red]0.00;[Green]\-0.00</c:formatCode>
-                <c:ptCount val="27"/>
+                <c:ptCount val="53"/>
                 <c:pt idx="0">
                   <c:v>77.57</c:v>
                 </c:pt>
@@ -2068,11 +2068,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="-2111905640"/>
-        <c:axId val="-2111903288"/>
+        <c:axId val="-2031307208"/>
+        <c:axId val="-2031304200"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="-2111905640"/>
+        <c:axId val="-2031307208"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2081,7 +2081,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-2111903288"/>
+        <c:crossAx val="-2031304200"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -2089,7 +2089,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="-2111903288"/>
+        <c:axId val="-2031304200"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2100,7 +2100,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-2111905640"/>
+        <c:crossAx val="-2031307208"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -2150,10 +2150,10 @@
           </c:marker>
           <c:val>
             <c:numRef>
-              <c:f>普邦股份!$D$9:$Q$9</c:f>
+              <c:f>普邦股份!$D$9:$BD$9</c:f>
               <c:numCache>
                 <c:formatCode>[Red]0.00;[Green]\-0.00</c:formatCode>
-                <c:ptCount val="14"/>
+                <c:ptCount val="53"/>
                 <c:pt idx="0">
                   <c:v>-1286.24</c:v>
                 </c:pt>
@@ -2211,11 +2211,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="-2109374520"/>
-        <c:axId val="-2109365256"/>
+        <c:axId val="-2031268392"/>
+        <c:axId val="-2031265384"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="-2109374520"/>
+        <c:axId val="-2031268392"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2224,7 +2224,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-2109365256"/>
+        <c:crossAx val="-2031265384"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -2232,7 +2232,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="-2109365256"/>
+        <c:axId val="-2031265384"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2243,7 +2243,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-2109374520"/>
+        <c:crossAx val="-2031268392"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -2293,10 +2293,10 @@
           </c:marker>
           <c:val>
             <c:numRef>
-              <c:f>贵州茅台!$D$9:$P$9</c:f>
+              <c:f>贵州茅台!$D$9:$BM$9</c:f>
               <c:numCache>
                 <c:formatCode>[Red]0.00;[Green]\-0.00</c:formatCode>
-                <c:ptCount val="13"/>
+                <c:ptCount val="62"/>
                 <c:pt idx="0">
                   <c:v>2678.35</c:v>
                 </c:pt>
@@ -2351,11 +2351,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="2142307256"/>
-        <c:axId val="2142295800"/>
+        <c:axId val="-2031225256"/>
+        <c:axId val="-2031222248"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="2142307256"/>
+        <c:axId val="-2031225256"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2364,7 +2364,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="2142295800"/>
+        <c:crossAx val="-2031222248"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -2372,7 +2372,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="2142295800"/>
+        <c:axId val="-2031222248"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2383,7 +2383,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="2142307256"/>
+        <c:crossAx val="-2031225256"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -2433,10 +2433,10 @@
           </c:marker>
           <c:val>
             <c:numRef>
-              <c:f>圆通!$D$9:$K$9</c:f>
+              <c:f>圆通!$D$9:$BM$9</c:f>
               <c:numCache>
                 <c:formatCode>[Red]0.00;[Green]\-0.00</c:formatCode>
-                <c:ptCount val="8"/>
+                <c:ptCount val="62"/>
                 <c:pt idx="0">
                   <c:v>30.43</c:v>
                 </c:pt>
@@ -2476,11 +2476,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="2145315704"/>
-        <c:axId val="-2119364488"/>
+        <c:axId val="-2031187720"/>
+        <c:axId val="-2031184696"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="2145315704"/>
+        <c:axId val="-2031187720"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2489,7 +2489,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-2119364488"/>
+        <c:crossAx val="-2031184696"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -2497,7 +2497,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="-2119364488"/>
+        <c:axId val="-2031184696"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2508,7 +2508,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="2145315704"/>
+        <c:crossAx val="-2031187720"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -2558,10 +2558,10 @@
           </c:marker>
           <c:val>
             <c:numRef>
-              <c:f>沪电股份!$D$9:$AD$9</c:f>
+              <c:f>沪电股份!$D$9:$BD$9</c:f>
               <c:numCache>
                 <c:formatCode>[Red]0.00;[Green]\-0.00</c:formatCode>
-                <c:ptCount val="27"/>
+                <c:ptCount val="53"/>
                 <c:pt idx="0">
                   <c:v>-296.07</c:v>
                 </c:pt>
@@ -2658,11 +2658,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="2140818696"/>
-        <c:axId val="2140821784"/>
+        <c:axId val="-2031899304"/>
+        <c:axId val="-2031896360"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="2140818696"/>
+        <c:axId val="-2031899304"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2671,7 +2671,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="2140821784"/>
+        <c:crossAx val="-2031896360"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -2679,7 +2679,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="2140821784"/>
+        <c:axId val="-2031896360"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2690,7 +2690,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="2140818696"/>
+        <c:crossAx val="-2031899304"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -2740,10 +2740,10 @@
           </c:marker>
           <c:val>
             <c:numRef>
-              <c:f>达华智能!$D$9:$AD$9</c:f>
+              <c:f>达华智能!$D$9:$BD$9</c:f>
               <c:numCache>
                 <c:formatCode>[Red]0.00;[Green]\-0.00</c:formatCode>
-                <c:ptCount val="27"/>
+                <c:ptCount val="53"/>
                 <c:pt idx="0">
                   <c:v>716.65</c:v>
                 </c:pt>
@@ -2840,11 +2840,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="2143196456"/>
-        <c:axId val="2143200920"/>
+        <c:axId val="-2031857176"/>
+        <c:axId val="-2031854232"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="2143196456"/>
+        <c:axId val="-2031857176"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2853,7 +2853,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="2143200920"/>
+        <c:crossAx val="-2031854232"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -2861,7 +2861,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="2143200920"/>
+        <c:axId val="-2031854232"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2872,7 +2872,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="2143196456"/>
+        <c:crossAx val="-2031857176"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -2922,10 +2922,10 @@
           </c:marker>
           <c:val>
             <c:numRef>
-              <c:f>民生银行!$D$9:$AD$9</c:f>
+              <c:f>民生银行!$D$9:$BD$9</c:f>
               <c:numCache>
                 <c:formatCode>[Red]0.00;[Green]\-0.00</c:formatCode>
-                <c:ptCount val="27"/>
+                <c:ptCount val="53"/>
                 <c:pt idx="0">
                   <c:v>-3240.47</c:v>
                 </c:pt>
@@ -3022,11 +3022,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="-2121597784"/>
-        <c:axId val="-2117818664"/>
+        <c:axId val="-2031815544"/>
+        <c:axId val="-2031812600"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="-2121597784"/>
+        <c:axId val="-2031815544"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3035,7 +3035,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-2117818664"/>
+        <c:crossAx val="-2031812600"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -3043,7 +3043,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="-2117818664"/>
+        <c:axId val="-2031812600"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3054,7 +3054,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-2121597784"/>
+        <c:crossAx val="-2031815544"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -3104,10 +3104,10 @@
           </c:marker>
           <c:val>
             <c:numRef>
-              <c:f>中远海发!$D$9:$AD$9</c:f>
+              <c:f>中远海发!$D$9:$BD$9</c:f>
               <c:numCache>
                 <c:formatCode>[Red]0.00;[Green]\-0.00</c:formatCode>
-                <c:ptCount val="27"/>
+                <c:ptCount val="53"/>
                 <c:pt idx="0">
                   <c:v>-14643.97</c:v>
                 </c:pt>
@@ -3204,11 +3204,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="-2121130568"/>
-        <c:axId val="-2120363352"/>
+        <c:axId val="-2031756552"/>
+        <c:axId val="-2031753608"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="-2121130568"/>
+        <c:axId val="-2031756552"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3217,7 +3217,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-2120363352"/>
+        <c:crossAx val="-2031753608"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -3225,7 +3225,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="-2120363352"/>
+        <c:axId val="-2031753608"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3236,7 +3236,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-2121130568"/>
+        <c:crossAx val="-2031756552"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -3286,10 +3286,10 @@
           </c:marker>
           <c:val>
             <c:numRef>
-              <c:f>包钢股份!$D$9:$AD$9</c:f>
+              <c:f>包钢股份!$D$9:$BD$9</c:f>
               <c:numCache>
                 <c:formatCode>[Red]0.00;[Green]\-0.00</c:formatCode>
-                <c:ptCount val="27"/>
+                <c:ptCount val="53"/>
                 <c:pt idx="0">
                   <c:v>-21881.24</c:v>
                 </c:pt>
@@ -3386,11 +3386,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="-2118740376"/>
-        <c:axId val="-2119514856"/>
+        <c:axId val="-2031714488"/>
+        <c:axId val="-2031711480"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="-2118740376"/>
+        <c:axId val="-2031714488"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3399,7 +3399,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-2119514856"/>
+        <c:crossAx val="-2031711480"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -3407,7 +3407,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="-2119514856"/>
+        <c:axId val="-2031711480"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3418,7 +3418,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-2118740376"/>
+        <c:crossAx val="-2031714488"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -3468,10 +3468,10 @@
           </c:marker>
           <c:val>
             <c:numRef>
-              <c:f>景兴纸业!$D$9:$AD$9</c:f>
+              <c:f>景兴纸业!$D$9:$BD$9</c:f>
               <c:numCache>
                 <c:formatCode>[Red]0.00;[Green]\-0.00</c:formatCode>
-                <c:ptCount val="27"/>
+                <c:ptCount val="53"/>
                 <c:pt idx="0">
                   <c:v>-2926.17</c:v>
                 </c:pt>
@@ -3568,11 +3568,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="-2117096360"/>
-        <c:axId val="-2117323832"/>
+        <c:axId val="-2031672648"/>
+        <c:axId val="-2031669640"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="-2117096360"/>
+        <c:axId val="-2031672648"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3581,7 +3581,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-2117323832"/>
+        <c:crossAx val="-2031669640"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -3589,7 +3589,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="-2117323832"/>
+        <c:axId val="-2031669640"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3600,7 +3600,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-2117096360"/>
+        <c:crossAx val="-2031672648"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -3650,10 +3650,10 @@
           </c:marker>
           <c:val>
             <c:numRef>
-              <c:f>浙江医药!$D$9:$AD$9</c:f>
+              <c:f>浙江医药!$D$9:$BD$9</c:f>
               <c:numCache>
                 <c:formatCode>[Red]0.00;[Green]\-0.00</c:formatCode>
-                <c:ptCount val="27"/>
+                <c:ptCount val="53"/>
                 <c:pt idx="0">
                   <c:v>1074.42</c:v>
                 </c:pt>
@@ -3750,11 +3750,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="2058554712"/>
-        <c:axId val="2140411592"/>
+        <c:axId val="-2031638920"/>
+        <c:axId val="-2031800648"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="2058554712"/>
+        <c:axId val="-2031638920"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3763,7 +3763,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="2140411592"/>
+        <c:crossAx val="-2031800648"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -3771,7 +3771,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="2140411592"/>
+        <c:axId val="-2031800648"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3782,7 +3782,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="2058554712"/>
+        <c:crossAx val="-2031638920"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -3832,10 +3832,10 @@
           </c:marker>
           <c:val>
             <c:numRef>
-              <c:f>st智慧!$D$9:$AD$9</c:f>
+              <c:f>st智慧!$D$9:$BD$9</c:f>
               <c:numCache>
                 <c:formatCode>[Red]0.00;[Green]\-0.00</c:formatCode>
-                <c:ptCount val="27"/>
+                <c:ptCount val="53"/>
                 <c:pt idx="0">
                   <c:v>1560.66</c:v>
                 </c:pt>
@@ -3932,11 +3932,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="-2116290440"/>
-        <c:axId val="-2116322152"/>
+        <c:axId val="-2031588056"/>
+        <c:axId val="-2031585048"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="-2116290440"/>
+        <c:axId val="-2031588056"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3945,7 +3945,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-2116322152"/>
+        <c:crossAx val="-2031585048"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -3953,7 +3953,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="-2116322152"/>
+        <c:axId val="-2031585048"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3964,7 +3964,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-2116290440"/>
+        <c:crossAx val="-2031588056"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -3996,10 +3996,10 @@
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>13</xdr:col>
-      <xdr:colOff>114300</xdr:colOff>
-      <xdr:row>28</xdr:row>
-      <xdr:rowOff>88900</xdr:rowOff>
+      <xdr:col>14</xdr:col>
+      <xdr:colOff>241300</xdr:colOff>
+      <xdr:row>29</xdr:row>
+      <xdr:rowOff>76200</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -4031,10 +4031,10 @@
       <xdr:rowOff>76200</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>9</xdr:col>
-      <xdr:colOff>469900</xdr:colOff>
-      <xdr:row>30</xdr:row>
-      <xdr:rowOff>152400</xdr:rowOff>
+      <xdr:col>12</xdr:col>
+      <xdr:colOff>457200</xdr:colOff>
+      <xdr:row>33</xdr:row>
+      <xdr:rowOff>50800</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -4066,10 +4066,10 @@
       <xdr:rowOff>127000</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>8</xdr:col>
-      <xdr:colOff>431800</xdr:colOff>
-      <xdr:row>31</xdr:row>
-      <xdr:rowOff>12700</xdr:rowOff>
+      <xdr:col>11</xdr:col>
+      <xdr:colOff>660400</xdr:colOff>
+      <xdr:row>32</xdr:row>
+      <xdr:rowOff>127000</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -4101,10 +4101,10 @@
       <xdr:rowOff>76200</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>10</xdr:col>
-      <xdr:colOff>38100</xdr:colOff>
-      <xdr:row>28</xdr:row>
-      <xdr:rowOff>152400</xdr:rowOff>
+      <xdr:col>13</xdr:col>
+      <xdr:colOff>279400</xdr:colOff>
+      <xdr:row>30</xdr:row>
+      <xdr:rowOff>88900</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -4136,10 +4136,10 @@
       <xdr:rowOff>127000</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>10</xdr:col>
-      <xdr:colOff>393700</xdr:colOff>
-      <xdr:row>29</xdr:row>
-      <xdr:rowOff>12700</xdr:rowOff>
+      <xdr:col>14</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>30</xdr:row>
+      <xdr:rowOff>165100</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -4171,10 +4171,10 @@
       <xdr:rowOff>177800</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>10</xdr:col>
-      <xdr:colOff>0</xdr:colOff>
-      <xdr:row>29</xdr:row>
-      <xdr:rowOff>177800</xdr:rowOff>
+      <xdr:col>12</xdr:col>
+      <xdr:colOff>622300</xdr:colOff>
+      <xdr:row>30</xdr:row>
+      <xdr:rowOff>165100</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -4206,10 +4206,10 @@
       <xdr:rowOff>114300</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>10</xdr:col>
-      <xdr:colOff>596900</xdr:colOff>
-      <xdr:row>27</xdr:row>
-      <xdr:rowOff>0</xdr:rowOff>
+      <xdr:col>14</xdr:col>
+      <xdr:colOff>241300</xdr:colOff>
+      <xdr:row>32</xdr:row>
+      <xdr:rowOff>165100</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -4241,10 +4241,10 @@
       <xdr:rowOff>76200</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>9</xdr:col>
-      <xdr:colOff>127000</xdr:colOff>
-      <xdr:row>28</xdr:row>
-      <xdr:rowOff>152400</xdr:rowOff>
+      <xdr:col>12</xdr:col>
+      <xdr:colOff>609600</xdr:colOff>
+      <xdr:row>31</xdr:row>
+      <xdr:rowOff>177800</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -4276,10 +4276,10 @@
       <xdr:rowOff>101600</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>9</xdr:col>
-      <xdr:colOff>482600</xdr:colOff>
-      <xdr:row>27</xdr:row>
-      <xdr:rowOff>177800</xdr:rowOff>
+      <xdr:col>12</xdr:col>
+      <xdr:colOff>203200</xdr:colOff>
+      <xdr:row>28</xdr:row>
+      <xdr:rowOff>38100</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -4311,10 +4311,10 @@
       <xdr:rowOff>25400</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>8</xdr:col>
-      <xdr:colOff>495300</xdr:colOff>
-      <xdr:row>28</xdr:row>
-      <xdr:rowOff>101600</xdr:rowOff>
+      <xdr:col>12</xdr:col>
+      <xdr:colOff>419100</xdr:colOff>
+      <xdr:row>29</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -4346,10 +4346,10 @@
       <xdr:rowOff>127000</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>9</xdr:col>
-      <xdr:colOff>203200</xdr:colOff>
-      <xdr:row>29</xdr:row>
-      <xdr:rowOff>12700</xdr:rowOff>
+      <xdr:col>14</xdr:col>
+      <xdr:colOff>165100</xdr:colOff>
+      <xdr:row>30</xdr:row>
+      <xdr:rowOff>114300</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -4381,10 +4381,10 @@
       <xdr:rowOff>101600</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>12</xdr:col>
-      <xdr:colOff>50800</xdr:colOff>
-      <xdr:row>26</xdr:row>
-      <xdr:rowOff>177800</xdr:rowOff>
+      <xdr:col>14</xdr:col>
+      <xdr:colOff>635000</xdr:colOff>
+      <xdr:row>27</xdr:row>
+      <xdr:rowOff>114300</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -4410,16 +4410,16 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>8</xdr:col>
-      <xdr:colOff>25400</xdr:colOff>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>12700</xdr:colOff>
       <xdr:row>12</xdr:row>
-      <xdr:rowOff>63500</xdr:rowOff>
+      <xdr:rowOff>127000</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>13</xdr:col>
-      <xdr:colOff>469900</xdr:colOff>
-      <xdr:row>26</xdr:row>
-      <xdr:rowOff>139700</xdr:rowOff>
+      <xdr:col>14</xdr:col>
+      <xdr:colOff>228600</xdr:colOff>
+      <xdr:row>28</xdr:row>
+      <xdr:rowOff>12700</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -4451,10 +4451,10 @@
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>11</xdr:col>
-      <xdr:colOff>457200</xdr:colOff>
-      <xdr:row>29</xdr:row>
-      <xdr:rowOff>76200</xdr:rowOff>
+      <xdr:col>13</xdr:col>
+      <xdr:colOff>723900</xdr:colOff>
+      <xdr:row>31</xdr:row>
+      <xdr:rowOff>88900</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -4486,10 +4486,10 @@
       <xdr:rowOff>101600</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>11</xdr:col>
-      <xdr:colOff>63500</xdr:colOff>
-      <xdr:row>31</xdr:row>
-      <xdr:rowOff>177800</xdr:rowOff>
+      <xdr:col>13</xdr:col>
+      <xdr:colOff>177800</xdr:colOff>
+      <xdr:row>32</xdr:row>
+      <xdr:rowOff>165100</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -4521,10 +4521,10 @@
       <xdr:rowOff>152400</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>10</xdr:col>
-      <xdr:colOff>190500</xdr:colOff>
+      <xdr:col>13</xdr:col>
+      <xdr:colOff>50800</xdr:colOff>
       <xdr:row>31</xdr:row>
-      <xdr:rowOff>38100</xdr:rowOff>
+      <xdr:rowOff>177800</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -4556,10 +4556,10 @@
       <xdr:rowOff>165100</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>8</xdr:col>
-      <xdr:colOff>736600</xdr:colOff>
-      <xdr:row>30</xdr:row>
-      <xdr:rowOff>50800</xdr:rowOff>
+      <xdr:col>11</xdr:col>
+      <xdr:colOff>25400</xdr:colOff>
+      <xdr:row>31</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -4591,10 +4591,10 @@
       <xdr:rowOff>38100</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>10</xdr:col>
-      <xdr:colOff>165100</xdr:colOff>
+      <xdr:col>14</xdr:col>
+      <xdr:colOff>228600</xdr:colOff>
       <xdr:row>34</xdr:row>
-      <xdr:rowOff>114300</xdr:rowOff>
+      <xdr:rowOff>25400</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -4626,10 +4626,10 @@
       <xdr:rowOff>12700</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>9</xdr:col>
-      <xdr:colOff>63500</xdr:colOff>
-      <xdr:row>32</xdr:row>
-      <xdr:rowOff>88900</xdr:rowOff>
+      <xdr:col>12</xdr:col>
+      <xdr:colOff>25400</xdr:colOff>
+      <xdr:row>33</xdr:row>
+      <xdr:rowOff>12700</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -4978,8 +4978,8 @@
   </sheetPr>
   <dimension ref="A2:AD13"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C9" sqref="C9:D9"/>
+    <sheetView topLeftCell="E1" workbookViewId="0">
+      <selection activeCell="P28" sqref="P28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -6121,7 +6121,7 @@
   </sheetPr>
   <dimension ref="A2:AD15"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView topLeftCell="D1" workbookViewId="0">
       <selection activeCell="D9" sqref="D9:AD9"/>
     </sheetView>
   </sheetViews>
@@ -6744,7 +6744,7 @@
   <dimension ref="A2:AD13"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D9" sqref="D9:AD9"/>
+      <selection activeCell="C21" sqref="C21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -7304,7 +7304,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A2:AD13"/>
   <sheetViews>
-    <sheetView topLeftCell="B2" workbookViewId="0">
+    <sheetView topLeftCell="D2" workbookViewId="0">
       <selection activeCell="D9" sqref="D9:AD9"/>
     </sheetView>
   </sheetViews>
@@ -7873,7 +7873,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A2:AD13"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView topLeftCell="D1" workbookViewId="0">
       <selection activeCell="D9" sqref="D9:AD9"/>
     </sheetView>
   </sheetViews>
@@ -8437,7 +8437,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A2:AD13"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView topLeftCell="D1" workbookViewId="0">
       <selection activeCell="L29" sqref="L29"/>
     </sheetView>
   </sheetViews>
@@ -8997,7 +8997,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A2:AD13"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView topLeftCell="D1" workbookViewId="0">
       <selection activeCell="D9" sqref="D9:AD9"/>
     </sheetView>
   </sheetViews>
@@ -10410,7 +10410,7 @@
   <dimension ref="A2:AD15"/>
   <sheetViews>
     <sheetView topLeftCell="D1" workbookViewId="0">
-      <selection activeCell="G29" sqref="G29"/>
+      <selection activeCell="K31" sqref="K31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -10984,6 +10984,7 @@
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
   <drawing r:id="rId1"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
@@ -10997,7 +10998,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A2:K13"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="D9" sqref="D9:K9"/>
     </sheetView>
   </sheetViews>
@@ -11233,8 +11234,8 @@
   </sheetPr>
   <dimension ref="A2:AD13"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D9" sqref="D9:AD9"/>
+    <sheetView topLeftCell="D1" workbookViewId="0">
+      <selection activeCell="N12" sqref="N12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -11810,7 +11811,7 @@
   </sheetPr>
   <dimension ref="A2:AD13"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView topLeftCell="B2" workbookViewId="0">
       <selection activeCell="D9" sqref="D9:AD9"/>
     </sheetView>
   </sheetViews>
@@ -12388,7 +12389,7 @@
   </sheetPr>
   <dimension ref="A2:AD16"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView topLeftCell="D1" workbookViewId="0">
       <selection activeCell="D9" sqref="D9:AD9"/>
     </sheetView>
   </sheetViews>
@@ -12990,8 +12991,8 @@
   </sheetPr>
   <dimension ref="A2:AD14"/>
   <sheetViews>
-    <sheetView topLeftCell="A2" workbookViewId="0">
-      <selection activeCell="D9" sqref="D9:AD9"/>
+    <sheetView topLeftCell="D1" workbookViewId="0">
+      <selection activeCell="L18" sqref="L18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -13576,7 +13577,7 @@
   </sheetPr>
   <dimension ref="A2:AD15"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView topLeftCell="D1" workbookViewId="0">
       <selection activeCell="D9" sqref="D9:AD9"/>
     </sheetView>
   </sheetViews>
@@ -14168,7 +14169,7 @@
   </sheetPr>
   <dimension ref="A2:AD17"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView topLeftCell="D1" workbookViewId="0">
       <selection activeCell="D9" sqref="D9:AD9"/>
     </sheetView>
   </sheetViews>
@@ -14747,7 +14748,7 @@
   </sheetPr>
   <dimension ref="A2:AD15"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView topLeftCell="D1" workbookViewId="0">
       <selection activeCell="D9" sqref="D9:AD9"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
sell 2 trash stocks
</commit_message>
<xml_diff>
--- a/stock.xlsx
+++ b/stock.xlsx
@@ -1,10 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="22416"/>
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="26405"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="2180" yWindow="0" windowWidth="25600" windowHeight="16060" tabRatio="996" activeTab="19"/>
+    <workbookView xWindow="2180" yWindow="0" windowWidth="25600" windowHeight="16060" tabRatio="996" activeTab="14"/>
   </bookViews>
   <sheets>
     <sheet name="美的集团" sheetId="21" r:id="rId1"/>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="277" uniqueCount="71">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="279" uniqueCount="72">
   <si>
     <t>达华智能</t>
   </si>
@@ -312,6 +312,9 @@
   </si>
   <si>
     <t>又高买低卖了。。。</t>
+  </si>
+  <si>
+    <t>sell</t>
   </si>
 </sst>
 </file>
@@ -855,11 +858,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="-2029431432"/>
-        <c:axId val="-2029428488"/>
+        <c:axId val="1772161272"/>
+        <c:axId val="1772140584"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="-2029431432"/>
+        <c:axId val="1772161272"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -868,7 +871,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-2029428488"/>
+        <c:crossAx val="1772140584"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -876,7 +879,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="-2029428488"/>
+        <c:axId val="1772140584"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -887,14 +890,13 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-2029431432"/>
+        <c:crossAx val="1772161272"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
     </c:plotArea>
     <c:legend>
       <c:legendPos val="r"/>
-      <c:layout/>
       <c:overlay val="0"/>
     </c:legend>
     <c:plotVisOnly val="1"/>
@@ -1106,11 +1108,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="-2028855000"/>
-        <c:axId val="-2028851992"/>
+        <c:axId val="-2100680024"/>
+        <c:axId val="-2101079512"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="-2028855000"/>
+        <c:axId val="-2100680024"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1119,7 +1121,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-2028851992"/>
+        <c:crossAx val="-2101079512"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -1127,7 +1129,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="-2028851992"/>
+        <c:axId val="-2101079512"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1138,14 +1140,13 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-2028855000"/>
+        <c:crossAx val="-2100680024"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
     </c:plotArea>
     <c:legend>
       <c:legendPos val="r"/>
-      <c:layout/>
       <c:overlay val="0"/>
     </c:legend>
     <c:plotVisOnly val="1"/>
@@ -1367,11 +1368,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="-2028820424"/>
-        <c:axId val="-2028817416"/>
+        <c:axId val="1773785192"/>
+        <c:axId val="1773788200"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="-2028820424"/>
+        <c:axId val="1773785192"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1380,7 +1381,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-2028817416"/>
+        <c:crossAx val="1773788200"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -1388,7 +1389,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="-2028817416"/>
+        <c:axId val="1773788200"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:min val="16.5"/>
@@ -1400,14 +1401,13 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-2028820424"/>
+        <c:crossAx val="1773785192"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
     </c:plotArea>
     <c:legend>
       <c:legendPos val="r"/>
-      <c:layout/>
       <c:overlay val="0"/>
     </c:legend>
     <c:plotVisOnly val="1"/>
@@ -1616,11 +1616,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:gapWidth val="150"/>
-        <c:axId val="-2028794120"/>
-        <c:axId val="-2028791112"/>
+        <c:axId val="1773457848"/>
+        <c:axId val="1773460856"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="-2028794120"/>
+        <c:axId val="1773457848"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1629,7 +1629,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-2028791112"/>
+        <c:crossAx val="1773460856"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -1637,7 +1637,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="-2028791112"/>
+        <c:axId val="1773460856"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1648,14 +1648,13 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-2028794120"/>
+        <c:crossAx val="1773457848"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
     </c:plotArea>
     <c:legend>
       <c:legendPos val="r"/>
-      <c:layout/>
       <c:overlay val="0"/>
     </c:legend>
     <c:plotVisOnly val="1"/>
@@ -1867,11 +1866,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="-2028751208"/>
-        <c:axId val="-2028748200"/>
+        <c:axId val="1772778120"/>
+        <c:axId val="1772781176"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="-2028751208"/>
+        <c:axId val="1772778120"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1880,7 +1879,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-2028748200"/>
+        <c:crossAx val="1772781176"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -1888,7 +1887,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="-2028748200"/>
+        <c:axId val="1772781176"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1899,14 +1898,13 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-2028751208"/>
+        <c:crossAx val="1772778120"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
     </c:plotArea>
     <c:legend>
       <c:legendPos val="r"/>
-      <c:layout/>
       <c:overlay val="0"/>
     </c:legend>
     <c:plotVisOnly val="1"/>
@@ -2128,11 +2126,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="-2032658552"/>
-        <c:axId val="-2032655544"/>
+        <c:axId val="1772325480"/>
+        <c:axId val="1772328488"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="-2032658552"/>
+        <c:axId val="1772325480"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2141,7 +2139,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-2032655544"/>
+        <c:crossAx val="1772328488"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -2149,7 +2147,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="-2032655544"/>
+        <c:axId val="1772328488"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2160,14 +2158,13 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-2032658552"/>
+        <c:crossAx val="1772325480"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
     </c:plotArea>
     <c:legend>
       <c:legendPos val="r"/>
-      <c:layout/>
       <c:overlay val="0"/>
     </c:legend>
     <c:plotVisOnly val="1"/>
@@ -2376,11 +2373,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:gapWidth val="150"/>
-        <c:axId val="-2032631864"/>
-        <c:axId val="-2032628856"/>
+        <c:axId val="1772650264"/>
+        <c:axId val="1772639800"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="-2032631864"/>
+        <c:axId val="1772650264"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2389,7 +2386,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-2032628856"/>
+        <c:crossAx val="1772639800"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -2397,7 +2394,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="-2032628856"/>
+        <c:axId val="1772639800"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2408,14 +2405,13 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-2032631864"/>
+        <c:crossAx val="1772650264"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
     </c:plotArea>
     <c:legend>
       <c:legendPos val="r"/>
-      <c:layout/>
       <c:overlay val="0"/>
     </c:legend>
     <c:plotVisOnly val="1"/>
@@ -2627,11 +2623,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="-2029781560"/>
-        <c:axId val="-2029778552"/>
+        <c:axId val="1772553496"/>
+        <c:axId val="1772556504"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="-2029781560"/>
+        <c:axId val="1772553496"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2640,7 +2636,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-2029778552"/>
+        <c:crossAx val="1772556504"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -2648,7 +2644,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="-2029778552"/>
+        <c:axId val="1772556504"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2659,14 +2655,13 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-2029781560"/>
+        <c:crossAx val="1772553496"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
     </c:plotArea>
     <c:legend>
       <c:legendPos val="r"/>
-      <c:layout/>
       <c:overlay val="0"/>
     </c:legend>
     <c:plotVisOnly val="1"/>
@@ -2888,11 +2883,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="-2029746568"/>
-        <c:axId val="-2029743560"/>
+        <c:axId val="1772303128"/>
+        <c:axId val="1772306136"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="-2029746568"/>
+        <c:axId val="1772303128"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2901,7 +2896,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-2029743560"/>
+        <c:crossAx val="1772306136"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -2909,7 +2904,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="-2029743560"/>
+        <c:axId val="1772306136"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2920,14 +2915,13 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-2029746568"/>
+        <c:crossAx val="1772303128"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
     </c:plotArea>
     <c:legend>
       <c:legendPos val="r"/>
-      <c:layout/>
       <c:overlay val="0"/>
     </c:legend>
     <c:plotVisOnly val="1"/>
@@ -3136,11 +3130,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:gapWidth val="150"/>
-        <c:axId val="-2029719800"/>
-        <c:axId val="-2029716792"/>
+        <c:axId val="1773021272"/>
+        <c:axId val="1772883912"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="-2029719800"/>
+        <c:axId val="1773021272"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3149,7 +3143,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-2029716792"/>
+        <c:crossAx val="1772883912"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -3157,7 +3151,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="-2029716792"/>
+        <c:axId val="1772883912"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3168,14 +3162,13 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-2029719800"/>
+        <c:crossAx val="1773021272"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
     </c:plotArea>
     <c:legend>
       <c:legendPos val="r"/>
-      <c:layout/>
       <c:overlay val="0"/>
     </c:legend>
     <c:plotVisOnly val="1"/>
@@ -3387,11 +3380,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="-2029676760"/>
-        <c:axId val="-2029673752"/>
+        <c:axId val="1772544312"/>
+        <c:axId val="1772547320"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="-2029676760"/>
+        <c:axId val="1772544312"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3400,7 +3393,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-2029673752"/>
+        <c:crossAx val="1772547320"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -3408,7 +3401,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="-2029673752"/>
+        <c:axId val="1772547320"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3419,14 +3412,13 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-2029676760"/>
+        <c:crossAx val="1772544312"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
     </c:plotArea>
     <c:legend>
       <c:legendPos val="r"/>
-      <c:layout/>
       <c:overlay val="0"/>
     </c:legend>
     <c:plotVisOnly val="1"/>
@@ -3530,11 +3522,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="-2029400040"/>
-        <c:axId val="-2029397096"/>
+        <c:axId val="1772155640"/>
+        <c:axId val="1772158648"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="-2029400040"/>
+        <c:axId val="1772155640"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3543,7 +3535,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-2029397096"/>
+        <c:crossAx val="1772158648"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -3551,7 +3543,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="-2029397096"/>
+        <c:axId val="1772158648"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3562,14 +3554,13 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-2029400040"/>
+        <c:crossAx val="1772155640"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
     </c:plotArea>
     <c:legend>
       <c:legendPos val="r"/>
-      <c:layout/>
       <c:overlay val="0"/>
     </c:legend>
     <c:plotVisOnly val="1"/>
@@ -3791,11 +3782,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="-2030034728"/>
-        <c:axId val="-2030031752"/>
+        <c:axId val="1772595384"/>
+        <c:axId val="1772732600"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="-2030034728"/>
+        <c:axId val="1772595384"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3804,7 +3795,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-2030031752"/>
+        <c:crossAx val="1772732600"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -3812,7 +3803,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="-2030031752"/>
+        <c:axId val="1772732600"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3823,14 +3814,13 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-2030034728"/>
+        <c:crossAx val="1772595384"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
     </c:plotArea>
     <c:legend>
       <c:legendPos val="r"/>
-      <c:layout/>
       <c:overlay val="0"/>
     </c:legend>
     <c:plotVisOnly val="1"/>
@@ -4039,11 +4029,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:gapWidth val="150"/>
-        <c:axId val="-2032939544"/>
-        <c:axId val="-2032936536"/>
+        <c:axId val="1772858824"/>
+        <c:axId val="1772863672"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="-2032939544"/>
+        <c:axId val="1772858824"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -4052,7 +4042,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-2032936536"/>
+        <c:crossAx val="1772863672"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -4060,7 +4050,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="-2032936536"/>
+        <c:axId val="1772863672"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -4071,14 +4061,13 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-2032939544"/>
+        <c:crossAx val="1772858824"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
     </c:plotArea>
     <c:legend>
       <c:legendPos val="r"/>
-      <c:layout/>
       <c:overlay val="0"/>
     </c:legend>
     <c:plotVisOnly val="1"/>
@@ -4290,11 +4279,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="-2032896312"/>
-        <c:axId val="-2032893304"/>
+        <c:axId val="1772984168"/>
+        <c:axId val="1772663752"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="-2032896312"/>
+        <c:axId val="1772984168"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -4303,7 +4292,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-2032893304"/>
+        <c:crossAx val="1772663752"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -4311,7 +4300,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="-2032893304"/>
+        <c:axId val="1772663752"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -4322,14 +4311,13 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-2032896312"/>
+        <c:crossAx val="1772984168"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
     </c:plotArea>
     <c:legend>
       <c:legendPos val="r"/>
-      <c:layout/>
       <c:overlay val="0"/>
     </c:legend>
     <c:plotVisOnly val="1"/>
@@ -4551,11 +4539,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="-2032213912"/>
-        <c:axId val="-2032210904"/>
+        <c:axId val="1772688968"/>
+        <c:axId val="1772691976"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="-2032213912"/>
+        <c:axId val="1772688968"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -4564,7 +4552,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-2032210904"/>
+        <c:crossAx val="1772691976"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -4572,7 +4560,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="-2032210904"/>
+        <c:axId val="1772691976"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -4583,14 +4571,13 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-2032213912"/>
+        <c:crossAx val="1772688968"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
     </c:plotArea>
     <c:legend>
       <c:legendPos val="r"/>
-      <c:layout/>
       <c:overlay val="0"/>
     </c:legend>
     <c:plotVisOnly val="1"/>
@@ -4799,11 +4786,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:gapWidth val="150"/>
-        <c:axId val="-2030007784"/>
-        <c:axId val="-2030004776"/>
+        <c:axId val="1772464456"/>
+        <c:axId val="1772467464"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="-2030007784"/>
+        <c:axId val="1772464456"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -4812,7 +4799,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-2030004776"/>
+        <c:crossAx val="1772467464"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -4820,7 +4807,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="-2030004776"/>
+        <c:axId val="1772467464"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -4831,14 +4818,13 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-2030007784"/>
+        <c:crossAx val="1772464456"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
     </c:plotArea>
     <c:legend>
       <c:legendPos val="r"/>
-      <c:layout/>
       <c:overlay val="0"/>
     </c:legend>
     <c:plotVisOnly val="1"/>
@@ -5050,11 +5036,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="-2032378392"/>
-        <c:axId val="-2032375384"/>
+        <c:axId val="1772315928"/>
+        <c:axId val="1772318936"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="-2032378392"/>
+        <c:axId val="1772315928"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -5063,7 +5049,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-2032375384"/>
+        <c:crossAx val="1772318936"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -5071,7 +5057,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="-2032375384"/>
+        <c:axId val="1772318936"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -5082,14 +5068,13 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-2032378392"/>
+        <c:crossAx val="1772315928"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
     </c:plotArea>
     <c:legend>
       <c:legendPos val="r"/>
-      <c:layout/>
       <c:overlay val="0"/>
     </c:legend>
     <c:plotVisOnly val="1"/>
@@ -5311,11 +5296,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="-2032343656"/>
-        <c:axId val="-2032340648"/>
+        <c:axId val="1773100360"/>
+        <c:axId val="1773103368"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="-2032343656"/>
+        <c:axId val="1773100360"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -5324,7 +5309,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-2032340648"/>
+        <c:crossAx val="1773103368"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -5332,7 +5317,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="-2032340648"/>
+        <c:axId val="1773103368"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -5343,14 +5328,13 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-2032343656"/>
+        <c:crossAx val="1773100360"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
     </c:plotArea>
     <c:legend>
       <c:legendPos val="r"/>
-      <c:layout/>
       <c:overlay val="0"/>
     </c:legend>
     <c:plotVisOnly val="1"/>
@@ -5559,11 +5543,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:gapWidth val="150"/>
-        <c:axId val="-2032317416"/>
-        <c:axId val="-2032314408"/>
+        <c:axId val="1773124744"/>
+        <c:axId val="1773061112"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="-2032317416"/>
+        <c:axId val="1773124744"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -5572,7 +5556,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-2032314408"/>
+        <c:crossAx val="1773061112"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -5580,7 +5564,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="-2032314408"/>
+        <c:axId val="1773061112"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -5591,14 +5575,13 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-2032317416"/>
+        <c:crossAx val="1773124744"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
     </c:plotArea>
     <c:legend>
       <c:legendPos val="r"/>
-      <c:layout/>
       <c:overlay val="0"/>
     </c:legend>
     <c:plotVisOnly val="1"/>
@@ -5810,11 +5793,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="-2032275432"/>
-        <c:axId val="-2032272424"/>
+        <c:axId val="1772766296"/>
+        <c:axId val="1772769304"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="-2032275432"/>
+        <c:axId val="1772766296"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -5823,7 +5806,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-2032272424"/>
+        <c:crossAx val="1772769304"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -5831,7 +5814,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="-2032272424"/>
+        <c:axId val="1772769304"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -5842,14 +5825,13 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-2032275432"/>
+        <c:crossAx val="1772766296"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
     </c:plotArea>
     <c:legend>
       <c:legendPos val="r"/>
-      <c:layout/>
       <c:overlay val="0"/>
     </c:legend>
     <c:plotVisOnly val="1"/>
@@ -6071,11 +6053,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="-2032242136"/>
-        <c:axId val="-2032239128"/>
+        <c:axId val="1772399704"/>
+        <c:axId val="1772916760"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="-2032242136"/>
+        <c:axId val="1772399704"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -6084,7 +6066,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-2032239128"/>
+        <c:crossAx val="1772916760"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -6092,7 +6074,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="-2032239128"/>
+        <c:axId val="1772916760"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -6103,14 +6085,13 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-2032242136"/>
+        <c:crossAx val="1772399704"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
     </c:plotArea>
     <c:legend>
       <c:legendPos val="r"/>
-      <c:layout/>
       <c:overlay val="0"/>
     </c:legend>
     <c:plotVisOnly val="1"/>
@@ -6211,11 +6192,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:gapWidth val="150"/>
-        <c:axId val="-2121184072"/>
-        <c:axId val="-2121264520"/>
+        <c:axId val="1772810888"/>
+        <c:axId val="1772114312"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="-2121184072"/>
+        <c:axId val="1772810888"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -6224,7 +6205,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-2121264520"/>
+        <c:crossAx val="1772114312"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -6232,7 +6213,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="-2121264520"/>
+        <c:axId val="1772114312"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -6243,14 +6224,13 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-2121184072"/>
+        <c:crossAx val="1772810888"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
     </c:plotArea>
     <c:legend>
       <c:legendPos val="r"/>
-      <c:layout/>
       <c:overlay val="0"/>
     </c:legend>
     <c:plotVisOnly val="1"/>
@@ -6459,11 +6439,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:gapWidth val="150"/>
-        <c:axId val="-2028447384"/>
-        <c:axId val="-2028444376"/>
+        <c:axId val="1788011656"/>
+        <c:axId val="1787871304"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="-2028447384"/>
+        <c:axId val="1788011656"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -6472,7 +6452,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-2028444376"/>
+        <c:crossAx val="1787871304"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -6480,7 +6460,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="-2028444376"/>
+        <c:axId val="1787871304"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -6491,14 +6471,13 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-2028447384"/>
+        <c:crossAx val="1788011656"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
     </c:plotArea>
     <c:legend>
       <c:legendPos val="r"/>
-      <c:layout/>
       <c:overlay val="0"/>
     </c:legend>
     <c:plotVisOnly val="1"/>
@@ -6710,11 +6689,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="-2032602664"/>
-        <c:axId val="-2032599656"/>
+        <c:axId val="1788039512"/>
+        <c:axId val="1788043144"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="-2032602664"/>
+        <c:axId val="1788039512"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -6723,7 +6702,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-2032599656"/>
+        <c:crossAx val="1788043144"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -6731,7 +6710,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="-2032599656"/>
+        <c:axId val="1788043144"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -6742,14 +6721,13 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-2032602664"/>
+        <c:crossAx val="1788039512"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
     </c:plotArea>
     <c:legend>
       <c:legendPos val="r"/>
-      <c:layout/>
       <c:overlay val="0"/>
     </c:legend>
     <c:plotVisOnly val="1"/>
@@ -6971,11 +6949,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="-2032567992"/>
-        <c:axId val="-2032564984"/>
+        <c:axId val="1788811576"/>
+        <c:axId val="1788814584"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="-2032567992"/>
+        <c:axId val="1788811576"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -6984,7 +6962,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-2032564984"/>
+        <c:crossAx val="1788814584"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -6992,7 +6970,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="-2032564984"/>
+        <c:axId val="1788814584"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:min val="3.0"/>
@@ -7004,14 +6982,13 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-2032567992"/>
+        <c:crossAx val="1788811576"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
     </c:plotArea>
     <c:legend>
       <c:legendPos val="r"/>
-      <c:layout/>
       <c:overlay val="0"/>
     </c:legend>
     <c:plotVisOnly val="1"/>
@@ -7220,11 +7197,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:gapWidth val="150"/>
-        <c:axId val="-2032541752"/>
-        <c:axId val="-2032538744"/>
+        <c:axId val="1788628776"/>
+        <c:axId val="1788631752"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="-2032541752"/>
+        <c:axId val="1788628776"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -7233,7 +7210,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-2032538744"/>
+        <c:crossAx val="1788631752"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -7241,7 +7218,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="-2032538744"/>
+        <c:axId val="1788631752"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -7252,14 +7229,13 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-2032541752"/>
+        <c:crossAx val="1788628776"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
     </c:plotArea>
     <c:legend>
       <c:legendPos val="r"/>
-      <c:layout/>
       <c:overlay val="0"/>
     </c:legend>
     <c:plotVisOnly val="1"/>
@@ -7471,11 +7447,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="-2028293000"/>
-        <c:axId val="-2028289992"/>
+        <c:axId val="1788093016"/>
+        <c:axId val="1787928696"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="-2028293000"/>
+        <c:axId val="1788093016"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -7484,7 +7460,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-2028289992"/>
+        <c:crossAx val="1787928696"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -7492,7 +7468,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="-2028289992"/>
+        <c:axId val="1787928696"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -7503,14 +7479,13 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-2028293000"/>
+        <c:crossAx val="1788093016"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
     </c:plotArea>
     <c:legend>
       <c:legendPos val="r"/>
-      <c:layout/>
       <c:overlay val="0"/>
     </c:legend>
     <c:plotVisOnly val="1"/>
@@ -7732,11 +7707,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="-2028258008"/>
-        <c:axId val="-2028255000"/>
+        <c:axId val="1788505208"/>
+        <c:axId val="1788508216"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="-2028258008"/>
+        <c:axId val="1788505208"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -7745,7 +7720,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-2028255000"/>
+        <c:crossAx val="1788508216"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -7753,7 +7728,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="-2028255000"/>
+        <c:axId val="1788508216"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:min val="6.5"/>
@@ -7765,14 +7740,13 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-2028258008"/>
+        <c:crossAx val="1788505208"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
     </c:plotArea>
     <c:legend>
       <c:legendPos val="r"/>
-      <c:layout/>
       <c:overlay val="0"/>
     </c:legend>
     <c:plotVisOnly val="1"/>
@@ -7981,11 +7955,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:gapWidth val="150"/>
-        <c:axId val="-2028231656"/>
-        <c:axId val="-2028228648"/>
+        <c:axId val="1788454280"/>
+        <c:axId val="1788457192"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="-2028231656"/>
+        <c:axId val="1788454280"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -7994,7 +7968,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-2028228648"/>
+        <c:crossAx val="1788457192"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -8002,7 +7976,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="-2028228648"/>
+        <c:axId val="1788457192"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -8013,14 +7987,13 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-2028231656"/>
+        <c:crossAx val="1788454280"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
     </c:plotArea>
     <c:legend>
       <c:legendPos val="r"/>
-      <c:layout/>
       <c:overlay val="0"/>
     </c:legend>
     <c:plotVisOnly val="1"/>
@@ -8232,11 +8205,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="-2028188568"/>
-        <c:axId val="-2028185560"/>
+        <c:axId val="1788182056"/>
+        <c:axId val="1788185064"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="-2028188568"/>
+        <c:axId val="1788182056"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -8245,7 +8218,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-2028185560"/>
+        <c:crossAx val="1788185064"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -8253,7 +8226,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="-2028185560"/>
+        <c:axId val="1788185064"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -8264,14 +8237,13 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-2028188568"/>
+        <c:crossAx val="1788182056"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
     </c:plotArea>
     <c:legend>
       <c:legendPos val="r"/>
-      <c:layout/>
       <c:overlay val="0"/>
     </c:legend>
     <c:plotVisOnly val="1"/>
@@ -8493,11 +8465,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="-2028153464"/>
-        <c:axId val="-2028150456"/>
+        <c:axId val="-2100212008"/>
+        <c:axId val="-2100206072"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="-2028153464"/>
+        <c:axId val="-2100212008"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -8506,7 +8478,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-2028150456"/>
+        <c:crossAx val="-2100206072"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -8514,7 +8486,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="-2028150456"/>
+        <c:axId val="-2100206072"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -8525,14 +8497,13 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-2028153464"/>
+        <c:crossAx val="-2100212008"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
     </c:plotArea>
     <c:legend>
       <c:legendPos val="r"/>
-      <c:layout/>
       <c:overlay val="0"/>
     </c:legend>
     <c:plotVisOnly val="1"/>
@@ -8741,11 +8712,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:gapWidth val="150"/>
-        <c:axId val="-2032386792"/>
-        <c:axId val="-2032383784"/>
+        <c:axId val="1772981752"/>
+        <c:axId val="1772932808"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="-2032386792"/>
+        <c:axId val="1772981752"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -8754,7 +8725,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-2032383784"/>
+        <c:crossAx val="1772932808"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -8762,7 +8733,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="-2032383784"/>
+        <c:axId val="1772932808"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -8773,14 +8744,13 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-2032386792"/>
+        <c:crossAx val="1772981752"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
     </c:plotArea>
     <c:legend>
       <c:legendPos val="r"/>
-      <c:layout/>
       <c:overlay val="0"/>
     </c:legend>
     <c:plotVisOnly val="1"/>
@@ -8992,11 +8962,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="-2028716856"/>
-        <c:axId val="-2028713912"/>
+        <c:axId val="1783836280"/>
+        <c:axId val="-2098070488"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="-2028716856"/>
+        <c:axId val="1783836280"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -9005,7 +8975,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-2028713912"/>
+        <c:crossAx val="-2098070488"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -9013,7 +8983,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="-2028713912"/>
+        <c:axId val="-2098070488"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -9024,14 +8994,13 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-2028716856"/>
+        <c:crossAx val="1783836280"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
     </c:plotArea>
     <c:legend>
       <c:legendPos val="r"/>
-      <c:layout/>
       <c:overlay val="0"/>
     </c:legend>
     <c:plotVisOnly val="1"/>
@@ -9243,11 +9212,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="-2029591000"/>
-        <c:axId val="-2029587992"/>
+        <c:axId val="1772358904"/>
+        <c:axId val="1772361912"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="-2029591000"/>
+        <c:axId val="1772358904"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -9256,7 +9225,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-2029587992"/>
+        <c:crossAx val="1772361912"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -9264,7 +9233,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="-2029587992"/>
+        <c:axId val="1772361912"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -9275,7 +9244,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-2029591000"/>
+        <c:crossAx val="1772358904"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -9504,11 +9473,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="-2029556248"/>
-        <c:axId val="-2029553240"/>
+        <c:axId val="1772942888"/>
+        <c:axId val="1772945896"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="-2029556248"/>
+        <c:axId val="1772942888"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -9517,7 +9486,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-2029553240"/>
+        <c:crossAx val="1772945896"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -9525,7 +9494,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="-2029553240"/>
+        <c:axId val="1772945896"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -9536,7 +9505,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-2029556248"/>
+        <c:crossAx val="1772942888"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -9752,11 +9721,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:gapWidth val="150"/>
-        <c:axId val="-2029530008"/>
-        <c:axId val="-2029527000"/>
+        <c:axId val="1772193928"/>
+        <c:axId val="1772196936"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="-2029530008"/>
+        <c:axId val="1772193928"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -9765,7 +9734,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-2029527000"/>
+        <c:crossAx val="1772196936"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -9773,7 +9742,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="-2029527000"/>
+        <c:axId val="1772196936"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -9784,7 +9753,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-2029530008"/>
+        <c:crossAx val="1772193928"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -10003,11 +9972,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="-2028664680"/>
-        <c:axId val="-2028661672"/>
+        <c:axId val="1772237160"/>
+        <c:axId val="1772240168"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="-2028664680"/>
+        <c:axId val="1772237160"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -10016,7 +9985,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-2028661672"/>
+        <c:crossAx val="1772240168"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -10024,7 +9993,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="-2028661672"/>
+        <c:axId val="1772240168"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -10035,7 +10004,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-2028664680"/>
+        <c:crossAx val="1772237160"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -10264,11 +10233,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="-2028630072"/>
-        <c:axId val="-2028627064"/>
+        <c:axId val="1772502088"/>
+        <c:axId val="1772505096"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="-2028630072"/>
+        <c:axId val="1772502088"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -10277,7 +10246,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-2028627064"/>
+        <c:crossAx val="1772505096"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -10285,7 +10254,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="-2028627064"/>
+        <c:axId val="1772505096"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:min val="8.0"/>
@@ -10297,7 +10266,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-2028630072"/>
+        <c:crossAx val="1772502088"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -10513,11 +10482,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:gapWidth val="150"/>
-        <c:axId val="-2029458200"/>
-        <c:axId val="-2029455192"/>
+        <c:axId val="2028485448"/>
+        <c:axId val="1772100856"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="-2029458200"/>
+        <c:axId val="2028485448"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -10526,7 +10495,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-2029455192"/>
+        <c:crossAx val="1772100856"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -10534,7 +10503,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="-2029455192"/>
+        <c:axId val="1772100856"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -10545,7 +10514,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-2029458200"/>
+        <c:crossAx val="2028485448"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -10764,11 +10733,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="-2029232296"/>
-        <c:axId val="-2029229288"/>
+        <c:axId val="-2068005096"/>
+        <c:axId val="-2068598840"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="-2029232296"/>
+        <c:axId val="-2068005096"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -10777,7 +10746,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-2029229288"/>
+        <c:crossAx val="-2068598840"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -10785,7 +10754,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="-2029229288"/>
+        <c:axId val="-2068598840"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -10796,14 +10765,13 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-2029232296"/>
+        <c:crossAx val="-2068005096"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
     </c:plotArea>
     <c:legend>
       <c:legendPos val="r"/>
-      <c:layout/>
       <c:overlay val="0"/>
     </c:legend>
     <c:plotVisOnly val="1"/>
@@ -11015,11 +10983,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="-2029197672"/>
-        <c:axId val="-2029194664"/>
+        <c:axId val="-2068792792"/>
+        <c:axId val="-2068098952"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="-2029197672"/>
+        <c:axId val="-2068792792"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -11028,7 +10996,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-2029194664"/>
+        <c:crossAx val="-2068098952"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -11036,7 +11004,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="-2029194664"/>
+        <c:axId val="-2068098952"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -11047,14 +11015,13 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-2029197672"/>
+        <c:crossAx val="-2068792792"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
     </c:plotArea>
     <c:legend>
       <c:legendPos val="r"/>
-      <c:layout/>
       <c:overlay val="0"/>
     </c:legend>
     <c:plotVisOnly val="1"/>
@@ -11263,11 +11230,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:gapWidth val="150"/>
-        <c:axId val="-2029171336"/>
-        <c:axId val="-2029168328"/>
+        <c:axId val="-2067819976"/>
+        <c:axId val="-2067816968"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="-2029171336"/>
+        <c:axId val="-2067819976"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -11276,7 +11243,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-2029168328"/>
+        <c:crossAx val="-2067816968"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -11284,7 +11251,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="-2029168328"/>
+        <c:axId val="-2067816968"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -11295,14 +11262,13 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-2029171336"/>
+        <c:crossAx val="-2067819976"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
     </c:plotArea>
     <c:legend>
       <c:legendPos val="r"/>
-      <c:layout/>
       <c:overlay val="0"/>
     </c:legend>
     <c:plotVisOnly val="1"/>
@@ -11514,11 +11480,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="-2029871240"/>
-        <c:axId val="-2029868232"/>
+        <c:axId val="-2067854600"/>
+        <c:axId val="-2067860440"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="-2029871240"/>
+        <c:axId val="-2067854600"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -11527,7 +11493,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-2029868232"/>
+        <c:crossAx val="-2067860440"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -11535,7 +11501,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="-2029868232"/>
+        <c:axId val="-2067860440"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -11546,14 +11512,13 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-2029871240"/>
+        <c:crossAx val="-2067854600"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
     </c:plotArea>
     <c:legend>
       <c:legendPos val="r"/>
-      <c:layout/>
       <c:overlay val="0"/>
     </c:legend>
     <c:plotVisOnly val="1"/>
@@ -11775,11 +11740,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="-2029383592"/>
-        <c:axId val="-2029380648"/>
+        <c:axId val="1783907912"/>
+        <c:axId val="-2083903400"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="-2029383592"/>
+        <c:axId val="1783907912"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -11788,7 +11753,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-2029380648"/>
+        <c:crossAx val="-2083903400"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -11796,7 +11761,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="-2029380648"/>
+        <c:axId val="-2083903400"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:min val="15.0"/>
@@ -11808,14 +11773,13 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-2029383592"/>
+        <c:crossAx val="1783907912"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
     </c:plotArea>
     <c:legend>
       <c:legendPos val="r"/>
-      <c:layout/>
       <c:overlay val="0"/>
     </c:legend>
     <c:plotVisOnly val="1"/>
@@ -12037,11 +12001,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="2147395384"/>
-        <c:axId val="2147462728"/>
+        <c:axId val="-2067898744"/>
+        <c:axId val="-2067895736"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="2147395384"/>
+        <c:axId val="-2067898744"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -12050,7 +12014,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="2147462728"/>
+        <c:crossAx val="-2067895736"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -12058,7 +12022,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="2147462728"/>
+        <c:axId val="-2067895736"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -12069,14 +12033,13 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="2147395384"/>
+        <c:crossAx val="-2067898744"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
     </c:plotArea>
     <c:legend>
       <c:legendPos val="r"/>
-      <c:layout/>
       <c:overlay val="0"/>
     </c:legend>
     <c:plotVisOnly val="1"/>
@@ -12285,11 +12248,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:gapWidth val="150"/>
-        <c:axId val="2147362984"/>
-        <c:axId val="-2029853928"/>
+        <c:axId val="-2067924952"/>
+        <c:axId val="-2067921976"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="2147362984"/>
+        <c:axId val="-2067924952"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -12298,7 +12261,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-2029853928"/>
+        <c:crossAx val="-2067921976"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -12306,7 +12269,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="-2029853928"/>
+        <c:axId val="-2067921976"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -12317,14 +12280,13 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="2147362984"/>
+        <c:crossAx val="-2067924952"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
     </c:plotArea>
     <c:legend>
       <c:legendPos val="r"/>
-      <c:layout/>
       <c:overlay val="0"/>
     </c:legend>
     <c:plotVisOnly val="1"/>
@@ -12497,11 +12459,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="-2029956072"/>
-        <c:axId val="-2029953064"/>
+        <c:axId val="-2067957080"/>
+        <c:axId val="-2067954072"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="-2029956072"/>
+        <c:axId val="-2067957080"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -12510,7 +12472,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-2029953064"/>
+        <c:crossAx val="-2067954072"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -12518,7 +12480,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="-2029953064"/>
+        <c:axId val="-2067954072"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -12529,7 +12491,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-2029956072"/>
+        <c:crossAx val="-2067957080"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -12719,11 +12681,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="-2029921432"/>
-        <c:axId val="-2029918424"/>
+        <c:axId val="-2068016920"/>
+        <c:axId val="-2068013912"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="-2029921432"/>
+        <c:axId val="-2068016920"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -12732,7 +12694,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-2029918424"/>
+        <c:crossAx val="-2068013912"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -12740,7 +12702,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="-2029918424"/>
+        <c:axId val="-2068013912"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -12751,7 +12713,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-2029921432"/>
+        <c:crossAx val="-2068016920"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -12928,11 +12890,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:gapWidth val="150"/>
-        <c:axId val="-2029795736"/>
-        <c:axId val="-2120256744"/>
+        <c:axId val="-2068046968"/>
+        <c:axId val="-2068043960"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="-2029795736"/>
+        <c:axId val="-2068046968"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -12941,7 +12903,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-2120256744"/>
+        <c:crossAx val="-2068043960"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -12949,7 +12911,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="-2120256744"/>
+        <c:axId val="-2068043960"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -12960,7 +12922,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-2029795736"/>
+        <c:crossAx val="-2068046968"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -13137,11 +13099,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="-2028129944"/>
-        <c:axId val="-2028126936"/>
+        <c:axId val="-2068088072"/>
+        <c:axId val="-2068097848"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="-2028129944"/>
+        <c:axId val="-2068088072"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -13150,7 +13112,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-2028126936"/>
+        <c:crossAx val="-2068097848"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -13158,7 +13120,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="-2028126936"/>
+        <c:axId val="-2068097848"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -13169,14 +13131,13 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-2028129944"/>
+        <c:crossAx val="-2068088072"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
     </c:plotArea>
     <c:legend>
       <c:legendPos val="r"/>
-      <c:layout/>
       <c:overlay val="0"/>
     </c:legend>
     <c:plotVisOnly val="1"/>
@@ -13356,11 +13317,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="-2028480584"/>
-        <c:axId val="-2028477576"/>
+        <c:axId val="-2068129288"/>
+        <c:axId val="-2068144120"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="-2028480584"/>
+        <c:axId val="-2068129288"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -13369,7 +13330,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-2028477576"/>
+        <c:crossAx val="-2068144120"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -13377,7 +13338,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="-2028477576"/>
+        <c:axId val="-2068144120"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:min val="350.0"/>
@@ -13389,14 +13350,13 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-2028480584"/>
+        <c:crossAx val="-2068129288"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
     </c:plotArea>
     <c:legend>
       <c:legendPos val="r"/>
-      <c:layout/>
       <c:overlay val="0"/>
     </c:legend>
     <c:plotVisOnly val="1"/>
@@ -13563,11 +13523,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:gapWidth val="150"/>
-        <c:axId val="-2028502440"/>
-        <c:axId val="-2028499432"/>
+        <c:axId val="1788842264"/>
+        <c:axId val="1788839448"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="-2028502440"/>
+        <c:axId val="1788842264"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -13576,7 +13536,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-2028499432"/>
+        <c:crossAx val="1788839448"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -13584,7 +13544,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="-2028499432"/>
+        <c:axId val="1788839448"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -13595,14 +13555,13 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-2028502440"/>
+        <c:crossAx val="1788842264"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
     </c:plotArea>
     <c:legend>
       <c:legendPos val="r"/>
-      <c:layout/>
       <c:overlay val="0"/>
     </c:legend>
     <c:plotVisOnly val="1"/>
@@ -13757,11 +13716,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="-2032824344"/>
-        <c:axId val="-2032763480"/>
+        <c:axId val="-2068193144"/>
+        <c:axId val="-2068190136"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="-2032824344"/>
+        <c:axId val="-2068193144"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -13770,7 +13729,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-2032763480"/>
+        <c:crossAx val="-2068190136"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -13778,7 +13737,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="-2032763480"/>
+        <c:axId val="-2068190136"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -13789,14 +13748,13 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-2032824344"/>
+        <c:crossAx val="-2068193144"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
     </c:plotArea>
     <c:legend>
       <c:legendPos val="r"/>
-      <c:layout/>
       <c:overlay val="0"/>
     </c:legend>
     <c:plotVisOnly val="1"/>
@@ -13961,11 +13919,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="-2032221544"/>
-        <c:axId val="-2120268696"/>
+        <c:axId val="-2068218584"/>
+        <c:axId val="-2068224536"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="-2032221544"/>
+        <c:axId val="-2068218584"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -13974,7 +13932,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-2120268696"/>
+        <c:crossAx val="-2068224536"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -13982,7 +13940,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="-2120268696"/>
+        <c:axId val="-2068224536"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:min val="15.0"/>
@@ -13994,14 +13952,13 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-2032221544"/>
+        <c:crossAx val="-2068218584"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
     </c:plotArea>
     <c:legend>
       <c:legendPos val="r"/>
-      <c:layout/>
       <c:overlay val="0"/>
     </c:legend>
     <c:plotVisOnly val="1"/>
@@ -14210,11 +14167,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:gapWidth val="150"/>
-        <c:axId val="-2029357320"/>
-        <c:axId val="-2029354312"/>
+        <c:axId val="1784013640"/>
+        <c:axId val="1784016648"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="-2029357320"/>
+        <c:axId val="1784013640"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -14223,7 +14180,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-2029354312"/>
+        <c:crossAx val="1784016648"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -14231,7 +14188,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="-2029354312"/>
+        <c:axId val="1784016648"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -14242,14 +14199,13 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-2029357320"/>
+        <c:crossAx val="1784013640"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
     </c:plotArea>
     <c:legend>
       <c:legendPos val="r"/>
-      <c:layout/>
       <c:overlay val="0"/>
     </c:legend>
     <c:plotVisOnly val="1"/>
@@ -14401,11 +14357,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:gapWidth val="150"/>
-        <c:axId val="-2028091176"/>
-        <c:axId val="-2028088168"/>
+        <c:axId val="-2068244696"/>
+        <c:axId val="-2068272568"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="-2028091176"/>
+        <c:axId val="-2068244696"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -14414,7 +14370,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-2028088168"/>
+        <c:crossAx val="-2068272568"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -14422,7 +14378,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="-2028088168"/>
+        <c:axId val="-2068272568"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -14433,7 +14389,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-2028091176"/>
+        <c:crossAx val="-2068244696"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -14652,11 +14608,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="-2028959384"/>
-        <c:axId val="-2028956376"/>
+        <c:axId val="1784606872"/>
+        <c:axId val="1784638040"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="-2028959384"/>
+        <c:axId val="1784606872"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -14665,7 +14621,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-2028956376"/>
+        <c:crossAx val="1784638040"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -14673,7 +14629,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="-2028956376"/>
+        <c:axId val="1784638040"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -14684,14 +14640,13 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-2028959384"/>
+        <c:crossAx val="1784606872"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
     </c:plotArea>
     <c:legend>
       <c:legendPos val="r"/>
-      <c:layout/>
       <c:overlay val="0"/>
     </c:legend>
     <c:plotVisOnly val="1"/>
@@ -14913,11 +14868,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="-2028924744"/>
-        <c:axId val="-2028921736"/>
+        <c:axId val="2129774136"/>
+        <c:axId val="-2098146232"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="-2028924744"/>
+        <c:axId val="2129774136"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -14926,7 +14881,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-2028921736"/>
+        <c:crossAx val="-2098146232"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -14934,7 +14889,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="-2028921736"/>
+        <c:axId val="-2098146232"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:min val="4.3"/>
@@ -14946,14 +14901,13 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-2028924744"/>
+        <c:crossAx val="2129774136"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
     </c:plotArea>
     <c:legend>
       <c:legendPos val="r"/>
-      <c:layout/>
       <c:overlay val="0"/>
     </c:legend>
     <c:plotVisOnly val="1"/>
@@ -15162,11 +15116,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:gapWidth val="150"/>
-        <c:axId val="-2028898248"/>
-        <c:axId val="-2028895240"/>
+        <c:axId val="1783972568"/>
+        <c:axId val="-2083895080"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="-2028898248"/>
+        <c:axId val="1783972568"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -15175,7 +15129,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-2028895240"/>
+        <c:crossAx val="-2083895080"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -15183,7 +15137,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="-2028895240"/>
+        <c:axId val="-2083895080"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -15194,14 +15148,13 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-2028898248"/>
+        <c:crossAx val="1783972568"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
     </c:plotArea>
     <c:legend>
       <c:legendPos val="r"/>
-      <c:layout/>
       <c:overlay val="0"/>
     </c:legend>
     <c:plotVisOnly val="1"/>
@@ -16091,16 +16044,16 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>4</xdr:col>
-      <xdr:colOff>38100</xdr:colOff>
-      <xdr:row>13</xdr:row>
-      <xdr:rowOff>101600</xdr:rowOff>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>14</xdr:row>
+      <xdr:rowOff>139700</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>12</xdr:col>
-      <xdr:colOff>203200</xdr:colOff>
-      <xdr:row>28</xdr:row>
-      <xdr:rowOff>38100</xdr:rowOff>
+      <xdr:col>13</xdr:col>
+      <xdr:colOff>165100</xdr:colOff>
+      <xdr:row>29</xdr:row>
+      <xdr:rowOff>76200</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -16153,16 +16106,16 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>12</xdr:col>
-      <xdr:colOff>622300</xdr:colOff>
+      <xdr:col>14</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
       <xdr:row>13</xdr:row>
-      <xdr:rowOff>63500</xdr:rowOff>
+      <xdr:rowOff>152400</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>22</xdr:col>
-      <xdr:colOff>254000</xdr:colOff>
-      <xdr:row>30</xdr:row>
-      <xdr:rowOff>127000</xdr:rowOff>
+      <xdr:col>23</xdr:col>
+      <xdr:colOff>457200</xdr:colOff>
+      <xdr:row>31</xdr:row>
+      <xdr:rowOff>25400</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -24656,13 +24609,10 @@
 
 <file path=xl/worksheets/sheet15.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <sheetPr enableFormatConditionsCalculation="0">
-    <tabColor rgb="FF008000"/>
-  </sheetPr>
-  <dimension ref="A2:BA13"/>
+  <dimension ref="A2:BA14"/>
   <sheetViews>
-    <sheetView topLeftCell="A17" workbookViewId="0">
-      <selection activeCell="BA7" sqref="BA7"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E15" sqref="E15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -25748,6 +25698,23 @@
       </c>
       <c r="G13" s="1" t="s">
         <v>32</v>
+      </c>
+    </row>
+    <row r="14" spans="1:53">
+      <c r="A14" t="s">
+        <v>71</v>
+      </c>
+      <c r="B14" s="38">
+        <v>46661</v>
+      </c>
+      <c r="C14">
+        <v>400</v>
+      </c>
+      <c r="D14">
+        <v>11.04</v>
+      </c>
+      <c r="E14">
+        <v>-6600</v>
       </c>
     </row>
   </sheetData>
@@ -27968,13 +27935,10 @@
 
 <file path=xl/worksheets/sheet18.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <sheetPr enableFormatConditionsCalculation="0">
-    <tabColor rgb="FFFFFF00"/>
-  </sheetPr>
-  <dimension ref="A2:AN13"/>
+  <dimension ref="A2:AN14"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="AN7" sqref="AN7"/>
+      <selection activeCell="E14" sqref="E14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -28797,6 +28761,23 @@
       </c>
       <c r="D13" s="10">
         <v>14.318</v>
+      </c>
+    </row>
+    <row r="14" spans="1:40">
+      <c r="A14" t="s">
+        <v>71</v>
+      </c>
+      <c r="B14" s="38">
+        <v>46661</v>
+      </c>
+      <c r="C14">
+        <v>800</v>
+      </c>
+      <c r="D14">
+        <v>5.52</v>
+      </c>
+      <c r="E14">
+        <v>-7040</v>
       </c>
     </row>
   </sheetData>
@@ -30741,7 +30722,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A2:AH13"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="W1" workbookViewId="0">
+    <sheetView topLeftCell="W1" workbookViewId="0">
       <selection activeCell="AH7" sqref="AH7"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
exchange better stock. Maybe =。=
</commit_message>
<xml_diff>
--- a/stock.xlsx
+++ b/stock.xlsx
@@ -1,10 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="22416"/>
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="26405"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="900" yWindow="0" windowWidth="25600" windowHeight="16060" tabRatio="996" activeTab="19"/>
+    <workbookView xWindow="4200" yWindow="2660" windowWidth="25600" windowHeight="16060" tabRatio="996" activeTab="7"/>
   </bookViews>
   <sheets>
     <sheet name="美的集团" sheetId="21" r:id="rId1"/>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="282" uniqueCount="72">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="287" uniqueCount="72">
   <si>
     <t>达华智能</t>
   </si>
@@ -594,7 +594,7 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="41">
+  <cellXfs count="42">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
@@ -636,6 +636,7 @@
     <xf numFmtId="17" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="17" fontId="7" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="17" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
   </cellXfs>
   <cellStyles count="133">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
@@ -872,11 +873,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="2145201352"/>
-        <c:axId val="2144453688"/>
+        <c:axId val="1774113704"/>
+        <c:axId val="1774116712"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="2145201352"/>
+        <c:axId val="1774113704"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -885,7 +886,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="2144453688"/>
+        <c:crossAx val="1774116712"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -893,7 +894,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="2144453688"/>
+        <c:axId val="1774116712"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -904,7 +905,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="2145201352"/>
+        <c:crossAx val="1774113704"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -1129,11 +1130,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="-2021750456"/>
-        <c:axId val="-2021747448"/>
+        <c:axId val="1773233704"/>
+        <c:axId val="1773251592"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="-2021750456"/>
+        <c:axId val="1773233704"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1142,7 +1143,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-2021747448"/>
+        <c:crossAx val="1773251592"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -1150,7 +1151,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="-2021747448"/>
+        <c:axId val="1773251592"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1161,14 +1162,13 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-2021750456"/>
+        <c:crossAx val="1773233704"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
     </c:plotArea>
     <c:legend>
       <c:legendPos val="r"/>
-      <c:layout/>
       <c:overlay val="0"/>
     </c:legend>
     <c:plotVisOnly val="1"/>
@@ -1396,11 +1396,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="-2021810088"/>
-        <c:axId val="-2021807080"/>
+        <c:axId val="1773355464"/>
+        <c:axId val="1773358472"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="-2021810088"/>
+        <c:axId val="1773355464"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1409,7 +1409,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-2021807080"/>
+        <c:crossAx val="1773358472"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -1417,7 +1417,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="-2021807080"/>
+        <c:axId val="1773358472"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:min val="16.5"/>
@@ -1429,14 +1429,13 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-2021810088"/>
+        <c:crossAx val="1773355464"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
     </c:plotArea>
     <c:legend>
       <c:legendPos val="r"/>
-      <c:layout/>
       <c:overlay val="0"/>
     </c:legend>
     <c:plotVisOnly val="1"/>
@@ -1651,11 +1650,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:gapWidth val="150"/>
-        <c:axId val="-2022623272"/>
-        <c:axId val="-2022620264"/>
+        <c:axId val="1773228792"/>
+        <c:axId val="1773209912"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="-2022623272"/>
+        <c:axId val="1773228792"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1664,7 +1663,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-2022620264"/>
+        <c:crossAx val="1773209912"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -1672,7 +1671,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="-2022620264"/>
+        <c:axId val="1773209912"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1683,14 +1682,13 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-2022623272"/>
+        <c:crossAx val="1773228792"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
     </c:plotArea>
     <c:legend>
       <c:legendPos val="r"/>
-      <c:layout/>
       <c:overlay val="0"/>
     </c:legend>
     <c:plotVisOnly val="1"/>
@@ -1908,11 +1906,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="-2021836904"/>
-        <c:axId val="-2021833896"/>
+        <c:axId val="1772797752"/>
+        <c:axId val="1772795800"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="-2021836904"/>
+        <c:axId val="1772797752"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1921,7 +1919,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-2021833896"/>
+        <c:crossAx val="1772795800"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -1929,7 +1927,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="-2021833896"/>
+        <c:axId val="1772795800"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1940,7 +1938,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-2021836904"/>
+        <c:crossAx val="1772797752"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -2175,11 +2173,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="-2022101624"/>
-        <c:axId val="-2022098616"/>
+        <c:axId val="1773171144"/>
+        <c:axId val="1773198184"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="-2022101624"/>
+        <c:axId val="1773171144"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2188,7 +2186,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-2022098616"/>
+        <c:crossAx val="1773198184"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -2196,7 +2194,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="-2022098616"/>
+        <c:axId val="1773198184"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2207,7 +2205,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-2022101624"/>
+        <c:crossAx val="1773171144"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -2429,11 +2427,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:gapWidth val="150"/>
-        <c:axId val="2145307320"/>
-        <c:axId val="-2022630776"/>
+        <c:axId val="1773180904"/>
+        <c:axId val="1773332536"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="2145307320"/>
+        <c:axId val="1773180904"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2442,7 +2440,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-2022630776"/>
+        <c:crossAx val="1773332536"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -2450,7 +2448,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="-2022630776"/>
+        <c:axId val="1773332536"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2461,7 +2459,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="2145307320"/>
+        <c:crossAx val="1773180904"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -2686,11 +2684,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="-2021894536"/>
-        <c:axId val="-2022409784"/>
+        <c:axId val="2043528472"/>
+        <c:axId val="2043506936"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="-2021894536"/>
+        <c:axId val="2043528472"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2699,7 +2697,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-2022409784"/>
+        <c:crossAx val="2043506936"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -2707,7 +2705,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="-2022409784"/>
+        <c:axId val="2043506936"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2718,14 +2716,13 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-2021894536"/>
+        <c:crossAx val="2043528472"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
     </c:plotArea>
     <c:legend>
       <c:legendPos val="r"/>
-      <c:layout/>
       <c:overlay val="0"/>
     </c:legend>
     <c:plotVisOnly val="1"/>
@@ -2953,11 +2950,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="-2022377880"/>
-        <c:axId val="-2022413656"/>
+        <c:axId val="1772807080"/>
+        <c:axId val="1772461784"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="-2022377880"/>
+        <c:axId val="1772807080"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2966,7 +2963,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-2022413656"/>
+        <c:crossAx val="1772461784"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -2974,7 +2971,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="-2022413656"/>
+        <c:axId val="1772461784"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2985,14 +2982,13 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-2022377880"/>
+        <c:crossAx val="1772807080"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
     </c:plotArea>
     <c:legend>
       <c:legendPos val="r"/>
-      <c:layout/>
       <c:overlay val="0"/>
     </c:legend>
     <c:plotVisOnly val="1"/>
@@ -3207,11 +3203,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:gapWidth val="150"/>
-        <c:axId val="-2022256696"/>
-        <c:axId val="-2022502296"/>
+        <c:axId val="1773418584"/>
+        <c:axId val="1773402984"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="-2022256696"/>
+        <c:axId val="1773418584"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3220,7 +3216,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-2022502296"/>
+        <c:crossAx val="1773402984"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -3228,7 +3224,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="-2022502296"/>
+        <c:axId val="1773402984"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3239,14 +3235,13 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-2022256696"/>
+        <c:crossAx val="1773418584"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
     </c:plotArea>
     <c:legend>
       <c:legendPos val="r"/>
-      <c:layout/>
       <c:overlay val="0"/>
     </c:legend>
     <c:plotVisOnly val="1"/>
@@ -3464,11 +3459,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="-2022514008"/>
-        <c:axId val="-2022511000"/>
+        <c:axId val="2039211016"/>
+        <c:axId val="2029701336"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="-2022514008"/>
+        <c:axId val="2039211016"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3477,7 +3472,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-2022511000"/>
+        <c:crossAx val="2029701336"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -3485,7 +3480,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="-2022511000"/>
+        <c:axId val="2029701336"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3496,14 +3491,13 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-2022514008"/>
+        <c:crossAx val="2039211016"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
     </c:plotArea>
     <c:legend>
       <c:legendPos val="r"/>
-      <c:layout/>
       <c:overlay val="0"/>
     </c:legend>
     <c:plotVisOnly val="1"/>
@@ -3613,11 +3607,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="2145156136"/>
-        <c:axId val="2144986792"/>
+        <c:axId val="1773829816"/>
+        <c:axId val="1773832824"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="2145156136"/>
+        <c:axId val="1773829816"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3626,7 +3620,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="2144986792"/>
+        <c:crossAx val="1773832824"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -3634,7 +3628,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="2144986792"/>
+        <c:axId val="1773832824"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3645,7 +3639,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="2145156136"/>
+        <c:crossAx val="1773829816"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -3880,11 +3874,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="2145315704"/>
-        <c:axId val="2145312664"/>
+        <c:axId val="2039280040"/>
+        <c:axId val="1783818808"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="2145315704"/>
+        <c:axId val="2039280040"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3893,7 +3887,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="2145312664"/>
+        <c:crossAx val="1783818808"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -3901,7 +3895,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="2145312664"/>
+        <c:axId val="1783818808"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3912,14 +3906,13 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="2145315704"/>
+        <c:crossAx val="2039280040"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
     </c:plotArea>
     <c:legend>
       <c:legendPos val="r"/>
-      <c:layout/>
       <c:overlay val="0"/>
     </c:legend>
     <c:plotVisOnly val="1"/>
@@ -4134,11 +4127,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:gapWidth val="150"/>
-        <c:axId val="2144427288"/>
-        <c:axId val="2144390824"/>
+        <c:axId val="1783822600"/>
+        <c:axId val="1783879880"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="2144427288"/>
+        <c:axId val="1783822600"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -4147,7 +4140,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="2144390824"/>
+        <c:crossAx val="1783879880"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -4155,7 +4148,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="2144390824"/>
+        <c:axId val="1783879880"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -4166,14 +4159,13 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="2144427288"/>
+        <c:crossAx val="1783822600"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
     </c:plotArea>
     <c:legend>
       <c:legendPos val="r"/>
-      <c:layout/>
       <c:overlay val="0"/>
     </c:legend>
     <c:plotVisOnly val="1"/>
@@ -4391,11 +4383,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="2145236360"/>
-        <c:axId val="-2022299752"/>
+        <c:axId val="1772543224"/>
+        <c:axId val="1772546280"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="2145236360"/>
+        <c:axId val="1772543224"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -4404,7 +4396,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-2022299752"/>
+        <c:crossAx val="1772546280"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -4412,7 +4404,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="-2022299752"/>
+        <c:axId val="1772546280"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -4423,7 +4415,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="2145236360"/>
+        <c:crossAx val="1772543224"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -4658,11 +4650,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="-2021953768"/>
-        <c:axId val="-2021950760"/>
+        <c:axId val="1772506872"/>
+        <c:axId val="1772509880"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="-2021953768"/>
+        <c:axId val="1772506872"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -4671,7 +4663,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-2021950760"/>
+        <c:crossAx val="1772509880"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -4679,7 +4671,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="-2021950760"/>
+        <c:axId val="1772509880"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -4690,7 +4682,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-2021953768"/>
+        <c:crossAx val="1772506872"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -4912,11 +4904,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:gapWidth val="150"/>
-        <c:axId val="-2021927784"/>
-        <c:axId val="-2021924776"/>
+        <c:axId val="2043230856"/>
+        <c:axId val="2042871544"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="-2021927784"/>
+        <c:axId val="2043230856"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -4925,7 +4917,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-2021924776"/>
+        <c:crossAx val="2042871544"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -4933,7 +4925,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="-2021924776"/>
+        <c:axId val="2042871544"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -4944,7 +4936,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-2021927784"/>
+        <c:crossAx val="2043230856"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -5169,11 +5161,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="-2021802136"/>
-        <c:axId val="-2021799128"/>
+        <c:axId val="1772515784"/>
+        <c:axId val="1772524344"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="-2021802136"/>
+        <c:axId val="1772515784"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -5182,7 +5174,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-2021799128"/>
+        <c:crossAx val="1772524344"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -5190,7 +5182,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="-2021799128"/>
+        <c:axId val="1772524344"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -5201,14 +5193,13 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-2021802136"/>
+        <c:crossAx val="1772515784"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
     </c:plotArea>
     <c:legend>
       <c:legendPos val="r"/>
-      <c:layout/>
       <c:overlay val="0"/>
     </c:legend>
     <c:plotVisOnly val="1"/>
@@ -5436,11 +5427,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="-2021887256"/>
-        <c:axId val="-2021884248"/>
+        <c:axId val="2039271480"/>
+        <c:axId val="-2104708776"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="-2021887256"/>
+        <c:axId val="2039271480"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -5449,7 +5440,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-2021884248"/>
+        <c:crossAx val="-2104708776"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -5457,7 +5448,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="-2021884248"/>
+        <c:axId val="-2104708776"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -5468,14 +5459,13 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-2021887256"/>
+        <c:crossAx val="2039271480"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
     </c:plotArea>
     <c:legend>
       <c:legendPos val="r"/>
-      <c:layout/>
       <c:overlay val="0"/>
     </c:legend>
     <c:plotVisOnly val="1"/>
@@ -5690,11 +5680,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:gapWidth val="150"/>
-        <c:axId val="-2022126760"/>
-        <c:axId val="-2022123976"/>
+        <c:axId val="1773554328"/>
+        <c:axId val="1773557352"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="-2022126760"/>
+        <c:axId val="1773554328"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -5703,7 +5693,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-2022123976"/>
+        <c:crossAx val="1773557352"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -5711,7 +5701,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="-2022123976"/>
+        <c:axId val="1773557352"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -5722,14 +5712,13 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-2022126760"/>
+        <c:crossAx val="1773554328"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
     </c:plotArea>
     <c:legend>
       <c:legendPos val="r"/>
-      <c:layout/>
       <c:overlay val="0"/>
     </c:legend>
     <c:plotVisOnly val="1"/>
@@ -5947,11 +5936,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="-2022065944"/>
-        <c:axId val="-2022063256"/>
+        <c:axId val="2028629464"/>
+        <c:axId val="2038687160"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="-2022065944"/>
+        <c:axId val="2028629464"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -5960,7 +5949,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-2022063256"/>
+        <c:crossAx val="2038687160"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -5968,7 +5957,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="-2022063256"/>
+        <c:axId val="2038687160"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -5979,14 +5968,13 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-2022065944"/>
+        <c:crossAx val="2028629464"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
     </c:plotArea>
     <c:legend>
       <c:legendPos val="r"/>
-      <c:layout/>
       <c:overlay val="0"/>
     </c:legend>
     <c:plotVisOnly val="1"/>
@@ -6214,11 +6202,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="-2022033128"/>
-        <c:axId val="-2022030120"/>
+        <c:axId val="2029842872"/>
+        <c:axId val="1783809976"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="-2022033128"/>
+        <c:axId val="2029842872"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -6227,7 +6215,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-2022030120"/>
+        <c:crossAx val="1783809976"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -6235,7 +6223,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="-2022030120"/>
+        <c:axId val="1783809976"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -6246,14 +6234,13 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-2022033128"/>
+        <c:crossAx val="2029842872"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
     </c:plotArea>
     <c:legend>
       <c:legendPos val="r"/>
-      <c:layout/>
       <c:overlay val="0"/>
     </c:legend>
     <c:plotVisOnly val="1"/>
@@ -6360,11 +6347,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:gapWidth val="150"/>
-        <c:axId val="2144556664"/>
-        <c:axId val="2145318680"/>
+        <c:axId val="1773653656"/>
+        <c:axId val="1773543576"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="2144556664"/>
+        <c:axId val="1773653656"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -6373,7 +6360,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="2145318680"/>
+        <c:crossAx val="1773543576"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -6381,7 +6368,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="2145318680"/>
+        <c:axId val="1773543576"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -6392,7 +6379,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="2144556664"/>
+        <c:crossAx val="1773653656"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -6614,11 +6601,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:gapWidth val="150"/>
-        <c:axId val="-2022352264"/>
-        <c:axId val="-2022600408"/>
+        <c:axId val="1772375304"/>
+        <c:axId val="1772378136"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="-2022352264"/>
+        <c:axId val="1772375304"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -6627,7 +6614,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-2022600408"/>
+        <c:crossAx val="1772378136"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -6635,7 +6622,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="-2022600408"/>
+        <c:axId val="1772378136"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -6646,14 +6633,13 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-2022352264"/>
+        <c:crossAx val="1772375304"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
     </c:plotArea>
     <c:legend>
       <c:legendPos val="r"/>
-      <c:layout/>
       <c:overlay val="0"/>
     </c:legend>
     <c:plotVisOnly val="1"/>
@@ -6871,11 +6857,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="-2022075656"/>
-        <c:axId val="-2022592376"/>
+        <c:axId val="1773740184"/>
+        <c:axId val="1773728600"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="-2022075656"/>
+        <c:axId val="1773740184"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -6884,7 +6870,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-2022592376"/>
+        <c:crossAx val="1773728600"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -6892,7 +6878,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="-2022592376"/>
+        <c:axId val="1773728600"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -6903,14 +6889,13 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-2022075656"/>
+        <c:crossAx val="1773740184"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
     </c:plotArea>
     <c:legend>
       <c:legendPos val="r"/>
-      <c:layout/>
       <c:overlay val="0"/>
     </c:legend>
     <c:plotVisOnly val="1"/>
@@ -7138,11 +7123,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="-2022673048"/>
-        <c:axId val="-2022670040"/>
+        <c:axId val="1783842152"/>
+        <c:axId val="1783831640"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="-2022673048"/>
+        <c:axId val="1783842152"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -7151,7 +7136,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-2022670040"/>
+        <c:crossAx val="1783831640"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -7159,7 +7144,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="-2022670040"/>
+        <c:axId val="1783831640"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:min val="3.0"/>
@@ -7171,14 +7156,13 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-2022673048"/>
+        <c:crossAx val="1783842152"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
     </c:plotArea>
     <c:legend>
       <c:legendPos val="r"/>
-      <c:layout/>
       <c:overlay val="0"/>
     </c:legend>
     <c:plotVisOnly val="1"/>
@@ -7393,11 +7377,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:gapWidth val="150"/>
-        <c:axId val="-2022681640"/>
-        <c:axId val="-2021740440"/>
+        <c:axId val="1783836936"/>
+        <c:axId val="2042884584"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="-2022681640"/>
+        <c:axId val="1783836936"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -7406,7 +7390,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-2021740440"/>
+        <c:crossAx val="2042884584"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -7414,7 +7398,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="-2021740440"/>
+        <c:axId val="2042884584"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -7425,14 +7409,13 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-2022681640"/>
+        <c:crossAx val="1783836936"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
     </c:plotArea>
     <c:legend>
       <c:legendPos val="r"/>
-      <c:layout/>
       <c:overlay val="0"/>
     </c:legend>
     <c:plotVisOnly val="1"/>
@@ -7650,11 +7633,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="-2021700744"/>
-        <c:axId val="-2021697736"/>
+        <c:axId val="1773772136"/>
+        <c:axId val="1773775144"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="-2021700744"/>
+        <c:axId val="1773772136"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -7663,7 +7646,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-2021697736"/>
+        <c:crossAx val="1773775144"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -7671,7 +7654,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="-2021697736"/>
+        <c:axId val="1773775144"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -7682,7 +7665,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-2021700744"/>
+        <c:crossAx val="1773772136"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -7917,11 +7900,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="-2022367032"/>
-        <c:axId val="2089212296"/>
+        <c:axId val="1773822840"/>
+        <c:axId val="1773825816"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="-2022367032"/>
+        <c:axId val="1773822840"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -7930,7 +7913,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="2089212296"/>
+        <c:crossAx val="1773825816"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -7938,7 +7921,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="2089212296"/>
+        <c:axId val="1773825816"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:min val="6.5"/>
@@ -7950,7 +7933,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-2022367032"/>
+        <c:crossAx val="1773822840"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -8172,11 +8155,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:gapWidth val="150"/>
-        <c:axId val="-2095409752"/>
-        <c:axId val="-2095074488"/>
+        <c:axId val="2042607608"/>
+        <c:axId val="2042366520"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="-2095409752"/>
+        <c:axId val="2042607608"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -8185,7 +8168,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-2095074488"/>
+        <c:crossAx val="2042366520"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -8193,7 +8176,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="-2095074488"/>
+        <c:axId val="2042366520"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -8204,7 +8187,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-2095409752"/>
+        <c:crossAx val="2042607608"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -8429,11 +8412,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="-2095294936"/>
-        <c:axId val="-2095610312"/>
+        <c:axId val="2042694040"/>
+        <c:axId val="2042697048"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="-2095294936"/>
+        <c:axId val="2042694040"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -8442,7 +8425,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-2095610312"/>
+        <c:crossAx val="2042697048"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -8450,7 +8433,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="-2095610312"/>
+        <c:axId val="2042697048"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -8461,7 +8444,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-2095294936"/>
+        <c:crossAx val="2042694040"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -8696,11 +8679,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="-2095956760"/>
-        <c:axId val="-2095200872"/>
+        <c:axId val="1773667032"/>
+        <c:axId val="1773877752"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="-2095956760"/>
+        <c:axId val="1773667032"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -8709,7 +8692,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-2095200872"/>
+        <c:crossAx val="1773877752"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -8717,7 +8700,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="-2095200872"/>
+        <c:axId val="1773877752"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -8728,7 +8711,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-2095956760"/>
+        <c:crossAx val="1773667032"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -8950,11 +8933,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:gapWidth val="150"/>
-        <c:axId val="-2095689400"/>
-        <c:axId val="-2095708264"/>
+        <c:axId val="1773852056"/>
+        <c:axId val="1773293032"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="-2095689400"/>
+        <c:axId val="1773852056"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -8963,7 +8946,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-2095708264"/>
+        <c:crossAx val="1773293032"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -8971,7 +8954,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="-2095708264"/>
+        <c:axId val="1773293032"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -8982,7 +8965,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-2095689400"/>
+        <c:crossAx val="1773852056"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -9207,11 +9190,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="-2022285368"/>
-        <c:axId val="-2021796312"/>
+        <c:axId val="1774002488"/>
+        <c:axId val="1774005432"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="-2022285368"/>
+        <c:axId val="1774002488"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -9220,7 +9203,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-2021796312"/>
+        <c:crossAx val="1774005432"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -9228,7 +9211,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="-2021796312"/>
+        <c:axId val="1774005432"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -9239,7 +9222,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-2022285368"/>
+        <c:crossAx val="1774002488"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -9464,11 +9447,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="-2095097032"/>
-        <c:axId val="-2095105016"/>
+        <c:axId val="1774061784"/>
+        <c:axId val="1774064792"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="-2095097032"/>
+        <c:axId val="1774061784"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -9477,7 +9460,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-2095105016"/>
+        <c:crossAx val="1774064792"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -9485,7 +9468,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="-2095105016"/>
+        <c:axId val="1774064792"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -9496,7 +9479,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-2095097032"/>
+        <c:crossAx val="1774061784"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -9731,11 +9714,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="-2095150616"/>
-        <c:axId val="-2095154920"/>
+        <c:axId val="-2101862120"/>
+        <c:axId val="2039608664"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="-2095150616"/>
+        <c:axId val="-2101862120"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -9744,7 +9727,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-2095154920"/>
+        <c:crossAx val="2039608664"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -9752,7 +9735,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="-2095154920"/>
+        <c:axId val="2039608664"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -9763,7 +9746,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-2095150616"/>
+        <c:crossAx val="-2101862120"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -9985,11 +9968,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:gapWidth val="150"/>
-        <c:axId val="-2095182568"/>
-        <c:axId val="-2095186024"/>
+        <c:axId val="2029213720"/>
+        <c:axId val="2029199880"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="-2095182568"/>
+        <c:axId val="2029213720"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -9998,7 +9981,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-2095186024"/>
+        <c:crossAx val="2029199880"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -10006,7 +9989,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="-2095186024"/>
+        <c:axId val="2029199880"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -10017,7 +10000,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-2095182568"/>
+        <c:crossAx val="2029213720"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -10242,11 +10225,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="-2095243480"/>
-        <c:axId val="-2095240568"/>
+        <c:axId val="2039617304"/>
+        <c:axId val="2039620360"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="-2095243480"/>
+        <c:axId val="2039617304"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -10255,7 +10238,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-2095240568"/>
+        <c:crossAx val="2039620360"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -10263,7 +10246,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="-2095240568"/>
+        <c:axId val="2039620360"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -10274,7 +10257,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-2095243480"/>
+        <c:crossAx val="2039617304"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -10509,11 +10492,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="-2095269128"/>
-        <c:axId val="-2095281352"/>
+        <c:axId val="1788170216"/>
+        <c:axId val="1788193992"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="-2095269128"/>
+        <c:axId val="1788170216"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -10522,7 +10505,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-2095281352"/>
+        <c:crossAx val="1788193992"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -10530,7 +10513,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="-2095281352"/>
+        <c:axId val="1788193992"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:min val="8.0"/>
@@ -10542,7 +10525,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-2095269128"/>
+        <c:crossAx val="1788170216"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -10764,11 +10747,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:gapWidth val="150"/>
-        <c:axId val="-2095313256"/>
-        <c:axId val="-2095314360"/>
+        <c:axId val="2043743192"/>
+        <c:axId val="2043746248"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="-2095313256"/>
+        <c:axId val="2043743192"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -10777,7 +10760,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-2095314360"/>
+        <c:crossAx val="2043746248"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -10785,7 +10768,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="-2095314360"/>
+        <c:axId val="2043746248"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -10796,7 +10779,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-2095313256"/>
+        <c:crossAx val="2043743192"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -11021,11 +11004,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="-2095370344"/>
-        <c:axId val="-2095374968"/>
+        <c:axId val="-2095603144"/>
+        <c:axId val="-2095600136"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="-2095370344"/>
+        <c:axId val="-2095603144"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -11034,7 +11017,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-2095374968"/>
+        <c:crossAx val="-2095600136"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -11042,7 +11025,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="-2095374968"/>
+        <c:axId val="-2095600136"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -11053,7 +11036,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-2095370344"/>
+        <c:crossAx val="-2095603144"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -11278,11 +11261,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="-2095416152"/>
-        <c:axId val="-2095426392"/>
+        <c:axId val="1773944904"/>
+        <c:axId val="1773947960"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="-2095416152"/>
+        <c:axId val="1773944904"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -11291,7 +11274,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-2095426392"/>
+        <c:crossAx val="1773947960"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -11299,7 +11282,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="-2095426392"/>
+        <c:axId val="1773947960"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -11310,7 +11293,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-2095416152"/>
+        <c:crossAx val="1773944904"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -11532,11 +11515,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:gapWidth val="150"/>
-        <c:axId val="-2095470072"/>
-        <c:axId val="-2095477816"/>
+        <c:axId val="1774082584"/>
+        <c:axId val="1774085592"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="-2095470072"/>
+        <c:axId val="1774082584"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -11545,7 +11528,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-2095477816"/>
+        <c:crossAx val="1774085592"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -11553,7 +11536,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="-2095477816"/>
+        <c:axId val="1774085592"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -11564,7 +11547,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-2095470072"/>
+        <c:crossAx val="1774082584"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -11789,11 +11772,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="-2095533736"/>
-        <c:axId val="-2095540216"/>
+        <c:axId val="-2100224472"/>
+        <c:axId val="-2104656664"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="-2095533736"/>
+        <c:axId val="-2100224472"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -11802,7 +11785,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-2095540216"/>
+        <c:crossAx val="-2104656664"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -11810,7 +11793,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="-2095540216"/>
+        <c:axId val="-2104656664"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -11821,7 +11804,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-2095533736"/>
+        <c:crossAx val="-2100224472"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -12056,11 +12039,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="-2022419032"/>
-        <c:axId val="-2022391000"/>
+        <c:axId val="1773924680"/>
+        <c:axId val="1773927624"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="-2022419032"/>
+        <c:axId val="1773924680"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -12069,7 +12052,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-2022391000"/>
+        <c:crossAx val="1773927624"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -12077,7 +12060,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="-2022391000"/>
+        <c:axId val="1773927624"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:min val="15.0"/>
@@ -12089,7 +12072,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-2022419032"/>
+        <c:crossAx val="1773924680"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -12324,11 +12307,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="-2095595192"/>
-        <c:axId val="-2095617048"/>
+        <c:axId val="-2104632952"/>
+        <c:axId val="-2104629944"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="-2095595192"/>
+        <c:axId val="-2104632952"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -12337,7 +12320,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-2095617048"/>
+        <c:crossAx val="-2104629944"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -12345,7 +12328,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="-2095617048"/>
+        <c:axId val="-2104629944"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -12356,7 +12339,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-2095595192"/>
+        <c:crossAx val="-2104632952"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -12578,11 +12561,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:gapWidth val="150"/>
-        <c:axId val="-2095657352"/>
-        <c:axId val="-2095662264"/>
+        <c:axId val="-2100186088"/>
+        <c:axId val="-2100239144"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="-2095657352"/>
+        <c:axId val="-2100186088"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -12591,7 +12574,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-2095662264"/>
+        <c:crossAx val="-2100239144"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -12599,7 +12582,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="-2095662264"/>
+        <c:axId val="-2100239144"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -12610,7 +12593,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-2095657352"/>
+        <c:crossAx val="-2100186088"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -12796,11 +12779,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="-2095713784"/>
-        <c:axId val="-2095721080"/>
+        <c:axId val="1783850808"/>
+        <c:axId val="1783871112"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="-2095713784"/>
+        <c:axId val="1783850808"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -12809,7 +12792,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-2095721080"/>
+        <c:crossAx val="1783871112"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -12817,7 +12800,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="-2095721080"/>
+        <c:axId val="1783871112"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -12828,14 +12811,13 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-2095713784"/>
+        <c:crossAx val="1783850808"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
     </c:plotArea>
     <c:legend>
       <c:legendPos val="r"/>
-      <c:layout/>
       <c:overlay val="0"/>
     </c:legend>
     <c:plotVisOnly val="1"/>
@@ -13024,11 +13006,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="-2095805192"/>
-        <c:axId val="-2095848056"/>
+        <c:axId val="1774024696"/>
+        <c:axId val="1774022136"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="-2095805192"/>
+        <c:axId val="1774024696"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -13037,7 +13019,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-2095848056"/>
+        <c:crossAx val="1774022136"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -13045,7 +13027,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="-2095848056"/>
+        <c:axId val="1774022136"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -13056,14 +13038,13 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-2095805192"/>
+        <c:crossAx val="1774024696"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
     </c:plotArea>
     <c:legend>
       <c:legendPos val="r"/>
-      <c:layout/>
       <c:overlay val="0"/>
     </c:legend>
     <c:plotVisOnly val="1"/>
@@ -13239,11 +13220,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:gapWidth val="150"/>
-        <c:axId val="-2095888216"/>
-        <c:axId val="-2095892200"/>
+        <c:axId val="1774145992"/>
+        <c:axId val="1774125160"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="-2095888216"/>
+        <c:axId val="1774145992"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -13252,7 +13233,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-2095892200"/>
+        <c:crossAx val="1774125160"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -13260,7 +13241,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="-2095892200"/>
+        <c:axId val="1774125160"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -13271,14 +13252,13 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-2095888216"/>
+        <c:crossAx val="1774145992"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
     </c:plotArea>
     <c:legend>
       <c:legendPos val="r"/>
-      <c:layout/>
       <c:overlay val="0"/>
     </c:legend>
     <c:plotVisOnly val="1"/>
@@ -13454,11 +13434,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="-2095930808"/>
-        <c:axId val="-2095943560"/>
+        <c:axId val="-2029485480"/>
+        <c:axId val="-2029374360"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="-2095930808"/>
+        <c:axId val="-2029485480"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -13467,7 +13447,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-2095943560"/>
+        <c:crossAx val="-2029374360"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -13475,7 +13455,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="-2095943560"/>
+        <c:axId val="-2029374360"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -13486,14 +13466,13 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-2095930808"/>
+        <c:crossAx val="-2029485480"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
     </c:plotArea>
     <c:legend>
       <c:legendPos val="r"/>
-      <c:layout/>
       <c:overlay val="0"/>
     </c:legend>
     <c:plotVisOnly val="1"/>
@@ -13679,11 +13658,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="-2095990024"/>
-        <c:axId val="-2095992296"/>
+        <c:axId val="-2029083560"/>
+        <c:axId val="-2029293304"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="-2095990024"/>
+        <c:axId val="-2029083560"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -13692,7 +13671,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-2095992296"/>
+        <c:crossAx val="-2029293304"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -13700,7 +13679,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="-2095992296"/>
+        <c:axId val="-2029293304"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:min val="350.0"/>
@@ -13712,14 +13691,13 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-2095990024"/>
+        <c:crossAx val="-2029083560"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
     </c:plotArea>
     <c:legend>
       <c:legendPos val="r"/>
-      <c:layout/>
       <c:overlay val="0"/>
     </c:legend>
     <c:plotVisOnly val="1"/>
@@ -13892,11 +13870,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:gapWidth val="150"/>
-        <c:axId val="-2096021512"/>
-        <c:axId val="-2096018504"/>
+        <c:axId val="2043772168"/>
+        <c:axId val="2043775224"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="-2096021512"/>
+        <c:axId val="2043772168"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -13905,7 +13883,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-2096018504"/>
+        <c:crossAx val="2043775224"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -13913,7 +13891,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="-2096018504"/>
+        <c:axId val="2043775224"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -13924,14 +13902,13 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-2096021512"/>
+        <c:crossAx val="2043772168"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
     </c:plotArea>
     <c:legend>
       <c:legendPos val="r"/>
-      <c:layout/>
       <c:overlay val="0"/>
     </c:legend>
     <c:plotVisOnly val="1"/>
@@ -14092,11 +14069,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="-2096070840"/>
-        <c:axId val="-2096079688"/>
+        <c:axId val="-2029602472"/>
+        <c:axId val="-2029983352"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="-2096070840"/>
+        <c:axId val="-2029602472"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -14105,7 +14082,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-2096079688"/>
+        <c:crossAx val="-2029983352"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -14113,7 +14090,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="-2096079688"/>
+        <c:axId val="-2029983352"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -14124,14 +14101,13 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-2096070840"/>
+        <c:crossAx val="-2029602472"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
     </c:plotArea>
     <c:legend>
       <c:legendPos val="r"/>
-      <c:layout/>
       <c:overlay val="0"/>
     </c:legend>
     <c:plotVisOnly val="1"/>
@@ -14302,11 +14278,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="-2093784792"/>
-        <c:axId val="-2093083048"/>
+        <c:axId val="-2029012472"/>
+        <c:axId val="-2029015848"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="-2093784792"/>
+        <c:axId val="-2029012472"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -14315,7 +14291,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-2093083048"/>
+        <c:crossAx val="-2029015848"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -14323,7 +14299,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="-2093083048"/>
+        <c:axId val="-2029015848"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:min val="15.0"/>
@@ -14335,14 +14311,13 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-2093784792"/>
+        <c:crossAx val="-2029012472"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
     </c:plotArea>
     <c:legend>
       <c:legendPos val="r"/>
-      <c:layout/>
       <c:overlay val="0"/>
     </c:legend>
     <c:plotVisOnly val="1"/>
@@ -14557,11 +14532,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:gapWidth val="150"/>
-        <c:axId val="-2022307928"/>
-        <c:axId val="2089217368"/>
+        <c:axId val="1773708504"/>
+        <c:axId val="1773656920"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="-2022307928"/>
+        <c:axId val="1773708504"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -14570,7 +14545,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="2089217368"/>
+        <c:crossAx val="1773656920"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -14578,7 +14553,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="2089217368"/>
+        <c:axId val="1773656920"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -14589,7 +14564,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-2022307928"/>
+        <c:crossAx val="1773708504"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -14754,11 +14729,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:gapWidth val="150"/>
-        <c:axId val="-2093695672"/>
-        <c:axId val="-2093098952"/>
+        <c:axId val="-2029057672"/>
+        <c:axId val="-2029060472"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="-2093695672"/>
+        <c:axId val="-2029057672"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -14767,7 +14742,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-2093098952"/>
+        <c:crossAx val="-2029060472"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -14775,7 +14750,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="-2093098952"/>
+        <c:axId val="-2029060472"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -14786,14 +14761,13 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-2093695672"/>
+        <c:crossAx val="-2029057672"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
     </c:plotArea>
     <c:legend>
       <c:legendPos val="r"/>
-      <c:layout/>
       <c:overlay val="0"/>
     </c:legend>
     <c:plotVisOnly val="1"/>
@@ -15011,11 +14985,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="-2022465096"/>
-        <c:axId val="-2021988504"/>
+        <c:axId val="1773632072"/>
+        <c:axId val="1773674216"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="-2022465096"/>
+        <c:axId val="1773632072"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -15024,7 +14998,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-2021988504"/>
+        <c:crossAx val="1773674216"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -15032,7 +15006,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="-2021988504"/>
+        <c:axId val="1773674216"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -15043,14 +15017,13 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-2022465096"/>
+        <c:crossAx val="1773632072"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
     </c:plotArea>
     <c:legend>
       <c:legendPos val="r"/>
-      <c:layout/>
       <c:overlay val="0"/>
     </c:legend>
     <c:plotVisOnly val="1"/>
@@ -15278,11 +15251,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="-2022472600"/>
-        <c:axId val="-2022474360"/>
+        <c:axId val="2044306152"/>
+        <c:axId val="1772836376"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="-2022472600"/>
+        <c:axId val="2044306152"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -15291,7 +15264,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-2022474360"/>
+        <c:crossAx val="1772836376"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -15299,7 +15272,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="-2022474360"/>
+        <c:axId val="1772836376"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:min val="4.3"/>
@@ -15311,14 +15284,13 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-2022472600"/>
+        <c:crossAx val="2044306152"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
     </c:plotArea>
     <c:legend>
       <c:legendPos val="r"/>
-      <c:layout/>
       <c:overlay val="0"/>
     </c:legend>
     <c:plotVisOnly val="1"/>
@@ -15533,11 +15505,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:gapWidth val="150"/>
-        <c:axId val="-2022011496"/>
-        <c:axId val="-2022008488"/>
+        <c:axId val="1772774792"/>
+        <c:axId val="1772777800"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="-2022011496"/>
+        <c:axId val="1772774792"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -15546,7 +15518,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-2022008488"/>
+        <c:crossAx val="1772777800"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -15554,7 +15526,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="-2022008488"/>
+        <c:axId val="1772777800"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -15565,14 +15537,13 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-2022011496"/>
+        <c:crossAx val="1772774792"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
     </c:plotArea>
     <c:legend>
       <c:legendPos val="r"/>
-      <c:layout/>
       <c:overlay val="0"/>
     </c:legend>
     <c:plotVisOnly val="1"/>
@@ -21750,7 +21721,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A2:BC16"/>
   <sheetViews>
-    <sheetView topLeftCell="AL1" workbookViewId="0">
+    <sheetView topLeftCell="A13" workbookViewId="0">
       <selection activeCell="BC5" sqref="BC5"/>
     </sheetView>
   </sheetViews>
@@ -22974,7 +22945,7 @@
   </sheetPr>
   <dimension ref="A2:BC15"/>
   <sheetViews>
-    <sheetView topLeftCell="AN1" workbookViewId="0">
+    <sheetView topLeftCell="A6" workbookViewId="0">
       <selection activeCell="BC5" sqref="BC5"/>
     </sheetView>
   </sheetViews>
@@ -24142,10 +24113,10 @@
 
 <file path=xl/worksheets/sheet14.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A2:BC13"/>
+  <dimension ref="A2:BC14"/>
   <sheetViews>
-    <sheetView topLeftCell="AT1" workbookViewId="0">
-      <selection activeCell="BC5" sqref="BC5"/>
+    <sheetView topLeftCell="A9" workbookViewId="0">
+      <selection activeCell="E15" sqref="E15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -25280,6 +25251,23 @@
       </c>
       <c r="D13">
         <v>9.1660000000000004</v>
+      </c>
+    </row>
+    <row r="14" spans="1:55">
+      <c r="A14" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="B14" s="38">
+        <v>11597</v>
+      </c>
+      <c r="C14">
+        <v>800</v>
+      </c>
+      <c r="D14">
+        <v>5.09</v>
+      </c>
+      <c r="E14">
+        <v>-3139</v>
       </c>
     </row>
   </sheetData>
@@ -26458,10 +26446,10 @@
 
 <file path=xl/worksheets/sheet16.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A2:BC13"/>
+  <dimension ref="A2:BC14"/>
   <sheetViews>
-    <sheetView topLeftCell="AN1" workbookViewId="0">
-      <selection activeCell="BC5" sqref="BC5"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D15" sqref="D15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -27584,6 +27572,23 @@
       </c>
       <c r="D13" s="10">
         <v>7.2480000000000002</v>
+      </c>
+    </row>
+    <row r="14" spans="1:55">
+      <c r="A14" s="41" t="s">
+        <v>29</v>
+      </c>
+      <c r="B14" s="38">
+        <v>11597</v>
+      </c>
+      <c r="C14">
+        <v>600</v>
+      </c>
+      <c r="D14">
+        <v>3.04</v>
+      </c>
+      <c r="E14">
+        <v>-2508</v>
       </c>
     </row>
   </sheetData>
@@ -27600,10 +27605,10 @@
 
 <file path=xl/worksheets/sheet17.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A2:BC13"/>
+  <dimension ref="A2:BC14"/>
   <sheetViews>
-    <sheetView topLeftCell="AO1" workbookViewId="0">
-      <selection activeCell="BC5" sqref="BC5"/>
+    <sheetView topLeftCell="A8" workbookViewId="0">
+      <selection activeCell="E15" sqref="E15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -28726,6 +28731,23 @@
       </c>
       <c r="D13" s="10">
         <v>8.4870000000000001</v>
+      </c>
+    </row>
+    <row r="14" spans="1:55">
+      <c r="A14" s="41" t="s">
+        <v>29</v>
+      </c>
+      <c r="B14" s="38">
+        <v>11597</v>
+      </c>
+      <c r="C14">
+        <v>300</v>
+      </c>
+      <c r="D14">
+        <v>5.56</v>
+      </c>
+      <c r="E14">
+        <v>-887.8</v>
       </c>
     </row>
   </sheetData>
@@ -30505,10 +30527,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A2:BC13"/>
+  <dimension ref="A2:BC14"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="BC7" sqref="BC7"/>
+    <sheetView topLeftCell="A2" workbookViewId="0">
+      <selection activeCell="E15" sqref="E15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -31637,6 +31659,23 @@
       </c>
       <c r="D13" s="10">
         <v>27.286999999999999</v>
+      </c>
+    </row>
+    <row r="14" spans="1:55">
+      <c r="A14" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="B14" s="38">
+        <v>11597</v>
+      </c>
+      <c r="C14">
+        <v>300</v>
+      </c>
+      <c r="D14">
+        <v>15.71</v>
+      </c>
+      <c r="E14">
+        <v>-3434</v>
       </c>
     </row>
   </sheetData>
@@ -31655,7 +31694,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A2:AJ13"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="AB1" workbookViewId="0">
+    <sheetView topLeftCell="AB1" workbookViewId="0">
       <selection activeCell="AJ5" sqref="AJ5"/>
     </sheetView>
   </sheetViews>
@@ -35093,7 +35132,7 @@
   </sheetPr>
   <dimension ref="A2:BC13"/>
   <sheetViews>
-    <sheetView topLeftCell="AW2" workbookViewId="0">
+    <sheetView topLeftCell="A22" workbookViewId="0">
       <selection activeCell="BC5" sqref="BC5"/>
     </sheetView>
   </sheetViews>
@@ -38589,10 +38628,10 @@
   <sheetPr enableFormatConditionsCalculation="0">
     <tabColor rgb="FFFF0000"/>
   </sheetPr>
-  <dimension ref="A2:BC18"/>
+  <dimension ref="A2:BC19"/>
   <sheetViews>
-    <sheetView topLeftCell="AQ1" workbookViewId="0">
-      <selection activeCell="BC5" sqref="BC5"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E19" sqref="E19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -39750,6 +39789,20 @@
       </c>
       <c r="D18">
         <v>10.78</v>
+      </c>
+    </row>
+    <row r="19" spans="1:6">
+      <c r="A19" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="B19" s="38">
+        <v>11597</v>
+      </c>
+      <c r="C19">
+        <v>1100</v>
+      </c>
+      <c r="D19">
+        <v>10.56</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
sell zhejiang medicine, buy meidi & minsheng bank
</commit_message>
<xml_diff>
--- a/stock.xlsx
+++ b/stock.xlsx
@@ -1,10 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="22416"/>
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="26405"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="1520" yWindow="20" windowWidth="25600" windowHeight="16060" tabRatio="996" activeTab="12"/>
+    <workbookView xWindow="1520" yWindow="20" windowWidth="25600" windowHeight="16060" tabRatio="996" activeTab="6"/>
   </bookViews>
   <sheets>
     <sheet name="达华智能" sheetId="1" r:id="rId1"/>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="287" uniqueCount="72">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="290" uniqueCount="72">
   <si>
     <t>达华智能</t>
   </si>
@@ -459,8 +459,10 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="133">
+  <cellStyleXfs count="135">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -638,7 +640,7 @@
     <xf numFmtId="17" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
   </cellXfs>
-  <cellStyles count="133">
+  <cellStyles count="135">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
@@ -705,6 +707,7 @@
     <cellStyle name="Followed Hyperlink" xfId="128" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="130" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="132" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="134" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
@@ -771,6 +774,7 @@
     <cellStyle name="Hyperlink" xfId="127" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="129" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="131" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="133" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -984,11 +988,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="-2029534024"/>
-        <c:axId val="-2029531016"/>
+        <c:axId val="1772814552"/>
+        <c:axId val="2044623272"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="-2029534024"/>
+        <c:axId val="1772814552"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -997,7 +1001,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-2029531016"/>
+        <c:crossAx val="2044623272"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -1005,7 +1009,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="-2029531016"/>
+        <c:axId val="2044623272"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1016,14 +1020,13 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-2029534024"/>
+        <c:crossAx val="1772814552"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
     </c:plotArea>
     <c:legend>
       <c:legendPos val="r"/>
-      <c:layout/>
       <c:overlay val="0"/>
     </c:legend>
     <c:plotVisOnly val="1"/>
@@ -1244,11 +1247,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="-2033050568"/>
-        <c:axId val="-2033047560"/>
+        <c:axId val="2043786040"/>
+        <c:axId val="2043789048"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="-2033050568"/>
+        <c:axId val="2043786040"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1257,7 +1260,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-2033047560"/>
+        <c:crossAx val="2043789048"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -1265,7 +1268,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="-2033047560"/>
+        <c:axId val="2043789048"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1276,7 +1279,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-2033050568"/>
+        <c:crossAx val="2043786040"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -1514,11 +1517,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="-2032191560"/>
-        <c:axId val="-2032188552"/>
+        <c:axId val="1773250072"/>
+        <c:axId val="-2101295832"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="-2032191560"/>
+        <c:axId val="1773250072"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1527,7 +1530,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-2032188552"/>
+        <c:crossAx val="-2101295832"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -1535,7 +1538,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="-2032188552"/>
+        <c:axId val="-2101295832"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1546,7 +1549,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-2032191560"/>
+        <c:crossAx val="1773250072"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -1771,11 +1774,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:gapWidth val="150"/>
-        <c:axId val="-2029406232"/>
-        <c:axId val="-2029403224"/>
+        <c:axId val="-2096094424"/>
+        <c:axId val="2039613096"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="-2029406232"/>
+        <c:axId val="-2096094424"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1784,7 +1787,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-2029403224"/>
+        <c:crossAx val="2039613096"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -1792,7 +1795,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="-2029403224"/>
+        <c:axId val="2039613096"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1803,7 +1806,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-2029406232"/>
+        <c:crossAx val="-2096094424"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -1923,11 +1926,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="-2026098808"/>
-        <c:axId val="-2026095864"/>
+        <c:axId val="2038687160"/>
+        <c:axId val="-2104522792"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="-2026098808"/>
+        <c:axId val="2038687160"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1936,7 +1939,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-2026095864"/>
+        <c:crossAx val="-2104522792"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -1944,7 +1947,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="-2026095864"/>
+        <c:axId val="-2104522792"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1955,7 +1958,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-2026098808"/>
+        <c:crossAx val="2038687160"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -2075,11 +2078,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="-2026690776"/>
-        <c:axId val="-2026687832"/>
+        <c:axId val="-2104741704"/>
+        <c:axId val="2129121752"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="-2026690776"/>
+        <c:axId val="-2104741704"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2088,7 +2091,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-2026687832"/>
+        <c:crossAx val="2129121752"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -2096,7 +2099,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="-2026687832"/>
+        <c:axId val="2129121752"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2107,7 +2110,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-2026690776"/>
+        <c:crossAx val="-2104741704"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -2224,11 +2227,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:gapWidth val="150"/>
-        <c:axId val="-2026393032"/>
-        <c:axId val="-2026390088"/>
+        <c:axId val="1784553832"/>
+        <c:axId val="1783934152"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="-2026393032"/>
+        <c:axId val="1784553832"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2237,7 +2240,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-2026390088"/>
+        <c:crossAx val="1783934152"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -2245,7 +2248,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="-2026390088"/>
+        <c:axId val="1783934152"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2256,7 +2259,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-2026393032"/>
+        <c:crossAx val="1784553832"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -2484,11 +2487,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="-2026350824"/>
-        <c:axId val="-2026347880"/>
+        <c:axId val="1774063944"/>
+        <c:axId val="1774066952"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="-2026350824"/>
+        <c:axId val="1774063944"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2497,7 +2500,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-2026347880"/>
+        <c:crossAx val="1774066952"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -2505,7 +2508,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="-2026347880"/>
+        <c:axId val="1774066952"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2516,14 +2519,13 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-2026350824"/>
+        <c:crossAx val="1774063944"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
     </c:plotArea>
     <c:legend>
       <c:legendPos val="r"/>
-      <c:layout/>
       <c:overlay val="0"/>
     </c:legend>
     <c:plotVisOnly val="1"/>
@@ -2754,11 +2756,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="-2026715592"/>
-        <c:axId val="-2026712648"/>
+        <c:axId val="-2105503128"/>
+        <c:axId val="1784318856"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="-2026715592"/>
+        <c:axId val="-2105503128"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2767,7 +2769,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-2026712648"/>
+        <c:crossAx val="1784318856"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -2775,7 +2777,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="-2026712648"/>
+        <c:axId val="1784318856"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:min val="15.0"/>
@@ -2787,14 +2789,13 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-2026715592"/>
+        <c:crossAx val="-2105503128"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
     </c:plotArea>
     <c:legend>
       <c:legendPos val="r"/>
-      <c:layout/>
       <c:overlay val="0"/>
     </c:legend>
     <c:plotVisOnly val="1"/>
@@ -3012,11 +3013,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:gapWidth val="150"/>
-        <c:axId val="-2026648456"/>
-        <c:axId val="-2026645448"/>
+        <c:axId val="-2104682840"/>
+        <c:axId val="1784410344"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="-2026648456"/>
+        <c:axId val="-2104682840"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3025,7 +3026,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-2026645448"/>
+        <c:crossAx val="1784410344"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -3033,7 +3034,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="-2026645448"/>
+        <c:axId val="1784410344"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3044,14 +3045,13 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-2026648456"/>
+        <c:crossAx val="-2104682840"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
     </c:plotArea>
     <c:legend>
       <c:legendPos val="r"/>
-      <c:layout/>
       <c:overlay val="0"/>
     </c:legend>
     <c:plotVisOnly val="1"/>
@@ -3272,11 +3272,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="-2026627592"/>
-        <c:axId val="-2026624584"/>
+        <c:axId val="-2104768040"/>
+        <c:axId val="1784216936"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="-2026627592"/>
+        <c:axId val="-2104768040"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3285,7 +3285,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-2026624584"/>
+        <c:crossAx val="1784216936"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -3293,7 +3293,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="-2026624584"/>
+        <c:axId val="1784216936"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3304,7 +3304,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-2026627592"/>
+        <c:crossAx val="-2104768040"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -3542,11 +3542,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="-2028129064"/>
-        <c:axId val="-2028126056"/>
+        <c:axId val="-2101286808"/>
+        <c:axId val="1774043624"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="-2028129064"/>
+        <c:axId val="-2101286808"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3555,7 +3555,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-2028126056"/>
+        <c:crossAx val="1774043624"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -3563,7 +3563,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="-2028126056"/>
+        <c:axId val="1774043624"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:min val="16.5"/>
@@ -3575,14 +3575,13 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-2028129064"/>
+        <c:crossAx val="-2101286808"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
     </c:plotArea>
     <c:legend>
       <c:legendPos val="r"/>
-      <c:layout/>
       <c:overlay val="0"/>
     </c:legend>
     <c:plotVisOnly val="1"/>
@@ -3813,11 +3812,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="-2026314456"/>
-        <c:axId val="-2026311448"/>
+        <c:axId val="-2105373160"/>
+        <c:axId val="1784387176"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="-2026314456"/>
+        <c:axId val="-2105373160"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3826,7 +3825,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-2026311448"/>
+        <c:crossAx val="1784387176"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -3834,7 +3833,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="-2026311448"/>
+        <c:axId val="1784387176"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3845,7 +3844,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-2026314456"/>
+        <c:crossAx val="-2105373160"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -4070,11 +4069,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:gapWidth val="150"/>
-        <c:axId val="-2026287768"/>
-        <c:axId val="-2026509080"/>
+        <c:axId val="1784331864"/>
+        <c:axId val="1784291304"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="-2026287768"/>
+        <c:axId val="1784331864"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -4083,7 +4082,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-2026509080"/>
+        <c:crossAx val="1784291304"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -4091,7 +4090,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="-2026509080"/>
+        <c:axId val="1784291304"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -4102,7 +4101,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-2026287768"/>
+        <c:crossAx val="1784331864"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -4330,11 +4329,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="-2029732936"/>
-        <c:axId val="2142267848"/>
+        <c:axId val="1773169832"/>
+        <c:axId val="-2101179992"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="-2029732936"/>
+        <c:axId val="1773169832"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -4343,7 +4342,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="2142267848"/>
+        <c:crossAx val="-2101179992"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -4351,7 +4350,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="2142267848"/>
+        <c:axId val="-2101179992"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -4362,14 +4361,13 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-2029732936"/>
+        <c:crossAx val="1773169832"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
     </c:plotArea>
     <c:legend>
       <c:legendPos val="r"/>
-      <c:layout/>
       <c:overlay val="0"/>
     </c:legend>
     <c:plotVisOnly val="1"/>
@@ -4600,11 +4598,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="-2029287992"/>
-        <c:axId val="2142797448"/>
+        <c:axId val="-2101233976"/>
+        <c:axId val="1773780904"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="-2029287992"/>
+        <c:axId val="-2101233976"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -4613,7 +4611,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="2142797448"/>
+        <c:crossAx val="1773780904"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -4621,7 +4619,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="2142797448"/>
+        <c:axId val="1773780904"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -4632,14 +4630,13 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-2029287992"/>
+        <c:crossAx val="-2101233976"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
     </c:plotArea>
     <c:legend>
       <c:legendPos val="r"/>
-      <c:layout/>
       <c:overlay val="0"/>
     </c:legend>
     <c:plotVisOnly val="1"/>
@@ -4857,11 +4854,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:gapWidth val="150"/>
-        <c:axId val="-2028739848"/>
-        <c:axId val="-2028736840"/>
+        <c:axId val="1773883800"/>
+        <c:axId val="1773752904"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="-2028739848"/>
+        <c:axId val="1773883800"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -4870,7 +4867,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-2028736840"/>
+        <c:crossAx val="1773752904"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -4878,7 +4875,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="-2028736840"/>
+        <c:axId val="1773752904"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -4889,14 +4886,13 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-2028739848"/>
+        <c:crossAx val="1773883800"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
     </c:plotArea>
     <c:legend>
       <c:legendPos val="r"/>
-      <c:layout/>
       <c:overlay val="0"/>
     </c:legend>
     <c:plotVisOnly val="1"/>
@@ -5117,11 +5113,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="-2032746936"/>
-        <c:axId val="-2032743928"/>
+        <c:axId val="1773668568"/>
+        <c:axId val="-2101126456"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="-2032746936"/>
+        <c:axId val="1773668568"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -5130,7 +5126,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-2032743928"/>
+        <c:crossAx val="-2101126456"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -5138,7 +5134,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="-2032743928"/>
+        <c:axId val="-2101126456"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -5149,14 +5145,13 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-2032746936"/>
+        <c:crossAx val="1773668568"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
     </c:plotArea>
     <c:legend>
       <c:legendPos val="r"/>
-      <c:layout/>
       <c:overlay val="0"/>
     </c:legend>
     <c:plotVisOnly val="1"/>
@@ -5387,11 +5382,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="-2033120568"/>
-        <c:axId val="-2033117560"/>
+        <c:axId val="1784183832"/>
+        <c:axId val="1784186888"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="-2033120568"/>
+        <c:axId val="1784183832"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -5400,7 +5395,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-2033117560"/>
+        <c:crossAx val="1784186888"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -5408,7 +5403,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="-2033117560"/>
+        <c:axId val="1784186888"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -5419,14 +5414,13 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-2033120568"/>
+        <c:crossAx val="1784183832"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
     </c:plotArea>
     <c:legend>
       <c:legendPos val="r"/>
-      <c:layout/>
       <c:overlay val="0"/>
     </c:legend>
     <c:plotVisOnly val="1"/>
@@ -5644,11 +5638,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:gapWidth val="150"/>
-        <c:axId val="-2033094168"/>
-        <c:axId val="-2033091160"/>
+        <c:axId val="-2095277400"/>
+        <c:axId val="-2096093656"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="-2033094168"/>
+        <c:axId val="-2095277400"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -5657,7 +5651,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-2033091160"/>
+        <c:crossAx val="-2096093656"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -5665,7 +5659,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="-2033091160"/>
+        <c:axId val="-2096093656"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -5676,14 +5670,13 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-2033094168"/>
+        <c:crossAx val="-2095277400"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
     </c:plotArea>
     <c:legend>
       <c:legendPos val="r"/>
-      <c:layout/>
       <c:overlay val="0"/>
     </c:legend>
     <c:plotVisOnly val="1"/>
@@ -5904,11 +5897,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="-2028417192"/>
-        <c:axId val="-2029722104"/>
+        <c:axId val="1773382232"/>
+        <c:axId val="-2101172968"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="-2028417192"/>
+        <c:axId val="1773382232"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -5917,7 +5910,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-2029722104"/>
+        <c:crossAx val="-2101172968"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -5925,7 +5918,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="-2029722104"/>
+        <c:axId val="-2101172968"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -5936,14 +5929,13 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-2028417192"/>
+        <c:crossAx val="1773382232"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
     </c:plotArea>
     <c:legend>
       <c:legendPos val="r"/>
-      <c:layout/>
       <c:overlay val="0"/>
     </c:legend>
     <c:plotVisOnly val="1"/>
@@ -6174,11 +6166,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="-2032456904"/>
-        <c:axId val="-2032453896"/>
+        <c:axId val="1773403928"/>
+        <c:axId val="-2101095368"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="-2032456904"/>
+        <c:axId val="1773403928"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -6187,7 +6179,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-2032453896"/>
+        <c:crossAx val="-2101095368"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -6195,7 +6187,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="-2032453896"/>
+        <c:axId val="-2101095368"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -6206,14 +6198,13 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-2032456904"/>
+        <c:crossAx val="1773403928"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
     </c:plotArea>
     <c:legend>
       <c:legendPos val="r"/>
-      <c:layout/>
       <c:overlay val="0"/>
     </c:legend>
     <c:plotVisOnly val="1"/>
@@ -6431,11 +6422,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:gapWidth val="150"/>
-        <c:axId val="-2029767400"/>
-        <c:axId val="-2029764392"/>
+        <c:axId val="1774125816"/>
+        <c:axId val="1774128760"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="-2029767400"/>
+        <c:axId val="1774125816"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -6444,7 +6435,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-2029764392"/>
+        <c:crossAx val="1774128760"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -6452,7 +6443,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="-2029764392"/>
+        <c:axId val="1774128760"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -6463,14 +6454,13 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-2029767400"/>
+        <c:crossAx val="1774125816"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
     </c:plotArea>
     <c:legend>
       <c:legendPos val="r"/>
-      <c:layout/>
       <c:overlay val="0"/>
     </c:legend>
     <c:plotVisOnly val="1"/>
@@ -6688,11 +6678,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:gapWidth val="150"/>
-        <c:axId val="-2028333000"/>
-        <c:axId val="-2028329992"/>
+        <c:axId val="-2101163288"/>
+        <c:axId val="-2101160536"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="-2028333000"/>
+        <c:axId val="-2101163288"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -6701,7 +6691,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-2028329992"/>
+        <c:crossAx val="-2101160536"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -6709,7 +6699,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="-2028329992"/>
+        <c:axId val="-2101160536"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -6720,14 +6710,13 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-2028333000"/>
+        <c:crossAx val="-2101163288"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
     </c:plotArea>
     <c:legend>
       <c:legendPos val="r"/>
-      <c:layout/>
       <c:overlay val="0"/>
     </c:legend>
     <c:plotVisOnly val="1"/>
@@ -6948,11 +6937,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="-2032416472"/>
-        <c:axId val="-2032413496"/>
+        <c:axId val="1773329656"/>
+        <c:axId val="1773332664"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="-2032416472"/>
+        <c:axId val="1773329656"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -6961,7 +6950,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-2032413496"/>
+        <c:crossAx val="1773332664"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -6969,7 +6958,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="-2032413496"/>
+        <c:axId val="1773332664"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -6980,14 +6969,13 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-2032416472"/>
+        <c:crossAx val="1773329656"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
     </c:plotArea>
     <c:legend>
       <c:legendPos val="r"/>
-      <c:layout/>
       <c:overlay val="0"/>
     </c:legend>
     <c:plotVisOnly val="1"/>
@@ -7218,11 +7206,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="-2028270568"/>
-        <c:axId val="-2028267560"/>
+        <c:axId val="1773224136"/>
+        <c:axId val="1774146888"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="-2028270568"/>
+        <c:axId val="1773224136"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -7231,7 +7219,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-2028267560"/>
+        <c:crossAx val="1774146888"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -7239,7 +7227,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="-2028267560"/>
+        <c:axId val="1774146888"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -7250,14 +7238,13 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-2028270568"/>
+        <c:crossAx val="1773224136"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
     </c:plotArea>
     <c:legend>
       <c:legendPos val="r"/>
-      <c:layout/>
       <c:overlay val="0"/>
     </c:legend>
     <c:plotVisOnly val="1"/>
@@ -7475,11 +7462,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:gapWidth val="150"/>
-        <c:axId val="-2028458344"/>
-        <c:axId val="-2028455336"/>
+        <c:axId val="1773251400"/>
+        <c:axId val="1773504584"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="-2028458344"/>
+        <c:axId val="1773251400"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -7488,7 +7475,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-2028455336"/>
+        <c:crossAx val="1773504584"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -7496,7 +7483,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="-2028455336"/>
+        <c:axId val="1773504584"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -7507,14 +7494,13 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-2028458344"/>
+        <c:crossAx val="1773251400"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
     </c:plotArea>
     <c:legend>
       <c:legendPos val="r"/>
-      <c:layout/>
       <c:overlay val="0"/>
     </c:legend>
     <c:plotVisOnly val="1"/>
@@ -7735,11 +7721,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="-2028785448"/>
-        <c:axId val="-2028782440"/>
+        <c:axId val="1773738296"/>
+        <c:axId val="1773628328"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="-2028785448"/>
+        <c:axId val="1773738296"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -7748,7 +7734,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-2028782440"/>
+        <c:crossAx val="1773628328"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -7756,7 +7742,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="-2028782440"/>
+        <c:axId val="1773628328"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -7767,14 +7753,13 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-2028785448"/>
+        <c:crossAx val="1773738296"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
     </c:plotArea>
     <c:legend>
       <c:legendPos val="r"/>
-      <c:layout/>
       <c:overlay val="0"/>
     </c:legend>
     <c:plotVisOnly val="1"/>
@@ -8005,11 +7990,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="-2028305720"/>
-        <c:axId val="-2028302712"/>
+        <c:axId val="1772156504"/>
+        <c:axId val="1772144168"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="-2028305720"/>
+        <c:axId val="1772156504"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -8018,7 +8003,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-2028302712"/>
+        <c:crossAx val="1772144168"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -8026,7 +8011,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="-2028302712"/>
+        <c:axId val="1772144168"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:min val="3.0"/>
@@ -8038,14 +8023,13 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-2028305720"/>
+        <c:crossAx val="1772156504"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
     </c:plotArea>
     <c:legend>
       <c:legendPos val="r"/>
-      <c:layout/>
       <c:overlay val="0"/>
     </c:legend>
     <c:plotVisOnly val="1"/>
@@ -8263,11 +8247,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:gapWidth val="150"/>
-        <c:axId val="-2029600072"/>
-        <c:axId val="-2029597064"/>
+        <c:axId val="1772249144"/>
+        <c:axId val="1772252152"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="-2029600072"/>
+        <c:axId val="1772249144"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -8276,7 +8260,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-2029597064"/>
+        <c:crossAx val="1772252152"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -8284,7 +8268,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="-2029597064"/>
+        <c:axId val="1772252152"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -8295,14 +8279,13 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-2029600072"/>
+        <c:crossAx val="1772249144"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
     </c:plotArea>
     <c:legend>
       <c:legendPos val="r"/>
-      <c:layout/>
       <c:overlay val="0"/>
     </c:legend>
     <c:plotVisOnly val="1"/>
@@ -8523,11 +8506,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="-2032826472"/>
-        <c:axId val="-2032823464"/>
+        <c:axId val="1774001448"/>
+        <c:axId val="1774004456"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="-2032826472"/>
+        <c:axId val="1774001448"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -8536,7 +8519,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-2032823464"/>
+        <c:crossAx val="1774004456"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -8544,7 +8527,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="-2032823464"/>
+        <c:axId val="1774004456"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -8555,7 +8538,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-2032826472"/>
+        <c:crossAx val="1774001448"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -8793,11 +8776,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="-2027965256"/>
-        <c:axId val="-2029484040"/>
+        <c:axId val="-2100677496"/>
+        <c:axId val="1773904936"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="-2027965256"/>
+        <c:axId val="-2100677496"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -8806,7 +8789,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-2029484040"/>
+        <c:crossAx val="1773904936"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -8814,7 +8797,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="-2029484040"/>
+        <c:axId val="1773904936"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -8825,7 +8808,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-2027965256"/>
+        <c:crossAx val="-2100677496"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -9050,11 +9033,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:gapWidth val="150"/>
-        <c:axId val="-2028569016"/>
-        <c:axId val="-2121241176"/>
+        <c:axId val="-2038845832"/>
+        <c:axId val="-2038780328"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="-2028569016"/>
+        <c:axId val="-2038845832"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -9063,7 +9046,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-2121241176"/>
+        <c:crossAx val="-2038780328"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -9071,7 +9054,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="-2121241176"/>
+        <c:axId val="-2038780328"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -9082,7 +9065,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-2028569016"/>
+        <c:crossAx val="-2038845832"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -9310,11 +9293,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="-2032900088"/>
-        <c:axId val="-2032897080"/>
+        <c:axId val="2039280040"/>
+        <c:axId val="2029204744"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="-2032900088"/>
+        <c:axId val="2039280040"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -9323,7 +9306,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-2032897080"/>
+        <c:crossAx val="2029204744"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -9331,7 +9314,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="-2032897080"/>
+        <c:axId val="2029204744"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -9342,14 +9325,13 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-2032900088"/>
+        <c:crossAx val="2039280040"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
     </c:plotArea>
     <c:legend>
       <c:legendPos val="r"/>
-      <c:layout/>
       <c:overlay val="0"/>
     </c:legend>
     <c:plotVisOnly val="1"/>
@@ -9570,11 +9552,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="-2028165160"/>
-        <c:axId val="-2028162152"/>
+        <c:axId val="-2101132600"/>
+        <c:axId val="-2038452152"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="-2028165160"/>
+        <c:axId val="-2101132600"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -9583,7 +9565,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-2028162152"/>
+        <c:crossAx val="-2038452152"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -9591,7 +9573,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="-2028162152"/>
+        <c:axId val="-2038452152"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -9602,14 +9584,13 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-2028165160"/>
+        <c:crossAx val="-2101132600"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
     </c:plotArea>
     <c:legend>
       <c:legendPos val="r"/>
-      <c:layout/>
       <c:overlay val="0"/>
     </c:legend>
     <c:plotVisOnly val="1"/>
@@ -9840,11 +9821,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="-2029807784"/>
-        <c:axId val="-2029804776"/>
+        <c:axId val="-2038489256"/>
+        <c:axId val="-2038498792"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="-2029807784"/>
+        <c:axId val="-2038489256"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -9853,7 +9834,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-2029804776"/>
+        <c:crossAx val="-2038498792"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -9861,7 +9842,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="-2029804776"/>
+        <c:axId val="-2038498792"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -9872,14 +9853,13 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-2029807784"/>
+        <c:crossAx val="-2038489256"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
     </c:plotArea>
     <c:legend>
       <c:legendPos val="r"/>
-      <c:layout/>
       <c:overlay val="0"/>
     </c:legend>
     <c:plotVisOnly val="1"/>
@@ -10097,11 +10077,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:gapWidth val="150"/>
-        <c:axId val="2142309416"/>
-        <c:axId val="2142444376"/>
+        <c:axId val="-2038510152"/>
+        <c:axId val="-2038521992"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="2142309416"/>
+        <c:axId val="-2038510152"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -10110,7 +10090,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="2142444376"/>
+        <c:crossAx val="-2038521992"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -10118,7 +10098,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="2142444376"/>
+        <c:axId val="-2038521992"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -10129,14 +10109,13 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="2142309416"/>
+        <c:crossAx val="-2038510152"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
     </c:plotArea>
     <c:legend>
       <c:legendPos val="r"/>
-      <c:layout/>
       <c:overlay val="0"/>
     </c:legend>
     <c:plotVisOnly val="1"/>
@@ -10357,11 +10336,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="-2028902152"/>
-        <c:axId val="-2028262904"/>
+        <c:axId val="-2038564488"/>
+        <c:axId val="-2038570680"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="-2028902152"/>
+        <c:axId val="-2038564488"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -10370,7 +10349,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-2028262904"/>
+        <c:crossAx val="-2038570680"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -10378,7 +10357,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="-2028262904"/>
+        <c:axId val="-2038570680"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -10389,14 +10368,13 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-2028902152"/>
+        <c:crossAx val="-2038564488"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
     </c:plotArea>
     <c:legend>
       <c:legendPos val="r"/>
-      <c:layout/>
       <c:overlay val="0"/>
     </c:legend>
     <c:plotVisOnly val="1"/>
@@ -10627,11 +10605,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="-2028884552"/>
-        <c:axId val="-2028881544"/>
+        <c:axId val="-2038614824"/>
+        <c:axId val="-2038623656"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="-2028884552"/>
+        <c:axId val="-2038614824"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -10640,7 +10618,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-2028881544"/>
+        <c:crossAx val="-2038623656"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -10648,7 +10626,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="-2028881544"/>
+        <c:axId val="-2038623656"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:min val="8.0"/>
@@ -10660,14 +10638,13 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-2028884552"/>
+        <c:crossAx val="-2038614824"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
     </c:plotArea>
     <c:legend>
       <c:legendPos val="r"/>
-      <c:layout/>
       <c:overlay val="0"/>
     </c:legend>
     <c:plotVisOnly val="1"/>
@@ -10885,11 +10862,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:gapWidth val="150"/>
-        <c:axId val="-2028157736"/>
-        <c:axId val="-2028154760"/>
+        <c:axId val="-2038661304"/>
+        <c:axId val="-2038658424"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="-2028157736"/>
+        <c:axId val="-2038661304"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -10898,7 +10875,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-2028154760"/>
+        <c:crossAx val="-2038658424"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -10906,7 +10883,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="-2028154760"/>
+        <c:axId val="-2038658424"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -10917,14 +10894,13 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-2028157736"/>
+        <c:crossAx val="-2038661304"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
     </c:plotArea>
     <c:legend>
       <c:legendPos val="r"/>
-      <c:layout/>
       <c:overlay val="0"/>
     </c:legend>
     <c:plotVisOnly val="1"/>
@@ -11145,11 +11121,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="-2028517944"/>
-        <c:axId val="-2029446376"/>
+        <c:axId val="-2038705976"/>
+        <c:axId val="-2038720584"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="-2028517944"/>
+        <c:axId val="-2038705976"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -11158,7 +11134,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-2029446376"/>
+        <c:crossAx val="-2038720584"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -11166,7 +11142,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="-2029446376"/>
+        <c:axId val="-2038720584"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -11177,14 +11153,13 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-2028517944"/>
+        <c:crossAx val="-2038705976"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
     </c:plotArea>
     <c:legend>
       <c:legendPos val="r"/>
-      <c:layout/>
       <c:overlay val="0"/>
     </c:legend>
     <c:plotVisOnly val="1"/>
@@ -11405,11 +11380,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="-2033028104"/>
-        <c:axId val="-2033025096"/>
+        <c:axId val="-2038763384"/>
+        <c:axId val="-2038771736"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="-2033028104"/>
+        <c:axId val="-2038763384"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -11418,7 +11393,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-2033025096"/>
+        <c:crossAx val="-2038771736"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -11426,7 +11401,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="-2033025096"/>
+        <c:axId val="-2038771736"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -11437,14 +11412,13 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-2033028104"/>
+        <c:crossAx val="-2038763384"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
     </c:plotArea>
     <c:legend>
       <c:legendPos val="r"/>
-      <c:layout/>
       <c:overlay val="0"/>
     </c:legend>
     <c:plotVisOnly val="1"/>
@@ -11662,11 +11636,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:gapWidth val="150"/>
-        <c:axId val="-2033001800"/>
-        <c:axId val="-2032998792"/>
+        <c:axId val="-2038811000"/>
+        <c:axId val="-2038808168"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="-2033001800"/>
+        <c:axId val="-2038811000"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -11675,7 +11649,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-2032998792"/>
+        <c:crossAx val="-2038808168"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -11683,7 +11657,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="-2032998792"/>
+        <c:axId val="-2038808168"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -11694,14 +11668,13 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-2033001800"/>
+        <c:crossAx val="-2038811000"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
     </c:plotArea>
     <c:legend>
       <c:legendPos val="r"/>
-      <c:layout/>
       <c:overlay val="0"/>
     </c:legend>
     <c:plotVisOnly val="1"/>
@@ -11922,11 +11895,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="-2029276888"/>
-        <c:axId val="-2028361720"/>
+        <c:axId val="-2038859608"/>
+        <c:axId val="-2038856600"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="-2029276888"/>
+        <c:axId val="-2038859608"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -11935,7 +11908,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-2028361720"/>
+        <c:crossAx val="-2038856600"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -11943,7 +11916,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="-2028361720"/>
+        <c:axId val="-2038856600"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -11954,14 +11927,13 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-2029276888"/>
+        <c:crossAx val="-2038859608"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
     </c:plotArea>
     <c:legend>
       <c:legendPos val="r"/>
-      <c:layout/>
       <c:overlay val="0"/>
     </c:legend>
     <c:plotVisOnly val="1"/>
@@ -12192,11 +12164,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="-2032865640"/>
-        <c:axId val="-2032862632"/>
+        <c:axId val="1773022248"/>
+        <c:axId val="1772862712"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="-2032865640"/>
+        <c:axId val="1773022248"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -12205,7 +12177,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-2032862632"/>
+        <c:crossAx val="1772862712"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -12213,7 +12185,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="-2032862632"/>
+        <c:axId val="1772862712"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:min val="4.3"/>
@@ -12225,14 +12197,13 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-2032865640"/>
+        <c:crossAx val="1773022248"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
     </c:plotArea>
     <c:legend>
       <c:legendPos val="r"/>
-      <c:layout/>
       <c:overlay val="0"/>
     </c:legend>
     <c:plotVisOnly val="1"/>
@@ -12463,11 +12434,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="-2028609240"/>
-        <c:axId val="-2028606232"/>
+        <c:axId val="-2038911080"/>
+        <c:axId val="-2038908072"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="-2028609240"/>
+        <c:axId val="-2038911080"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -12476,7 +12447,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-2028606232"/>
+        <c:crossAx val="-2038908072"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -12484,7 +12455,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="-2028606232"/>
+        <c:axId val="-2038908072"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -12495,14 +12466,13 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-2028609240"/>
+        <c:crossAx val="-2038911080"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
     </c:plotArea>
     <c:legend>
       <c:legendPos val="r"/>
-      <c:layout/>
       <c:overlay val="0"/>
     </c:legend>
     <c:plotVisOnly val="1"/>
@@ -12720,11 +12690,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:gapWidth val="150"/>
-        <c:axId val="-2029838808"/>
-        <c:axId val="-2029835800"/>
+        <c:axId val="-2038917880"/>
+        <c:axId val="-2038944328"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="-2029838808"/>
+        <c:axId val="-2038917880"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -12733,7 +12703,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-2029835800"/>
+        <c:crossAx val="-2038944328"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -12741,7 +12711,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="-2029835800"/>
+        <c:axId val="-2038944328"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -12752,14 +12722,13 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-2029838808"/>
+        <c:crossAx val="-2038917880"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
     </c:plotArea>
     <c:legend>
       <c:legendPos val="r"/>
-      <c:layout/>
       <c:overlay val="0"/>
     </c:legend>
     <c:plotVisOnly val="1"/>
@@ -12941,11 +12910,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="-2029875592"/>
-        <c:axId val="-2029872584"/>
+        <c:axId val="-2038969944"/>
+        <c:axId val="-2038978200"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="-2029875592"/>
+        <c:axId val="-2038969944"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -12954,7 +12923,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-2029872584"/>
+        <c:crossAx val="-2038978200"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -12962,7 +12931,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="-2029872584"/>
+        <c:axId val="-2038978200"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -12973,14 +12942,13 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-2029875592"/>
+        <c:crossAx val="-2038969944"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
     </c:plotArea>
     <c:legend>
       <c:legendPos val="r"/>
-      <c:layout/>
       <c:overlay val="0"/>
     </c:legend>
     <c:plotVisOnly val="1"/>
@@ -13172,11 +13140,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="2142921256"/>
-        <c:axId val="-2121189128"/>
+        <c:axId val="-2039017272"/>
+        <c:axId val="-2039014264"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="2142921256"/>
+        <c:axId val="-2039017272"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -13185,7 +13153,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-2121189128"/>
+        <c:crossAx val="-2039014264"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -13193,7 +13161,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="-2121189128"/>
+        <c:axId val="-2039014264"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -13204,14 +13172,13 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="2142921256"/>
+        <c:crossAx val="-2039017272"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
     </c:plotArea>
     <c:legend>
       <c:legendPos val="r"/>
-      <c:layout/>
       <c:overlay val="0"/>
     </c:legend>
     <c:plotVisOnly val="1"/>
@@ -13390,11 +13357,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:gapWidth val="150"/>
-        <c:axId val="-2028003096"/>
-        <c:axId val="-2028000088"/>
+        <c:axId val="-2039066440"/>
+        <c:axId val="-2039071560"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="-2028003096"/>
+        <c:axId val="-2039066440"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -13403,7 +13370,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-2028000088"/>
+        <c:crossAx val="-2039071560"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -13411,7 +13378,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="-2028000088"/>
+        <c:axId val="-2039071560"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -13422,14 +13389,13 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-2028003096"/>
+        <c:crossAx val="-2039066440"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
     </c:plotArea>
     <c:legend>
       <c:legendPos val="r"/>
-      <c:layout/>
       <c:overlay val="0"/>
     </c:legend>
     <c:plotVisOnly val="1"/>
@@ -13608,11 +13574,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="-2029455096"/>
-        <c:axId val="-2028294296"/>
+        <c:axId val="-2039118296"/>
+        <c:axId val="-2039115320"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="-2029455096"/>
+        <c:axId val="-2039118296"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -13621,7 +13587,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-2028294296"/>
+        <c:crossAx val="-2039115320"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -13629,7 +13595,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="-2028294296"/>
+        <c:axId val="-2039115320"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -13640,14 +13606,13 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-2029455096"/>
+        <c:crossAx val="-2039118296"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
     </c:plotArea>
     <c:legend>
       <c:legendPos val="r"/>
-      <c:layout/>
       <c:overlay val="0"/>
     </c:legend>
     <c:plotVisOnly val="1"/>
@@ -13836,11 +13801,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="-2028061224"/>
-        <c:axId val="-2028058248"/>
+        <c:axId val="-2039152488"/>
+        <c:axId val="-2039155352"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="-2028061224"/>
+        <c:axId val="-2039152488"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -13849,7 +13814,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-2028058248"/>
+        <c:crossAx val="-2039155352"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -13857,7 +13822,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="-2028058248"/>
+        <c:axId val="-2039155352"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:min val="350.0"/>
@@ -13869,14 +13834,13 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-2028061224"/>
+        <c:crossAx val="-2039152488"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
     </c:plotArea>
     <c:legend>
       <c:legendPos val="r"/>
-      <c:layout/>
       <c:overlay val="0"/>
     </c:legend>
     <c:plotVisOnly val="1"/>
@@ -14052,11 +14016,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:gapWidth val="150"/>
-        <c:axId val="-2028035000"/>
-        <c:axId val="2142158472"/>
+        <c:axId val="-2039179784"/>
+        <c:axId val="-2039183368"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="-2028035000"/>
+        <c:axId val="-2039179784"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -14065,7 +14029,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="2142158472"/>
+        <c:crossAx val="-2039183368"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -14073,7 +14037,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="2142158472"/>
+        <c:axId val="-2039183368"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -14084,14 +14048,13 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-2028035000"/>
+        <c:crossAx val="-2039179784"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
     </c:plotArea>
     <c:legend>
       <c:legendPos val="r"/>
-      <c:layout/>
       <c:overlay val="0"/>
     </c:legend>
     <c:plotVisOnly val="1"/>
@@ -14255,11 +14218,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="-2029243432"/>
-        <c:axId val="-2029240424"/>
+        <c:axId val="-2039225656"/>
+        <c:axId val="-2039229016"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="-2029243432"/>
+        <c:axId val="-2039225656"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -14268,7 +14231,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-2029240424"/>
+        <c:crossAx val="-2039229016"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -14276,7 +14239,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="-2029240424"/>
+        <c:axId val="-2039229016"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -14287,14 +14250,13 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-2029243432"/>
+        <c:crossAx val="-2039225656"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
     </c:plotArea>
     <c:legend>
       <c:legendPos val="r"/>
-      <c:layout/>
       <c:overlay val="0"/>
     </c:legend>
     <c:plotVisOnly val="1"/>
@@ -14468,11 +14430,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="-2029744264"/>
-        <c:axId val="-2029741256"/>
+        <c:axId val="-2039263400"/>
+        <c:axId val="-2039275208"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="-2029744264"/>
+        <c:axId val="-2039263400"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -14481,7 +14443,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-2029741256"/>
+        <c:crossAx val="-2039275208"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -14489,7 +14451,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="-2029741256"/>
+        <c:axId val="-2039275208"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:min val="15.0"/>
@@ -14501,14 +14463,13 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-2029744264"/>
+        <c:crossAx val="-2039263400"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
     </c:plotArea>
     <c:legend>
       <c:legendPos val="r"/>
-      <c:layout/>
       <c:overlay val="0"/>
     </c:legend>
     <c:plotVisOnly val="1"/>
@@ -14726,11 +14687,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:gapWidth val="150"/>
-        <c:axId val="-2032626760"/>
-        <c:axId val="-2032623752"/>
+        <c:axId val="2043747800"/>
+        <c:axId val="2043750808"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="-2032626760"/>
+        <c:axId val="2043747800"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -14739,7 +14700,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-2032623752"/>
+        <c:crossAx val="2043750808"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -14747,7 +14708,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="-2032623752"/>
+        <c:axId val="2043750808"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -14758,14 +14719,13 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-2032626760"/>
+        <c:crossAx val="2043747800"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
     </c:plotArea>
     <c:legend>
       <c:legendPos val="r"/>
-      <c:layout/>
       <c:overlay val="0"/>
     </c:legend>
     <c:plotVisOnly val="1"/>
@@ -14926,11 +14886,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:gapWidth val="150"/>
-        <c:axId val="-2029695080"/>
-        <c:axId val="-2029692072"/>
+        <c:axId val="-2039290920"/>
+        <c:axId val="-2039315352"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="-2029695080"/>
+        <c:axId val="-2039290920"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -14939,7 +14899,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-2029692072"/>
+        <c:crossAx val="-2039315352"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -14947,7 +14907,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="-2029692072"/>
+        <c:axId val="-2039315352"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -14958,14 +14918,13 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-2029695080"/>
+        <c:crossAx val="-2039290920"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
     </c:plotArea>
     <c:legend>
       <c:legendPos val="r"/>
-      <c:layout/>
       <c:overlay val="0"/>
     </c:legend>
     <c:plotVisOnly val="1"/>
@@ -15186,11 +15145,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="2142969272"/>
-        <c:axId val="-2028625688"/>
+        <c:axId val="2042877064"/>
+        <c:axId val="2042880072"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="2142969272"/>
+        <c:axId val="2042877064"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -15199,7 +15158,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-2028625688"/>
+        <c:crossAx val="2042880072"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -15207,7 +15166,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="-2028625688"/>
+        <c:axId val="2042880072"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -15218,14 +15177,13 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="2142969272"/>
+        <c:crossAx val="2042877064"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
     </c:plotArea>
     <c:legend>
       <c:legendPos val="r"/>
-      <c:layout/>
       <c:overlay val="0"/>
     </c:legend>
     <c:plotVisOnly val="1"/>
@@ -15456,11 +15414,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="-2032806360"/>
-        <c:axId val="-2032803352"/>
+        <c:axId val="-2095231400"/>
+        <c:axId val="-2095630648"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="-2032806360"/>
+        <c:axId val="-2095231400"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -15469,7 +15427,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-2032803352"/>
+        <c:crossAx val="-2095630648"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -15477,7 +15435,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="-2032803352"/>
+        <c:axId val="-2095630648"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:min val="6.5"/>
@@ -15489,14 +15447,13 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-2032806360"/>
+        <c:crossAx val="-2095231400"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
     </c:plotArea>
     <c:legend>
       <c:legendPos val="r"/>
-      <c:layout/>
       <c:overlay val="0"/>
     </c:legend>
     <c:plotVisOnly val="1"/>
@@ -15714,11 +15671,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:gapWidth val="150"/>
-        <c:axId val="-2032168408"/>
-        <c:axId val="-2032165400"/>
+        <c:axId val="-2101177288"/>
+        <c:axId val="1774091176"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="-2032168408"/>
+        <c:axId val="-2101177288"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -15727,7 +15684,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-2032165400"/>
+        <c:crossAx val="1774091176"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -15735,7 +15692,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="-2032165400"/>
+        <c:axId val="1774091176"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -15746,14 +15703,13 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-2032168408"/>
+        <c:crossAx val="-2101177288"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
     </c:plotArea>
     <c:legend>
       <c:legendPos val="r"/>
-      <c:layout/>
       <c:overlay val="0"/>
     </c:legend>
     <c:plotVisOnly val="1"/>
@@ -22872,7 +22828,7 @@
   </sheetPr>
   <dimension ref="A2:BD15"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A6" workbookViewId="0">
+    <sheetView topLeftCell="A6" workbookViewId="0">
       <selection activeCell="BD7" sqref="BD7"/>
     </sheetView>
   </sheetViews>
@@ -34121,10 +34077,10 @@
   <sheetPr enableFormatConditionsCalculation="0">
     <tabColor theme="5" tint="0.39997558519241921"/>
   </sheetPr>
-  <dimension ref="A2:BD19"/>
+  <dimension ref="A2:BD20"/>
   <sheetViews>
-    <sheetView topLeftCell="A12" workbookViewId="0">
-      <selection activeCell="BD7" sqref="BD7"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B20" sqref="B20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -35294,8 +35250,8 @@
       <c r="A18" s="1" t="s">
         <v>30</v>
       </c>
-      <c r="B18" s="38">
-        <v>11232</v>
+      <c r="B18" s="16">
+        <v>43038</v>
       </c>
       <c r="C18">
         <v>1100</v>
@@ -35308,14 +35264,28 @@
       <c r="A19" s="1" t="s">
         <v>30</v>
       </c>
-      <c r="B19" s="38">
-        <v>11597</v>
+      <c r="B19" s="16">
+        <v>43039</v>
       </c>
       <c r="C19">
         <v>1100</v>
       </c>
       <c r="D19">
         <v>10.56</v>
+      </c>
+    </row>
+    <row r="20" spans="1:6">
+      <c r="A20" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="B20" s="16">
+        <v>43040</v>
+      </c>
+      <c r="C20">
+        <v>2200</v>
+      </c>
+      <c r="D20">
+        <v>10.69</v>
       </c>
     </row>
   </sheetData>
@@ -35334,8 +35304,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AE45"/>
   <sheetViews>
-    <sheetView topLeftCell="B14" workbookViewId="0">
-      <selection activeCell="T7" sqref="T7"/>
+    <sheetView topLeftCell="A2" workbookViewId="0">
+      <selection activeCell="B14" sqref="B14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -36079,10 +36049,18 @@
       <c r="AE13" s="10"/>
     </row>
     <row r="14" spans="1:31">
-      <c r="A14" s="10"/>
-      <c r="B14" s="10"/>
-      <c r="C14" s="10"/>
-      <c r="D14" s="10"/>
+      <c r="A14" s="17" t="s">
+        <v>30</v>
+      </c>
+      <c r="B14" s="16">
+        <v>43040</v>
+      </c>
+      <c r="C14" s="10">
+        <v>200</v>
+      </c>
+      <c r="D14" s="10">
+        <v>50.68</v>
+      </c>
       <c r="E14" s="10"/>
       <c r="F14" s="10"/>
       <c r="G14" s="10"/>
@@ -38023,10 +38001,10 @@
   <sheetPr enableFormatConditionsCalculation="0">
     <tabColor theme="5" tint="0.39997558519241921"/>
   </sheetPr>
-  <dimension ref="A2:BD13"/>
+  <dimension ref="A2:BD14"/>
   <sheetViews>
-    <sheetView topLeftCell="D17" workbookViewId="0">
-      <selection activeCell="BD7" sqref="BD7"/>
+    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
+      <selection activeCell="E14" sqref="E14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -39189,6 +39167,20 @@
       </c>
       <c r="F13" s="18" t="s">
         <v>39</v>
+      </c>
+    </row>
+    <row r="14" spans="1:56">
+      <c r="A14" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="B14" s="16">
+        <v>43040</v>
+      </c>
+      <c r="C14">
+        <v>1700</v>
+      </c>
+      <c r="D14">
+        <v>8.23</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
add just chart y scope
</commit_message>
<xml_diff>
--- a/stock.xlsx
+++ b/stock.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="22416"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="1520" yWindow="20" windowWidth="25600" windowHeight="16060" tabRatio="996" activeTab="19"/>
+    <workbookView xWindow="1520" yWindow="20" windowWidth="25600" windowHeight="16060" tabRatio="996" activeTab="16"/>
   </bookViews>
   <sheets>
     <sheet name="民生银行" sheetId="13" r:id="rId1"/>
@@ -1667,10 +1667,10 @@
           <c:invertIfNegative val="0"/>
           <c:val>
             <c:numRef>
-              <c:f>沪电股份!$D$6:$BI$6</c:f>
+              <c:f>沪电股份!$D$6:$CD$6</c:f>
               <c:numCache>
                 <c:formatCode>[Red]0.00;[Green]\-0.00</c:formatCode>
-                <c:ptCount val="58"/>
+                <c:ptCount val="79"/>
                 <c:pt idx="0">
                   <c:v>-296.07</c:v>
                 </c:pt>
@@ -1844,6 +1844,12 @@
                 </c:pt>
                 <c:pt idx="57">
                   <c:v>36.28</c:v>
+                </c:pt>
+                <c:pt idx="58">
+                  <c:v>93.67</c:v>
+                </c:pt>
+                <c:pt idx="59">
+                  <c:v>2912.39</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -2512,10 +2518,10 @@
           <c:invertIfNegative val="0"/>
           <c:val>
             <c:numRef>
-              <c:f>宝钢股份!$D$6:$BI$6</c:f>
+              <c:f>宝钢股份!$D$6:$CD$6</c:f>
               <c:numCache>
                 <c:formatCode>[Red]0.00;[Green]\-0.00</c:formatCode>
-                <c:ptCount val="58"/>
+                <c:ptCount val="79"/>
                 <c:pt idx="0">
                   <c:v>-6879.03</c:v>
                 </c:pt>
@@ -2689,6 +2695,12 @@
                 </c:pt>
                 <c:pt idx="57">
                   <c:v>2415.61</c:v>
+                </c:pt>
+                <c:pt idx="58">
+                  <c:v>-356.88</c:v>
+                </c:pt>
+                <c:pt idx="59">
+                  <c:v>2411.7</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -3356,10 +3368,10 @@
           <c:invertIfNegative val="0"/>
           <c:val>
             <c:numRef>
-              <c:f>浙江医药!$D$6:$BI$6</c:f>
+              <c:f>浙江医药!$D$6:$CD$6</c:f>
               <c:numCache>
                 <c:formatCode>[Red]0.00;[Green]\-0.00</c:formatCode>
-                <c:ptCount val="58"/>
+                <c:ptCount val="79"/>
                 <c:pt idx="0">
                   <c:v>1074.42</c:v>
                 </c:pt>
@@ -3533,6 +3545,12 @@
                 </c:pt>
                 <c:pt idx="57">
                   <c:v>448.69</c:v>
+                </c:pt>
+                <c:pt idx="58">
+                  <c:v>2329.02</c:v>
+                </c:pt>
+                <c:pt idx="59">
+                  <c:v>4028.36</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -4492,10 +4510,10 @@
           <c:invertIfNegative val="0"/>
           <c:val>
             <c:numRef>
-              <c:f>远大控股!$D$6:$BI$6</c:f>
+              <c:f>远大控股!$D$6:$CD$6</c:f>
               <c:numCache>
                 <c:formatCode>[Red]0.00;[Green]\-0.00</c:formatCode>
-                <c:ptCount val="58"/>
+                <c:ptCount val="79"/>
                 <c:pt idx="0">
                   <c:v>47.13</c:v>
                 </c:pt>
@@ -4669,6 +4687,12 @@
                 </c:pt>
                 <c:pt idx="57">
                   <c:v>-615.13</c:v>
+                </c:pt>
+                <c:pt idx="58">
+                  <c:v>-613.4400000000001</c:v>
+                </c:pt>
+                <c:pt idx="59">
+                  <c:v>-367.65</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -5336,10 +5360,10 @@
           <c:invertIfNegative val="0"/>
           <c:val>
             <c:numRef>
-              <c:f>包钢股份!$D$6:$BI$6</c:f>
+              <c:f>包钢股份!$D$6:$CD$6</c:f>
               <c:numCache>
                 <c:formatCode>[Red]0.00;[Green]\-0.00</c:formatCode>
-                <c:ptCount val="58"/>
+                <c:ptCount val="79"/>
                 <c:pt idx="0">
                   <c:v>-21881.24</c:v>
                 </c:pt>
@@ -5513,6 +5537,12 @@
                 </c:pt>
                 <c:pt idx="57">
                   <c:v>7789.73</c:v>
+                </c:pt>
+                <c:pt idx="58">
+                  <c:v>89.51</c:v>
+                </c:pt>
+                <c:pt idx="59">
+                  <c:v>-729.4299999999999</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -6180,10 +6210,10 @@
           <c:invertIfNegative val="0"/>
           <c:val>
             <c:numRef>
-              <c:f>景兴纸业!$D$6:$BI$6</c:f>
+              <c:f>景兴纸业!$D$6:$CD$6</c:f>
               <c:numCache>
                 <c:formatCode>[Red]0.00;[Green]\-0.00</c:formatCode>
-                <c:ptCount val="58"/>
+                <c:ptCount val="79"/>
                 <c:pt idx="0">
                   <c:v>-2926.17</c:v>
                 </c:pt>
@@ -6357,6 +6387,12 @@
                 </c:pt>
                 <c:pt idx="57">
                   <c:v>-1349.76</c:v>
+                </c:pt>
+                <c:pt idx="58">
+                  <c:v>-965.15</c:v>
+                </c:pt>
+                <c:pt idx="59">
+                  <c:v>-1861.87</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -7024,10 +7060,10 @@
           <c:invertIfNegative val="0"/>
           <c:val>
             <c:numRef>
-              <c:f>民生银行!$D$6:$BI$6</c:f>
+              <c:f>民生银行!$D$6:$CD$6</c:f>
               <c:numCache>
                 <c:formatCode>[Red]0.00;[Green]\-0.00</c:formatCode>
-                <c:ptCount val="58"/>
+                <c:ptCount val="79"/>
                 <c:pt idx="0">
                   <c:v>-3240.47</c:v>
                 </c:pt>
@@ -7201,6 +7237,12 @@
                 </c:pt>
                 <c:pt idx="57">
                   <c:v>29738.23</c:v>
+                </c:pt>
+                <c:pt idx="58">
+                  <c:v>17179.85</c:v>
+                </c:pt>
+                <c:pt idx="59">
+                  <c:v>8780.43</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -7296,10 +7338,10 @@
           <c:invertIfNegative val="0"/>
           <c:val>
             <c:numRef>
-              <c:f>天宝食品!$D$6:$BI$6</c:f>
+              <c:f>天宝食品!$D$6:$CD$6</c:f>
               <c:numCache>
                 <c:formatCode>[Red]0.00;[Green]\-0.00</c:formatCode>
-                <c:ptCount val="58"/>
+                <c:ptCount val="79"/>
                 <c:pt idx="0">
                   <c:v>203.1</c:v>
                 </c:pt>
@@ -7473,6 +7515,12 @@
                 </c:pt>
                 <c:pt idx="57">
                   <c:v>74.59</c:v>
+                </c:pt>
+                <c:pt idx="58">
+                  <c:v>15.03</c:v>
+                </c:pt>
+                <c:pt idx="59">
+                  <c:v>49.42</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -8140,10 +8188,10 @@
           <c:invertIfNegative val="0"/>
           <c:val>
             <c:numRef>
-              <c:f>中远海发!$D$6:$BI$6</c:f>
+              <c:f>中远海发!$D$6:$CD$6</c:f>
               <c:numCache>
                 <c:formatCode>[Red]0.00;[Green]\-0.00</c:formatCode>
-                <c:ptCount val="58"/>
+                <c:ptCount val="79"/>
                 <c:pt idx="0">
                   <c:v>-14643.97</c:v>
                 </c:pt>
@@ -8317,6 +8365,12 @@
                 </c:pt>
                 <c:pt idx="57">
                   <c:v>-2970.09</c:v>
+                </c:pt>
+                <c:pt idx="58">
+                  <c:v>-445.7</c:v>
+                </c:pt>
+                <c:pt idx="59">
+                  <c:v>554.72</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -8651,6 +8705,7 @@
     </c:plotArea>
     <c:legend>
       <c:legendPos val="r"/>
+      <c:layout/>
       <c:overlay val="0"/>
     </c:legend>
     <c:plotVisOnly val="1"/>
@@ -8942,6 +8997,7 @@
     </c:plotArea>
     <c:legend>
       <c:legendPos val="r"/>
+      <c:layout/>
       <c:overlay val="0"/>
     </c:legend>
     <c:plotVisOnly val="1"/>
@@ -8983,10 +9039,10 @@
           <c:invertIfNegative val="0"/>
           <c:val>
             <c:numRef>
-              <c:f>st智慧!$D$6:$BI$6</c:f>
+              <c:f>st智慧!$D$6:$CD$6</c:f>
               <c:numCache>
                 <c:formatCode>[Red]0.00;[Green]\-0.00</c:formatCode>
-                <c:ptCount val="58"/>
+                <c:ptCount val="79"/>
                 <c:pt idx="0">
                   <c:v>1560.66</c:v>
                 </c:pt>
@@ -9160,6 +9216,12 @@
                 </c:pt>
                 <c:pt idx="57">
                   <c:v>126.97</c:v>
+                </c:pt>
+                <c:pt idx="58">
+                  <c:v>-141.59</c:v>
+                </c:pt>
+                <c:pt idx="59">
+                  <c:v>-300.53</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -9213,6 +9275,7 @@
     </c:plotArea>
     <c:legend>
       <c:legendPos val="r"/>
+      <c:layout/>
       <c:overlay val="0"/>
     </c:legend>
     <c:plotVisOnly val="1"/>
@@ -9826,10 +9889,10 @@
           <c:invertIfNegative val="0"/>
           <c:val>
             <c:numRef>
-              <c:f>中国石化!$D$6:$BI$6</c:f>
+              <c:f>中国石化!$D$6:$CD$6</c:f>
               <c:numCache>
                 <c:formatCode>[Red]0.00;[Green]\-0.00</c:formatCode>
-                <c:ptCount val="58"/>
+                <c:ptCount val="79"/>
                 <c:pt idx="0">
                   <c:v>12051.06</c:v>
                 </c:pt>
@@ -10003,6 +10066,12 @@
                 </c:pt>
                 <c:pt idx="57">
                   <c:v>-2392.08</c:v>
+                </c:pt>
+                <c:pt idx="58">
+                  <c:v>-12951.62</c:v>
+                </c:pt>
+                <c:pt idx="59">
+                  <c:v>620.4299999999999</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -10843,10 +10912,10 @@
           <c:invertIfNegative val="0"/>
           <c:val>
             <c:numRef>
-              <c:f>中国中冶!$D$6:$BI$6</c:f>
+              <c:f>中国中冶!$D$6:$CD$6</c:f>
               <c:numCache>
                 <c:formatCode>[Red]0.00;[Green]\-0.00</c:formatCode>
-                <c:ptCount val="58"/>
+                <c:ptCount val="79"/>
                 <c:pt idx="0">
                   <c:v>6669.91</c:v>
                 </c:pt>
@@ -11020,6 +11089,12 @@
                 </c:pt>
                 <c:pt idx="57">
                   <c:v>-1896.56</c:v>
+                </c:pt>
+                <c:pt idx="58">
+                  <c:v>-3976.43</c:v>
+                </c:pt>
+                <c:pt idx="59">
+                  <c:v>1449.35</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -11688,10 +11763,10 @@
           <c:invertIfNegative val="0"/>
           <c:val>
             <c:numRef>
-              <c:f>远望谷!$D$6:$BI$6</c:f>
+              <c:f>远望谷!$D$6:$CD$6</c:f>
               <c:numCache>
                 <c:formatCode>[Red]0.00;[Green]\-0.00</c:formatCode>
-                <c:ptCount val="58"/>
+                <c:ptCount val="79"/>
                 <c:pt idx="0">
                   <c:v>-5587.2</c:v>
                 </c:pt>
@@ -11865,6 +11940,12 @@
                 </c:pt>
                 <c:pt idx="57">
                   <c:v>-1061.08</c:v>
+                </c:pt>
+                <c:pt idx="58">
+                  <c:v>310.87</c:v>
+                </c:pt>
+                <c:pt idx="59">
+                  <c:v>3632.41</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -12522,10 +12603,10 @@
           <c:invertIfNegative val="0"/>
           <c:val>
             <c:numRef>
-              <c:f>巨轮智能!$D$6:$BI$6</c:f>
+              <c:f>巨轮智能!$D$6:$CD$6</c:f>
               <c:numCache>
                 <c:formatCode>[Red]0.00;[Green]\-0.00</c:formatCode>
-                <c:ptCount val="58"/>
+                <c:ptCount val="79"/>
                 <c:pt idx="0">
                   <c:v>-1260.64</c:v>
                 </c:pt>
@@ -12699,6 +12780,12 @@
                 </c:pt>
                 <c:pt idx="57">
                   <c:v>-71.54</c:v>
+                </c:pt>
+                <c:pt idx="58">
+                  <c:v>-114.08</c:v>
+                </c:pt>
+                <c:pt idx="59">
+                  <c:v>390.1</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -13539,10 +13626,10 @@
           <c:invertIfNegative val="0"/>
           <c:val>
             <c:numRef>
-              <c:f>大金重工!$D$6:$BI$6</c:f>
+              <c:f>大金重工!$D$6:$CD$6</c:f>
               <c:numCache>
                 <c:formatCode>[Red]0.00;[Green]\-0.00</c:formatCode>
-                <c:ptCount val="58"/>
+                <c:ptCount val="79"/>
                 <c:pt idx="0">
                   <c:v>77.57</c:v>
                 </c:pt>
@@ -13716,6 +13803,12 @@
                 </c:pt>
                 <c:pt idx="57">
                   <c:v>-35.4</c:v>
+                </c:pt>
+                <c:pt idx="58">
+                  <c:v>385.89</c:v>
+                </c:pt>
+                <c:pt idx="59">
+                  <c:v>81.16</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -14011,6 +14104,7 @@
     </c:plotArea>
     <c:legend>
       <c:legendPos val="r"/>
+      <c:layout/>
       <c:overlay val="0"/>
     </c:legend>
     <c:plotVisOnly val="1"/>
@@ -14262,6 +14356,7 @@
     </c:plotArea>
     <c:legend>
       <c:legendPos val="r"/>
+      <c:layout/>
       <c:overlay val="0"/>
     </c:legend>
     <c:plotVisOnly val="1"/>
@@ -14303,10 +14398,10 @@
           <c:invertIfNegative val="0"/>
           <c:val>
             <c:numRef>
-              <c:f>普邦股份!$D$6:$BI$6</c:f>
+              <c:f>普邦股份!$D$6:$CD$6</c:f>
               <c:numCache>
                 <c:formatCode>[Red]0.00;[Green]\-0.00</c:formatCode>
-                <c:ptCount val="58"/>
+                <c:ptCount val="79"/>
                 <c:pt idx="0">
                   <c:v>-1286.24</c:v>
                 </c:pt>
@@ -14500,6 +14595,7 @@
     </c:plotArea>
     <c:legend>
       <c:legendPos val="r"/>
+      <c:layout/>
       <c:overlay val="0"/>
     </c:legend>
     <c:plotVisOnly val="1"/>
@@ -15448,6 +15544,7 @@
     </c:plotArea>
     <c:legend>
       <c:legendPos val="r"/>
+      <c:layout/>
       <c:overlay val="0"/>
     </c:legend>
     <c:plotVisOnly val="1"/>
@@ -15682,6 +15779,7 @@
     </c:plotArea>
     <c:legend>
       <c:legendPos val="r"/>
+      <c:layout/>
       <c:overlay val="0"/>
     </c:legend>
     <c:plotVisOnly val="1"/>
@@ -16687,10 +16785,10 @@
           <c:invertIfNegative val="0"/>
           <c:val>
             <c:numRef>
-              <c:f>达华智能!$D$6:$BI$6</c:f>
+              <c:f>达华智能!$D$6:$CD$6</c:f>
               <c:numCache>
                 <c:formatCode>[Red]0.00;[Green]\-0.00</c:formatCode>
-                <c:ptCount val="58"/>
+                <c:ptCount val="79"/>
                 <c:pt idx="0">
                   <c:v>716.65</c:v>
                 </c:pt>
@@ -16864,6 +16962,12 @@
                 </c:pt>
                 <c:pt idx="57">
                   <c:v>614.27</c:v>
+                </c:pt>
+                <c:pt idx="58">
+                  <c:v>456.24</c:v>
+                </c:pt>
+                <c:pt idx="59">
+                  <c:v>456.24</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -16998,16 +17102,16 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>6</xdr:col>
-      <xdr:colOff>25400</xdr:colOff>
-      <xdr:row>52</xdr:row>
-      <xdr:rowOff>0</xdr:rowOff>
+      <xdr:col>17</xdr:col>
+      <xdr:colOff>508000</xdr:colOff>
+      <xdr:row>15</xdr:row>
+      <xdr:rowOff>38100</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>16</xdr:col>
-      <xdr:colOff>101600</xdr:colOff>
-      <xdr:row>68</xdr:row>
-      <xdr:rowOff>12700</xdr:rowOff>
+      <xdr:col>27</xdr:col>
+      <xdr:colOff>584200</xdr:colOff>
+      <xdr:row>31</xdr:row>
+      <xdr:rowOff>50800</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -19197,7 +19301,7 @@
   </sheetPr>
   <dimension ref="A2:BK14"/>
   <sheetViews>
-    <sheetView topLeftCell="A6" workbookViewId="0">
+    <sheetView topLeftCell="H6" workbookViewId="0">
       <selection activeCell="BK7" sqref="BK7"/>
     </sheetView>
   </sheetViews>
@@ -20532,7 +20636,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A2:BK15"/>
   <sheetViews>
-    <sheetView topLeftCell="A14" workbookViewId="0">
+    <sheetView topLeftCell="D9" workbookViewId="0">
       <selection activeCell="BK7" sqref="BK7"/>
     </sheetView>
   </sheetViews>
@@ -21849,7 +21953,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A2:BK18"/>
   <sheetViews>
-    <sheetView topLeftCell="A21" workbookViewId="0">
+    <sheetView topLeftCell="A12" workbookViewId="0">
       <selection activeCell="BK7" sqref="BK7"/>
     </sheetView>
   </sheetViews>
@@ -23214,7 +23318,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A2:BK15"/>
   <sheetViews>
-    <sheetView topLeftCell="AV1" workbookViewId="0">
+    <sheetView topLeftCell="C9" workbookViewId="0">
       <selection activeCell="BK7" sqref="BK7"/>
     </sheetView>
   </sheetViews>
@@ -24582,7 +24686,7 @@
   </sheetPr>
   <dimension ref="A2:BK15"/>
   <sheetViews>
-    <sheetView topLeftCell="A5" workbookViewId="0">
+    <sheetView topLeftCell="A9" workbookViewId="0">
       <selection activeCell="BK7" sqref="BK7"/>
     </sheetView>
   </sheetViews>
@@ -25912,7 +26016,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A2:BK14"/>
   <sheetViews>
-    <sheetView topLeftCell="A12" workbookViewId="0">
+    <sheetView topLeftCell="D10" workbookViewId="0">
       <selection activeCell="BK7" sqref="BK7"/>
     </sheetView>
   </sheetViews>
@@ -27243,7 +27347,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A2:BK14"/>
   <sheetViews>
-    <sheetView topLeftCell="A7" workbookViewId="0">
+    <sheetView topLeftCell="D11" workbookViewId="0">
       <selection activeCell="BK7" sqref="BK7"/>
     </sheetView>
   </sheetViews>
@@ -28565,7 +28669,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A2:BK14"/>
   <sheetViews>
-    <sheetView topLeftCell="A12" workbookViewId="0">
+    <sheetView topLeftCell="I8" workbookViewId="0">
       <selection activeCell="BK7" sqref="BK7"/>
     </sheetView>
   </sheetViews>
@@ -29884,7 +29988,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A2:BK14"/>
   <sheetViews>
-    <sheetView topLeftCell="A10" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="A6" workbookViewId="0">
       <selection activeCell="BK7" sqref="BK7"/>
     </sheetView>
   </sheetViews>
@@ -31203,7 +31307,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A2:AX14"/>
   <sheetViews>
-    <sheetView topLeftCell="AG1" workbookViewId="0">
+    <sheetView topLeftCell="D7" workbookViewId="0">
       <selection activeCell="AX7" sqref="AX7"/>
     </sheetView>
   </sheetViews>
@@ -32264,7 +32368,7 @@
   </sheetPr>
   <dimension ref="A2:AW13"/>
   <sheetViews>
-    <sheetView topLeftCell="A3" workbookViewId="0">
+    <sheetView topLeftCell="E5" workbookViewId="0">
       <selection activeCell="AW7" sqref="AW7"/>
     </sheetView>
   </sheetViews>
@@ -33289,8 +33393,8 @@
   </sheetPr>
   <dimension ref="A1:AE45"/>
   <sheetViews>
-    <sheetView topLeftCell="A6" workbookViewId="0">
-      <selection activeCell="AA7" sqref="AA7"/>
+    <sheetView topLeftCell="F7" workbookViewId="0">
+      <selection activeCell="B7" sqref="B7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -34884,7 +34988,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A2:AR13"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="AC2" workbookViewId="0">
+    <sheetView topLeftCell="A2" workbookViewId="0">
       <selection activeCell="AR7" sqref="AR7"/>
     </sheetView>
   </sheetViews>
@@ -36074,7 +36178,7 @@
   </sheetPr>
   <dimension ref="A2:BK15"/>
   <sheetViews>
-    <sheetView topLeftCell="A4" workbookViewId="0">
+    <sheetView topLeftCell="E2" workbookViewId="0">
       <selection activeCell="BK8" sqref="BK8"/>
     </sheetView>
   </sheetViews>
@@ -37426,7 +37530,7 @@
   </sheetPr>
   <dimension ref="A2:BK17"/>
   <sheetViews>
-    <sheetView topLeftCell="M1" workbookViewId="0">
+    <sheetView topLeftCell="L1" workbookViewId="0">
       <selection activeCell="BK7" sqref="BK7"/>
     </sheetView>
   </sheetViews>
@@ -38802,7 +38906,7 @@
   </sheetPr>
   <dimension ref="A2:BK16"/>
   <sheetViews>
-    <sheetView topLeftCell="BE4" workbookViewId="0">
+    <sheetView topLeftCell="E6" workbookViewId="0">
       <selection activeCell="BK7" sqref="BK7"/>
     </sheetView>
   </sheetViews>
@@ -40186,7 +40290,7 @@
   </sheetPr>
   <dimension ref="A2:BK20"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView topLeftCell="F9" workbookViewId="0">
       <selection activeCell="BK7" sqref="BK7"/>
     </sheetView>
   </sheetViews>
@@ -41551,7 +41655,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A2:BK14"/>
   <sheetViews>
-    <sheetView topLeftCell="A2" workbookViewId="0">
+    <sheetView topLeftCell="D6" workbookViewId="0">
       <selection activeCell="BK7" sqref="BK7"/>
     </sheetView>
   </sheetViews>
@@ -42876,7 +42980,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A2:BK14"/>
   <sheetViews>
-    <sheetView topLeftCell="A16" workbookViewId="0">
+    <sheetView topLeftCell="E11" workbookViewId="0">
       <selection activeCell="BK7" sqref="BK7"/>
     </sheetView>
   </sheetViews>
@@ -44200,7 +44304,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A2:BK15"/>
   <sheetViews>
-    <sheetView topLeftCell="A12" workbookViewId="0">
+    <sheetView topLeftCell="D10" workbookViewId="0">
       <selection activeCell="BK7" sqref="BK7"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
buy media, sell half of minsheng bank
</commit_message>
<xml_diff>
--- a/stock.xlsx
+++ b/stock.xlsx
@@ -1,10 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="22416"/>
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="26405"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="980" yWindow="560" windowWidth="25600" windowHeight="16060" tabRatio="996"/>
+    <workbookView xWindow="980" yWindow="560" windowWidth="25600" windowHeight="16060" tabRatio="996" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="民生银行" sheetId="13" r:id="rId1"/>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="293" uniqueCount="73">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="297" uniqueCount="75">
   <si>
     <t>达华智能</t>
   </si>
@@ -319,6 +319,12 @@
   <si>
     <t>没拿住啊</t>
   </si>
+  <si>
+    <t>小赚，大盘股涨幅慢</t>
+  </si>
+  <si>
+    <t>少赚2k啊。。。</t>
+  </si>
 </sst>
 </file>
 
@@ -462,7 +468,7 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="141">
+  <cellStyleXfs count="143">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -604,8 +610,10 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="42">
+  <cellXfs count="43">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
@@ -648,8 +656,9 @@
     <xf numFmtId="17" fontId="7" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="17" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
   </cellXfs>
-  <cellStyles count="141">
+  <cellStyles count="143">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
@@ -720,6 +729,7 @@
     <cellStyle name="Followed Hyperlink" xfId="136" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="138" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="140" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="142" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
@@ -790,6 +800,7 @@
     <cellStyle name="Hyperlink" xfId="135" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="137" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="139" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="141" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -1045,11 +1056,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="-2088177240"/>
-        <c:axId val="2141691112"/>
+        <c:axId val="-2100581160"/>
+        <c:axId val="-2100580808"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="-2088177240"/>
+        <c:axId val="-2100581160"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1058,7 +1069,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="2141691112"/>
+        <c:crossAx val="-2100580808"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -1066,7 +1077,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="2141691112"/>
+        <c:axId val="-2100580808"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1077,7 +1088,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-2088177240"/>
+        <c:crossAx val="-2100581160"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -1347,11 +1358,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="2145240104"/>
-        <c:axId val="-2122131928"/>
+        <c:axId val="-2097455544"/>
+        <c:axId val="-2097452552"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="2145240104"/>
+        <c:axId val="-2097455544"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1360,7 +1371,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-2122131928"/>
+        <c:crossAx val="-2097452552"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -1368,7 +1379,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="-2122131928"/>
+        <c:axId val="-2097452552"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1379,14 +1390,13 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="2145240104"/>
+        <c:crossAx val="-2097455544"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
     </c:plotArea>
     <c:legend>
       <c:legendPos val="r"/>
-      <c:layout/>
       <c:overlay val="0"/>
     </c:legend>
     <c:plotVisOnly val="1"/>
@@ -1659,11 +1669,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="1776997432"/>
-        <c:axId val="1777000408"/>
+        <c:axId val="-2100521736"/>
+        <c:axId val="-2100518744"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="1776997432"/>
+        <c:axId val="-2100521736"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1672,7 +1682,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="1777000408"/>
+        <c:crossAx val="-2100518744"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -1680,7 +1690,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="1777000408"/>
+        <c:axId val="-2100518744"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:min val="4.3"/>
@@ -1692,14 +1702,13 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="1776997432"/>
+        <c:crossAx val="-2100521736"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
     </c:plotArea>
     <c:legend>
       <c:legendPos val="r"/>
-      <c:layout/>
       <c:overlay val="0"/>
     </c:legend>
     <c:plotVisOnly val="1"/>
@@ -1959,11 +1968,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:gapWidth val="150"/>
-        <c:axId val="2089204072"/>
-        <c:axId val="2143366808"/>
+        <c:axId val="-2096712552"/>
+        <c:axId val="-2096709800"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="2089204072"/>
+        <c:axId val="-2096712552"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1972,7 +1981,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="2143366808"/>
+        <c:crossAx val="-2096709800"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -1980,7 +1989,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="2143366808"/>
+        <c:axId val="-2096709800"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1991,14 +2000,13 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="2089204072"/>
+        <c:crossAx val="-2096712552"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
     </c:plotArea>
     <c:legend>
       <c:legendPos val="r"/>
-      <c:layout/>
       <c:overlay val="0"/>
     </c:legend>
     <c:plotVisOnly val="1"/>
@@ -2261,11 +2269,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="-2102597544"/>
-        <c:axId val="-2102989144"/>
+        <c:axId val="-2100507464"/>
+        <c:axId val="-2100504472"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="-2102597544"/>
+        <c:axId val="-2100507464"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2274,7 +2282,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-2102989144"/>
+        <c:crossAx val="-2100504472"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -2282,7 +2290,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="-2102989144"/>
+        <c:axId val="-2100504472"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2293,14 +2301,13 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-2102597544"/>
+        <c:crossAx val="-2100507464"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
     </c:plotArea>
     <c:legend>
       <c:legendPos val="r"/>
-      <c:layout/>
       <c:overlay val="0"/>
     </c:legend>
     <c:plotVisOnly val="1"/>
@@ -2573,11 +2580,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="-2102766136"/>
-        <c:axId val="-2102687144"/>
+        <c:axId val="-2097441304"/>
+        <c:axId val="-2097438312"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="-2102766136"/>
+        <c:axId val="-2097441304"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2586,7 +2593,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-2102687144"/>
+        <c:crossAx val="-2097438312"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -2594,7 +2601,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="-2102687144"/>
+        <c:axId val="-2097438312"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:min val="6.5"/>
@@ -2606,14 +2613,13 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-2102766136"/>
+        <c:crossAx val="-2097441304"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
     </c:plotArea>
     <c:legend>
       <c:legendPos val="r"/>
-      <c:layout/>
       <c:overlay val="0"/>
     </c:legend>
     <c:plotVisOnly val="1"/>
@@ -2873,11 +2879,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:gapWidth val="150"/>
-        <c:axId val="-2102867176"/>
-        <c:axId val="-2102765144"/>
+        <c:axId val="-2095597960"/>
+        <c:axId val="-2095595272"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="-2102867176"/>
+        <c:axId val="-2095597960"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2886,7 +2892,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-2102765144"/>
+        <c:crossAx val="-2095595272"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -2894,7 +2900,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="-2102765144"/>
+        <c:axId val="-2095595272"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2905,14 +2911,13 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-2102867176"/>
+        <c:crossAx val="-2095597960"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
     </c:plotArea>
     <c:legend>
       <c:legendPos val="r"/>
-      <c:layout/>
       <c:overlay val="0"/>
     </c:legend>
     <c:plotVisOnly val="1"/>
@@ -3175,11 +3180,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="1777103048"/>
-        <c:axId val="1777106024"/>
+        <c:axId val="-2097385624"/>
+        <c:axId val="-2097382984"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="1777103048"/>
+        <c:axId val="-2097385624"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3188,7 +3193,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="1777106024"/>
+        <c:crossAx val="-2097382984"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -3196,7 +3201,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="1777106024"/>
+        <c:axId val="-2097382984"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3207,14 +3212,13 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="1777103048"/>
+        <c:crossAx val="-2097385624"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
     </c:plotArea>
     <c:legend>
       <c:legendPos val="r"/>
-      <c:layout/>
       <c:overlay val="0"/>
     </c:legend>
     <c:plotVisOnly val="1"/>
@@ -3487,11 +3491,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="1777301048"/>
-        <c:axId val="1777308072"/>
+        <c:axId val="-2097346424"/>
+        <c:axId val="-2097343752"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="1777301048"/>
+        <c:axId val="-2097346424"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3500,7 +3504,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="1777308072"/>
+        <c:crossAx val="-2097343752"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -3508,7 +3512,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="1777308072"/>
+        <c:axId val="-2097343752"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:min val="9.0"/>
@@ -3520,14 +3524,13 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="1777301048"/>
+        <c:crossAx val="-2097346424"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
     </c:plotArea>
     <c:legend>
       <c:legendPos val="r"/>
-      <c:layout/>
       <c:overlay val="0"/>
     </c:legend>
     <c:plotVisOnly val="1"/>
@@ -3787,11 +3790,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:gapWidth val="150"/>
-        <c:axId val="1776868968"/>
-        <c:axId val="1776871976"/>
+        <c:axId val="-2100469032"/>
+        <c:axId val="-2100466040"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="1776868968"/>
+        <c:axId val="-2100469032"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3800,7 +3803,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="1776871976"/>
+        <c:crossAx val="-2100466040"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -3808,7 +3811,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="1776871976"/>
+        <c:axId val="-2100466040"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3819,14 +3822,13 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="1776868968"/>
+        <c:crossAx val="-2100469032"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
     </c:plotArea>
     <c:legend>
       <c:legendPos val="r"/>
-      <c:layout/>
       <c:overlay val="0"/>
     </c:legend>
     <c:plotVisOnly val="1"/>
@@ -4089,11 +4091,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="1777318824"/>
-        <c:axId val="1777080360"/>
+        <c:axId val="-2097329480"/>
+        <c:axId val="-2097326200"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="1777318824"/>
+        <c:axId val="-2097329480"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -4102,7 +4104,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="1777080360"/>
+        <c:crossAx val="-2097326200"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -4110,7 +4112,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="1777080360"/>
+        <c:axId val="-2097326200"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -4121,14 +4123,13 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="1777318824"/>
+        <c:crossAx val="-2097329480"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
     </c:plotArea>
     <c:legend>
       <c:legendPos val="r"/>
-      <c:layout/>
       <c:overlay val="0"/>
     </c:legend>
     <c:plotVisOnly val="1"/>
@@ -4401,11 +4402,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="-2088694632"/>
-        <c:axId val="2142133592"/>
+        <c:axId val="-2100564280"/>
+        <c:axId val="-2100561224"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="-2088694632"/>
+        <c:axId val="-2100564280"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -4414,7 +4415,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="2142133592"/>
+        <c:crossAx val="-2100561224"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -4422,7 +4423,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="2142133592"/>
+        <c:axId val="-2100561224"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -4433,7 +4434,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-2088694632"/>
+        <c:crossAx val="-2100564280"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -4713,11 +4714,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="-2013009656"/>
-        <c:axId val="-2102736376"/>
+        <c:axId val="-2100437576"/>
+        <c:axId val="-2100434568"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="-2013009656"/>
+        <c:axId val="-2100437576"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -4726,7 +4727,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-2102736376"/>
+        <c:crossAx val="-2100434568"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -4734,7 +4735,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="-2102736376"/>
+        <c:axId val="-2100434568"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:min val="10.0"/>
@@ -4746,14 +4747,13 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-2013009656"/>
+        <c:crossAx val="-2100437576"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
     </c:plotArea>
     <c:legend>
       <c:legendPos val="r"/>
-      <c:layout/>
       <c:overlay val="0"/>
     </c:legend>
     <c:plotVisOnly val="1"/>
@@ -5013,11 +5013,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:gapWidth val="150"/>
-        <c:axId val="-2103273096"/>
-        <c:axId val="2147437112"/>
+        <c:axId val="-2095579240"/>
+        <c:axId val="-2095576248"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="-2103273096"/>
+        <c:axId val="-2095579240"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -5026,7 +5026,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="2147437112"/>
+        <c:crossAx val="-2095576248"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -5034,7 +5034,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="2147437112"/>
+        <c:axId val="-2095576248"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -5045,14 +5045,13 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-2103273096"/>
+        <c:crossAx val="-2095579240"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
     </c:plotArea>
     <c:legend>
       <c:legendPos val="r"/>
-      <c:layout/>
       <c:overlay val="0"/>
     </c:legend>
     <c:plotVisOnly val="1"/>
@@ -5315,11 +5314,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="1777132920"/>
-        <c:axId val="1777142936"/>
+        <c:axId val="-2101385256"/>
+        <c:axId val="-2101382248"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="1777132920"/>
+        <c:axId val="-2101385256"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -5328,7 +5327,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="1777142936"/>
+        <c:crossAx val="-2101382248"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -5336,7 +5335,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="1777142936"/>
+        <c:axId val="-2101382248"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -5347,14 +5346,13 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="1777132920"/>
+        <c:crossAx val="-2101385256"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
     </c:plotArea>
     <c:legend>
       <c:legendPos val="r"/>
-      <c:layout/>
       <c:overlay val="0"/>
     </c:legend>
     <c:plotVisOnly val="1"/>
@@ -5627,11 +5625,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="1777122984"/>
-        <c:axId val="1777125992"/>
+        <c:axId val="-2102206456"/>
+        <c:axId val="-2102209464"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="1777122984"/>
+        <c:axId val="-2102206456"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -5640,7 +5638,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="1777125992"/>
+        <c:crossAx val="-2102209464"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -5648,7 +5646,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="1777125992"/>
+        <c:axId val="-2102209464"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -5659,14 +5657,13 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="1777122984"/>
+        <c:crossAx val="-2102206456"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
     </c:plotArea>
     <c:legend>
       <c:legendPos val="r"/>
-      <c:layout/>
       <c:overlay val="0"/>
     </c:legend>
     <c:plotVisOnly val="1"/>
@@ -5926,11 +5923,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:gapWidth val="150"/>
-        <c:axId val="1777087208"/>
-        <c:axId val="1776359624"/>
+        <c:axId val="-2102228936"/>
+        <c:axId val="-2102239256"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="1777087208"/>
+        <c:axId val="-2102228936"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -5939,7 +5936,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="1776359624"/>
+        <c:crossAx val="-2102239256"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -5947,7 +5944,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="1776359624"/>
+        <c:axId val="-2102239256"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -5958,14 +5955,13 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="1777087208"/>
+        <c:crossAx val="-2102228936"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
     </c:plotArea>
     <c:legend>
       <c:legendPos val="r"/>
-      <c:layout/>
       <c:overlay val="0"/>
     </c:legend>
     <c:plotVisOnly val="1"/>
@@ -6228,11 +6224,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="1777233784"/>
-        <c:axId val="1777237096"/>
+        <c:axId val="-2102278968"/>
+        <c:axId val="-2102289336"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="1777233784"/>
+        <c:axId val="-2102278968"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -6241,7 +6237,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="1777237096"/>
+        <c:crossAx val="-2102289336"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -6249,7 +6245,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="1777237096"/>
+        <c:axId val="-2102289336"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -6260,14 +6256,13 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="1777233784"/>
+        <c:crossAx val="-2102278968"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
     </c:plotArea>
     <c:legend>
       <c:legendPos val="r"/>
-      <c:layout/>
       <c:overlay val="0"/>
     </c:legend>
     <c:plotVisOnly val="1"/>
@@ -6540,11 +6535,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="1776996312"/>
-        <c:axId val="2143313880"/>
+        <c:axId val="-2102316728"/>
+        <c:axId val="-2102327016"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="1776996312"/>
+        <c:axId val="-2102316728"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -6553,7 +6548,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="2143313880"/>
+        <c:crossAx val="-2102327016"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -6561,7 +6556,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="2143313880"/>
+        <c:axId val="-2102327016"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:min val="5.0"/>
@@ -6573,14 +6568,13 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="1776996312"/>
+        <c:crossAx val="-2102316728"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
     </c:plotArea>
     <c:legend>
       <c:legendPos val="r"/>
-      <c:layout/>
       <c:overlay val="0"/>
     </c:legend>
     <c:plotVisOnly val="1"/>
@@ -6840,11 +6834,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:gapWidth val="150"/>
-        <c:axId val="1776820184"/>
-        <c:axId val="1776823192"/>
+        <c:axId val="-2102342424"/>
+        <c:axId val="-2102352584"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="1776820184"/>
+        <c:axId val="-2102342424"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -6853,7 +6847,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="1776823192"/>
+        <c:crossAx val="-2102352584"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -6861,7 +6855,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="1776823192"/>
+        <c:axId val="-2102352584"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -6872,14 +6866,13 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="1776820184"/>
+        <c:crossAx val="-2102342424"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
     </c:plotArea>
     <c:legend>
       <c:legendPos val="r"/>
-      <c:layout/>
       <c:overlay val="0"/>
     </c:legend>
     <c:plotVisOnly val="1"/>
@@ -7142,11 +7135,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="1776754952"/>
-        <c:axId val="1776757960"/>
+        <c:axId val="-2096643992"/>
+        <c:axId val="-2096641048"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="1776754952"/>
+        <c:axId val="-2096643992"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -7155,7 +7148,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="1776757960"/>
+        <c:crossAx val="-2096641048"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -7163,7 +7156,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="1776757960"/>
+        <c:axId val="-2096641048"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -7174,14 +7167,13 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="1776754952"/>
+        <c:crossAx val="-2096643992"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
     </c:plotArea>
     <c:legend>
       <c:legendPos val="r"/>
-      <c:layout/>
       <c:overlay val="0"/>
     </c:legend>
     <c:plotVisOnly val="1"/>
@@ -7454,11 +7446,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="1776557880"/>
-        <c:axId val="1776560888"/>
+        <c:axId val="-2096605992"/>
+        <c:axId val="-2096603032"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="1776557880"/>
+        <c:axId val="-2096605992"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -7467,7 +7459,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="1776560888"/>
+        <c:crossAx val="-2096603032"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -7475,7 +7467,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="1776560888"/>
+        <c:axId val="-2096603032"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -7486,14 +7478,13 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="1776557880"/>
+        <c:crossAx val="-2096605992"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
     </c:plotArea>
     <c:legend>
       <c:legendPos val="r"/>
-      <c:layout/>
       <c:overlay val="0"/>
     </c:legend>
     <c:plotVisOnly val="1"/>
@@ -7753,11 +7744,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:gapWidth val="150"/>
-        <c:axId val="-2088336552"/>
-        <c:axId val="2103612984"/>
+        <c:axId val="-2101450136"/>
+        <c:axId val="-2101447288"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="-2088336552"/>
+        <c:axId val="-2101450136"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -7766,7 +7757,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="2103612984"/>
+        <c:crossAx val="-2101447288"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -7774,7 +7765,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="2103612984"/>
+        <c:axId val="-2101447288"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -7785,7 +7776,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-2088336552"/>
+        <c:crossAx val="-2101450136"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -8052,11 +8043,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:gapWidth val="150"/>
-        <c:axId val="1776530328"/>
-        <c:axId val="1776517800"/>
+        <c:axId val="-2095548664"/>
+        <c:axId val="-2095564408"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="1776530328"/>
+        <c:axId val="-2095548664"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -8065,7 +8056,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="1776517800"/>
+        <c:crossAx val="-2095564408"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -8073,7 +8064,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="1776517800"/>
+        <c:axId val="-2095564408"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -8084,14 +8075,13 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="1776530328"/>
+        <c:crossAx val="-2095548664"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
     </c:plotArea>
     <c:legend>
       <c:legendPos val="r"/>
-      <c:layout/>
       <c:overlay val="0"/>
     </c:legend>
     <c:plotVisOnly val="1"/>
@@ -8354,11 +8344,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="1776463656"/>
-        <c:axId val="1776466664"/>
+        <c:axId val="-2096578088"/>
+        <c:axId val="-2096575096"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="1776463656"/>
+        <c:axId val="-2096578088"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -8367,7 +8357,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="1776466664"/>
+        <c:crossAx val="-2096575096"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -8375,7 +8365,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="1776466664"/>
+        <c:axId val="-2096575096"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -8386,14 +8376,13 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="1776463656"/>
+        <c:crossAx val="-2096578088"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
     </c:plotArea>
     <c:legend>
       <c:legendPos val="r"/>
-      <c:layout/>
       <c:overlay val="0"/>
     </c:legend>
     <c:plotVisOnly val="1"/>
@@ -8666,11 +8655,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="1776514248"/>
-        <c:axId val="1776443992"/>
+        <c:axId val="-2102358744"/>
+        <c:axId val="-2102361752"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="1776514248"/>
+        <c:axId val="-2102358744"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -8679,7 +8668,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="1776443992"/>
+        <c:crossAx val="-2102361752"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -8687,7 +8676,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="1776443992"/>
+        <c:axId val="-2102361752"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -8698,14 +8687,13 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="1776514248"/>
+        <c:crossAx val="-2102358744"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
     </c:plotArea>
     <c:legend>
       <c:legendPos val="r"/>
-      <c:layout/>
       <c:overlay val="0"/>
     </c:legend>
     <c:plotVisOnly val="1"/>
@@ -8965,11 +8953,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:gapWidth val="150"/>
-        <c:axId val="1776690040"/>
-        <c:axId val="2143456040"/>
+        <c:axId val="-2102382824"/>
+        <c:axId val="-2102392600"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="1776690040"/>
+        <c:axId val="-2102382824"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -8978,7 +8966,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="2143456040"/>
+        <c:crossAx val="-2102392600"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -8986,7 +8974,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="2143456040"/>
+        <c:axId val="-2102392600"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -8997,14 +8985,13 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="1776690040"/>
+        <c:crossAx val="-2102382824"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
     </c:plotArea>
     <c:legend>
       <c:legendPos val="r"/>
-      <c:layout/>
       <c:overlay val="0"/>
     </c:legend>
     <c:plotVisOnly val="1"/>
@@ -9267,11 +9254,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="1776310168"/>
-        <c:axId val="-2121679752"/>
+        <c:axId val="-2096534040"/>
+        <c:axId val="-2096531032"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="1776310168"/>
+        <c:axId val="-2096534040"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -9280,7 +9267,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-2121679752"/>
+        <c:crossAx val="-2096531032"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -9288,7 +9275,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="-2121679752"/>
+        <c:axId val="-2096531032"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -9299,14 +9286,13 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="1776310168"/>
+        <c:crossAx val="-2096534040"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
     </c:plotArea>
     <c:legend>
       <c:legendPos val="r"/>
-      <c:layout/>
       <c:overlay val="0"/>
     </c:legend>
     <c:plotVisOnly val="1"/>
@@ -9579,11 +9565,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="1776804248"/>
-        <c:axId val="1776807256"/>
+        <c:axId val="-2093756648"/>
+        <c:axId val="-2093753640"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="1776804248"/>
+        <c:axId val="-2093756648"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -9592,7 +9578,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="1776807256"/>
+        <c:crossAx val="-2093753640"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -9600,7 +9586,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="1776807256"/>
+        <c:axId val="-2093753640"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:min val="3.0"/>
@@ -9612,14 +9598,13 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="1776804248"/>
+        <c:crossAx val="-2093756648"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
     </c:plotArea>
     <c:legend>
       <c:legendPos val="r"/>
-      <c:layout/>
       <c:overlay val="0"/>
     </c:legend>
     <c:plotVisOnly val="1"/>
@@ -9879,11 +9864,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:gapWidth val="150"/>
-        <c:axId val="-2121349864"/>
-        <c:axId val="1777025192"/>
+        <c:axId val="-2096546248"/>
+        <c:axId val="-2096542024"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="-2121349864"/>
+        <c:axId val="-2096546248"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -9892,7 +9877,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="1777025192"/>
+        <c:crossAx val="-2096542024"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -9900,7 +9885,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="1777025192"/>
+        <c:axId val="-2096542024"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -9911,14 +9896,13 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-2121349864"/>
+        <c:crossAx val="-2096546248"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
     </c:plotArea>
     <c:legend>
       <c:legendPos val="r"/>
-      <c:layout/>
       <c:overlay val="0"/>
     </c:legend>
     <c:plotVisOnly val="1"/>
@@ -10181,11 +10165,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="-2121557624"/>
-        <c:axId val="-2121958264"/>
+        <c:axId val="-2100385864"/>
+        <c:axId val="-2100382856"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="-2121557624"/>
+        <c:axId val="-2100385864"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -10194,7 +10178,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-2121958264"/>
+        <c:crossAx val="-2100382856"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -10202,7 +10186,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="-2121958264"/>
+        <c:axId val="-2100382856"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -10213,14 +10197,13 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-2121557624"/>
+        <c:crossAx val="-2100385864"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
     </c:plotArea>
     <c:legend>
       <c:legendPos val="r"/>
-      <c:layout/>
       <c:overlay val="0"/>
     </c:legend>
     <c:plotVisOnly val="1"/>
@@ -10493,11 +10476,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="-2121773592"/>
-        <c:axId val="-2121719544"/>
+        <c:axId val="-2093704648"/>
+        <c:axId val="-2093701624"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="-2121773592"/>
+        <c:axId val="-2093704648"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -10506,7 +10489,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-2121719544"/>
+        <c:crossAx val="-2093701624"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -10514,7 +10497,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="-2121719544"/>
+        <c:axId val="-2093701624"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -10525,14 +10508,13 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-2121773592"/>
+        <c:crossAx val="-2093704648"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
     </c:plotArea>
     <c:legend>
       <c:legendPos val="r"/>
-      <c:layout/>
       <c:overlay val="0"/>
     </c:legend>
     <c:plotVisOnly val="1"/>
@@ -10792,11 +10774,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:gapWidth val="150"/>
-        <c:axId val="-2122021000"/>
-        <c:axId val="-2121949864"/>
+        <c:axId val="-2093678744"/>
+        <c:axId val="-2093675720"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="-2122021000"/>
+        <c:axId val="-2093678744"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -10805,7 +10787,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-2121949864"/>
+        <c:crossAx val="-2093675720"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -10813,7 +10795,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="-2121949864"/>
+        <c:axId val="-2093675720"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -10824,14 +10806,13 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-2122021000"/>
+        <c:crossAx val="-2093678744"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
     </c:plotArea>
     <c:legend>
       <c:legendPos val="r"/>
-      <c:layout/>
       <c:overlay val="0"/>
     </c:legend>
     <c:plotVisOnly val="1"/>
@@ -10986,11 +10967,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="-2115314168"/>
-        <c:axId val="-1992966760"/>
+        <c:axId val="-2101430536"/>
+        <c:axId val="-2101427544"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="-2115314168"/>
+        <c:axId val="-2101430536"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -10999,7 +10980,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-1992966760"/>
+        <c:crossAx val="-2101427544"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -11008,7 +10989,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="-1992966760"/>
+        <c:axId val="-2101427544"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -11019,7 +11000,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-2115314168"/>
+        <c:crossAx val="-2101430536"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -11289,11 +11270,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="-2122165800"/>
-        <c:axId val="-2122298264"/>
+        <c:axId val="-2096511032"/>
+        <c:axId val="-2100416312"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="-2122165800"/>
+        <c:axId val="-2096511032"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -11302,7 +11283,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-2122298264"/>
+        <c:crossAx val="-2100416312"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -11310,7 +11291,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="-2122298264"/>
+        <c:axId val="-2100416312"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -11321,14 +11302,13 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-2122165800"/>
+        <c:crossAx val="-2096511032"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
     </c:plotArea>
     <c:legend>
       <c:legendPos val="r"/>
-      <c:layout/>
       <c:overlay val="0"/>
     </c:legend>
     <c:plotVisOnly val="1"/>
@@ -11601,11 +11581,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="-2121657528"/>
-        <c:axId val="-2121821016"/>
+        <c:axId val="-2096499304"/>
+        <c:axId val="-2096496280"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="-2121657528"/>
+        <c:axId val="-2096499304"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -11614,7 +11594,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-2121821016"/>
+        <c:crossAx val="-2096496280"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -11622,7 +11602,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="-2121821016"/>
+        <c:axId val="-2096496280"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -11633,14 +11613,13 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-2121657528"/>
+        <c:crossAx val="-2096499304"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
     </c:plotArea>
     <c:legend>
       <c:legendPos val="r"/>
-      <c:layout/>
       <c:overlay val="0"/>
     </c:legend>
     <c:plotVisOnly val="1"/>
@@ -11900,11 +11879,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:gapWidth val="150"/>
-        <c:axId val="1776295816"/>
-        <c:axId val="2143328616"/>
+        <c:axId val="-2096470136"/>
+        <c:axId val="-2096467128"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="1776295816"/>
+        <c:axId val="-2096470136"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -11913,7 +11892,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="2143328616"/>
+        <c:crossAx val="-2096467128"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -11921,7 +11900,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="2143328616"/>
+        <c:axId val="-2096467128"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -11932,14 +11911,13 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="1776295816"/>
+        <c:crossAx val="-2096470136"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
     </c:plotArea>
     <c:legend>
       <c:legendPos val="r"/>
-      <c:layout/>
       <c:overlay val="0"/>
     </c:legend>
     <c:plotVisOnly val="1"/>
@@ -12202,11 +12180,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="1776374200"/>
-        <c:axId val="1776377208"/>
+        <c:axId val="-2096453480"/>
+        <c:axId val="-2096450424"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="1776374200"/>
+        <c:axId val="-2096453480"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -12215,7 +12193,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="1776377208"/>
+        <c:crossAx val="-2096450424"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -12223,7 +12201,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="1776377208"/>
+        <c:axId val="-2096450424"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -12234,14 +12212,13 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="1776374200"/>
+        <c:crossAx val="-2096453480"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
     </c:plotArea>
     <c:legend>
       <c:legendPos val="r"/>
-      <c:layout/>
       <c:overlay val="0"/>
     </c:legend>
     <c:plotVisOnly val="1"/>
@@ -12514,11 +12491,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="2144713800"/>
-        <c:axId val="1776817368"/>
+        <c:axId val="-2093603064"/>
+        <c:axId val="-2093599992"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="2144713800"/>
+        <c:axId val="-2093603064"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -12527,7 +12504,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="1776817368"/>
+        <c:crossAx val="-2093599992"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -12535,7 +12512,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="1776817368"/>
+        <c:axId val="-2093599992"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:min val="8.0"/>
@@ -12547,14 +12524,13 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="2144713800"/>
+        <c:crossAx val="-2093603064"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
     </c:plotArea>
     <c:legend>
       <c:legendPos val="r"/>
-      <c:layout/>
       <c:overlay val="0"/>
     </c:legend>
     <c:plotVisOnly val="1"/>
@@ -12814,11 +12790,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:gapWidth val="150"/>
-        <c:axId val="1776665704"/>
-        <c:axId val="1776668712"/>
+        <c:axId val="-2096417192"/>
+        <c:axId val="-2096414136"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="1776665704"/>
+        <c:axId val="-2096417192"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -12827,7 +12803,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="1776668712"/>
+        <c:crossAx val="-2096414136"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -12835,7 +12811,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="1776668712"/>
+        <c:axId val="-2096414136"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -12846,14 +12822,13 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="1776665704"/>
+        <c:crossAx val="-2096417192"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
     </c:plotArea>
     <c:legend>
       <c:legendPos val="r"/>
-      <c:layout/>
       <c:overlay val="0"/>
     </c:legend>
     <c:plotVisOnly val="1"/>
@@ -13116,11 +13091,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="2144281432"/>
-        <c:axId val="1777184984"/>
+        <c:axId val="-2100342520"/>
+        <c:axId val="-2100339512"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="2144281432"/>
+        <c:axId val="-2100342520"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -13129,7 +13104,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="1777184984"/>
+        <c:crossAx val="-2100339512"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -13137,7 +13112,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="1777184984"/>
+        <c:axId val="-2100339512"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -13148,14 +13123,13 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="2144281432"/>
+        <c:crossAx val="-2100342520"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
     </c:plotArea>
     <c:legend>
       <c:legendPos val="r"/>
-      <c:layout/>
       <c:overlay val="0"/>
     </c:legend>
     <c:plotVisOnly val="1"/>
@@ -13418,11 +13392,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="1776419688"/>
-        <c:axId val="-2122230152"/>
+        <c:axId val="-2101157752"/>
+        <c:axId val="-2101167496"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="1776419688"/>
+        <c:axId val="-2101157752"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -13431,7 +13405,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-2122230152"/>
+        <c:crossAx val="-2101167496"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -13439,7 +13413,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="-2122230152"/>
+        <c:axId val="-2101167496"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -13450,14 +13424,13 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="1776419688"/>
+        <c:crossAx val="-2101157752"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
     </c:plotArea>
     <c:legend>
       <c:legendPos val="r"/>
-      <c:layout/>
       <c:overlay val="0"/>
     </c:legend>
     <c:plotVisOnly val="1"/>
@@ -13717,11 +13690,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:gapWidth val="150"/>
-        <c:axId val="2144597480"/>
-        <c:axId val="1776698440"/>
+        <c:axId val="-2101183896"/>
+        <c:axId val="-2101193368"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="2144597480"/>
+        <c:axId val="-2101183896"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -13730,7 +13703,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="1776698440"/>
+        <c:crossAx val="-2101193368"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -13738,7 +13711,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="1776698440"/>
+        <c:axId val="-2101193368"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -13749,14 +13722,13 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="2144597480"/>
+        <c:crossAx val="-2101183896"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
     </c:plotArea>
     <c:legend>
       <c:legendPos val="r"/>
-      <c:layout/>
       <c:overlay val="0"/>
     </c:legend>
     <c:plotVisOnly val="1"/>
@@ -14019,11 +13991,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="1776909880"/>
-        <c:axId val="1776912888"/>
+        <c:axId val="-2097257832"/>
+        <c:axId val="-2097254824"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="1776909880"/>
+        <c:axId val="-2097257832"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -14032,7 +14004,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="1776912888"/>
+        <c:crossAx val="-2097254824"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -14040,7 +14012,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="1776912888"/>
+        <c:axId val="-2097254824"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -14051,14 +14023,13 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="1776909880"/>
+        <c:crossAx val="-2097257832"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
     </c:plotArea>
     <c:legend>
       <c:legendPos val="r"/>
-      <c:layout/>
       <c:overlay val="0"/>
     </c:legend>
     <c:plotVisOnly val="1"/>
@@ -14213,11 +14184,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="2103762152"/>
-        <c:axId val="-2088408904"/>
+        <c:axId val="-2097478488"/>
+        <c:axId val="-2097475208"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="2103762152"/>
+        <c:axId val="-2097478488"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -14226,7 +14197,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-2088408904"/>
+        <c:crossAx val="-2097475208"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -14235,7 +14206,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="-2088408904"/>
+        <c:axId val="-2097475208"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -14246,7 +14217,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="2103762152"/>
+        <c:crossAx val="-2097478488"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -14526,11 +14497,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="-2074463736"/>
-        <c:axId val="-2074108952"/>
+        <c:axId val="-2093587736"/>
+        <c:axId val="-2093586232"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="-2074463736"/>
+        <c:axId val="-2093587736"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -14539,7 +14510,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-2074108952"/>
+        <c:crossAx val="-2093586232"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -14547,7 +14518,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="-2074108952"/>
+        <c:axId val="-2093586232"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:min val="4.5"/>
@@ -14559,14 +14530,13 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-2074463736"/>
+        <c:crossAx val="-2093587736"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
     </c:plotArea>
     <c:legend>
       <c:legendPos val="r"/>
-      <c:layout/>
       <c:overlay val="0"/>
     </c:legend>
     <c:plotVisOnly val="1"/>
@@ -14826,11 +14796,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:gapWidth val="150"/>
-        <c:axId val="-2074727496"/>
-        <c:axId val="-2074184216"/>
+        <c:axId val="-2097223560"/>
+        <c:axId val="-2097220504"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="-2074727496"/>
+        <c:axId val="-2097223560"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -14839,7 +14809,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-2074184216"/>
+        <c:crossAx val="-2097220504"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -14847,7 +14817,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="-2074184216"/>
+        <c:axId val="-2097220504"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -14858,14 +14828,13 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-2074727496"/>
+        <c:crossAx val="-2097223560"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
     </c:plotArea>
     <c:legend>
       <c:legendPos val="r"/>
-      <c:layout/>
       <c:overlay val="0"/>
     </c:legend>
     <c:plotVisOnly val="1"/>
@@ -15089,11 +15058,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="-2074621656"/>
-        <c:axId val="-2074854392"/>
+        <c:axId val="-2096392088"/>
+        <c:axId val="-2096389032"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="-2074621656"/>
+        <c:axId val="-2096392088"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -15102,7 +15071,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-2074854392"/>
+        <c:crossAx val="-2096389032"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -15110,7 +15079,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="-2074854392"/>
+        <c:axId val="-2096389032"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -15121,14 +15090,13 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-2074621656"/>
+        <c:crossAx val="-2096392088"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
     </c:plotArea>
     <c:legend>
       <c:legendPos val="r"/>
-      <c:layout/>
       <c:overlay val="0"/>
     </c:legend>
     <c:plotVisOnly val="1"/>
@@ -15362,11 +15330,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="-2074264408"/>
-        <c:axId val="-2074921384"/>
+        <c:axId val="-2096349816"/>
+        <c:axId val="-2096346808"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="-2074264408"/>
+        <c:axId val="-2096349816"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -15375,7 +15343,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-2074921384"/>
+        <c:crossAx val="-2096346808"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -15383,7 +15351,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="-2074921384"/>
+        <c:axId val="-2096346808"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -15394,14 +15362,13 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-2074264408"/>
+        <c:crossAx val="-2096349816"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
     </c:plotArea>
     <c:legend>
       <c:legendPos val="r"/>
-      <c:layout/>
       <c:overlay val="0"/>
     </c:legend>
     <c:plotVisOnly val="1"/>
@@ -15622,11 +15589,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:gapWidth val="150"/>
-        <c:axId val="-2074425352"/>
-        <c:axId val="-2074662792"/>
+        <c:axId val="-2097204952"/>
+        <c:axId val="-2097201896"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="-2074425352"/>
+        <c:axId val="-2097204952"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -15635,7 +15602,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-2074662792"/>
+        <c:crossAx val="-2097201896"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -15643,7 +15610,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="-2074662792"/>
+        <c:axId val="-2097201896"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -15654,14 +15621,13 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-2074425352"/>
+        <c:crossAx val="-2097204952"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
     </c:plotArea>
     <c:legend>
       <c:legendPos val="r"/>
-      <c:layout/>
       <c:overlay val="0"/>
     </c:legend>
     <c:plotVisOnly val="1"/>
@@ -15882,11 +15848,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="-2074127224"/>
-        <c:axId val="-2074142840"/>
+        <c:axId val="-2094847176"/>
+        <c:axId val="-2094844120"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="-2074127224"/>
+        <c:axId val="-2094847176"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -15895,7 +15861,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-2074142840"/>
+        <c:crossAx val="-2094844120"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -15903,7 +15869,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="-2074142840"/>
+        <c:axId val="-2094844120"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -15914,14 +15880,13 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-2074127224"/>
+        <c:crossAx val="-2094847176"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
     </c:plotArea>
     <c:legend>
       <c:legendPos val="r"/>
-      <c:layout/>
       <c:overlay val="0"/>
     </c:legend>
     <c:plotVisOnly val="1"/>
@@ -16152,11 +16117,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="-2074200168"/>
-        <c:axId val="-2074206472"/>
+        <c:axId val="-2094807400"/>
+        <c:axId val="-2094804392"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="-2074200168"/>
+        <c:axId val="-2094807400"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -16165,7 +16130,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-2074206472"/>
+        <c:crossAx val="-2094804392"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -16173,7 +16138,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="-2074206472"/>
+        <c:axId val="-2094804392"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:min val="450.0"/>
@@ -16185,14 +16150,13 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-2074200168"/>
+        <c:crossAx val="-2094807400"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
     </c:plotArea>
     <c:legend>
       <c:legendPos val="r"/>
-      <c:layout/>
       <c:overlay val="0"/>
     </c:legend>
     <c:plotVisOnly val="1"/>
@@ -16410,11 +16374,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:gapWidth val="150"/>
-        <c:axId val="-2074239672"/>
-        <c:axId val="-2074250376"/>
+        <c:axId val="-2101248424"/>
+        <c:axId val="-2101258728"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="-2074239672"/>
+        <c:axId val="-2101248424"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -16423,7 +16387,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-2074250376"/>
+        <c:crossAx val="-2101258728"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -16431,7 +16395,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="-2074250376"/>
+        <c:axId val="-2101258728"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -16442,14 +16406,13 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-2074239672"/>
+        <c:crossAx val="-2101248424"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
     </c:plotArea>
     <c:legend>
       <c:legendPos val="r"/>
-      <c:layout/>
       <c:overlay val="0"/>
     </c:legend>
     <c:plotVisOnly val="1"/>
@@ -16655,11 +16618,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="-2074301624"/>
-        <c:axId val="-2074308984"/>
+        <c:axId val="-2101268872"/>
+        <c:axId val="-2101271944"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="-2074301624"/>
+        <c:axId val="-2101268872"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -16668,7 +16631,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-2074308984"/>
+        <c:crossAx val="-2101271944"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -16676,7 +16639,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="-2074308984"/>
+        <c:axId val="-2101271944"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -16687,14 +16650,13 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-2074301624"/>
+        <c:crossAx val="-2101268872"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
     </c:plotArea>
     <c:legend>
       <c:legendPos val="r"/>
-      <c:layout/>
       <c:overlay val="0"/>
     </c:legend>
     <c:plotVisOnly val="1"/>
@@ -16910,11 +16872,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="-2074369240"/>
-        <c:axId val="-2074376904"/>
+        <c:axId val="-2101302008"/>
+        <c:axId val="-2101311480"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="-2074369240"/>
+        <c:axId val="-2101302008"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -16923,7 +16885,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-2074376904"/>
+        <c:crossAx val="-2101311480"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -16931,7 +16893,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="-2074376904"/>
+        <c:axId val="-2101311480"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:min val="15.0"/>
@@ -16943,14 +16905,13 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-2074369240"/>
+        <c:crossAx val="-2101302008"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
     </c:plotArea>
     <c:legend>
       <c:legendPos val="r"/>
-      <c:layout/>
       <c:overlay val="0"/>
     </c:legend>
     <c:plotVisOnly val="1"/>
@@ -17102,11 +17063,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:gapWidth val="150"/>
-        <c:axId val="2104373112"/>
-        <c:axId val="-2088548776"/>
+        <c:axId val="-2099276072"/>
+        <c:axId val="-2099273080"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="2104373112"/>
+        <c:axId val="-2099276072"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -17115,7 +17076,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-2088548776"/>
+        <c:crossAx val="-2099273080"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -17124,7 +17085,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="-2088548776"/>
+        <c:axId val="-2099273080"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -17135,7 +17096,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="2104373112"/>
+        <c:crossAx val="-2099276072"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -17345,11 +17306,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:gapWidth val="150"/>
-        <c:axId val="-2074403224"/>
-        <c:axId val="-2074410824"/>
+        <c:axId val="-2098013192"/>
+        <c:axId val="-2098022728"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="-2074403224"/>
+        <c:axId val="-2098013192"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -17358,7 +17319,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-2074410824"/>
+        <c:crossAx val="-2098022728"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -17366,7 +17327,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="-2074410824"/>
+        <c:axId val="-2098022728"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -17377,14 +17338,13 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-2074403224"/>
+        <c:crossAx val="-2098013192"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
     </c:plotArea>
     <c:legend>
       <c:legendPos val="r"/>
-      <c:layout/>
       <c:overlay val="0"/>
     </c:legend>
     <c:plotVisOnly val="1"/>
@@ -17647,11 +17607,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="1776488824"/>
-        <c:axId val="1776491832"/>
+        <c:axId val="-2101403880"/>
+        <c:axId val="-2101400888"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="1776488824"/>
+        <c:axId val="-2101403880"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -17660,7 +17620,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="1776491832"/>
+        <c:crossAx val="-2101400888"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -17668,7 +17628,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="1776491832"/>
+        <c:axId val="-2101400888"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -17679,14 +17639,13 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="1776488824"/>
+        <c:crossAx val="-2101403880"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
     </c:plotArea>
     <c:legend>
       <c:legendPos val="r"/>
-      <c:layout/>
       <c:overlay val="0"/>
     </c:legend>
     <c:plotVisOnly val="1"/>
@@ -17959,11 +17918,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="-2121935784"/>
-        <c:axId val="1776637592"/>
+        <c:axId val="-2098484888"/>
+        <c:axId val="-2098481944"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="-2121935784"/>
+        <c:axId val="-2098484888"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -17972,7 +17931,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="1776637592"/>
+        <c:crossAx val="-2098481944"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -17980,7 +17939,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="1776637592"/>
+        <c:axId val="-2098481944"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:min val="16.5"/>
@@ -17992,14 +17951,13 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-2121935784"/>
+        <c:crossAx val="-2098484888"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
     </c:plotArea>
     <c:legend>
       <c:legendPos val="r"/>
-      <c:layout/>
       <c:overlay val="0"/>
     </c:legend>
     <c:plotVisOnly val="1"/>
@@ -18259,11 +18217,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:gapWidth val="150"/>
-        <c:axId val="1776721960"/>
-        <c:axId val="1776724968"/>
+        <c:axId val="2138862632"/>
+        <c:axId val="2138981624"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="1776721960"/>
+        <c:axId val="2138862632"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -18272,7 +18230,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="1776724968"/>
+        <c:crossAx val="2138981624"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -18280,7 +18238,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="1776724968"/>
+        <c:axId val="2138981624"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -18291,14 +18249,13 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="1776721960"/>
+        <c:crossAx val="2138862632"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
     </c:plotArea>
     <c:legend>
       <c:legendPos val="r"/>
-      <c:layout/>
       <c:overlay val="0"/>
     </c:legend>
     <c:plotVisOnly val="1"/>
@@ -20576,10 +20533,10 @@
   <sheetPr enableFormatConditionsCalculation="0">
     <tabColor rgb="FFFF0000"/>
   </sheetPr>
-  <dimension ref="A2:BR15"/>
+  <dimension ref="A2:BR16"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="BR5" sqref="BR5"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A16" sqref="A16:B16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -22056,8 +22013,26 @@
         <v>8.34</v>
       </c>
     </row>
+    <row r="16" spans="1:70">
+      <c r="A16" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="B16" s="16">
+        <v>43060</v>
+      </c>
+      <c r="C16">
+        <v>2100</v>
+      </c>
+      <c r="D16">
+        <v>8.64</v>
+      </c>
+      <c r="E16" s="1" t="s">
+        <v>73</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
   <drawing r:id="rId1"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
@@ -36234,8 +36209,8 @@
   </sheetPr>
   <dimension ref="A1:AH45"/>
   <sheetViews>
-    <sheetView topLeftCell="Z1" workbookViewId="0">
-      <selection activeCell="AH5" sqref="AH5"/>
+    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
+      <selection activeCell="A17" sqref="A17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -37247,11 +37222,21 @@
       <c r="AE15" s="10"/>
     </row>
     <row r="16" spans="1:34">
-      <c r="A16" s="10"/>
-      <c r="B16" s="10"/>
-      <c r="C16" s="10"/>
-      <c r="D16" s="36"/>
-      <c r="E16" s="37"/>
+      <c r="A16" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="B16" s="16">
+        <v>43060</v>
+      </c>
+      <c r="C16" s="10">
+        <v>300</v>
+      </c>
+      <c r="D16" s="36">
+        <v>57.62</v>
+      </c>
+      <c r="E16" s="42" t="s">
+        <v>74</v>
+      </c>
       <c r="F16" s="37"/>
       <c r="G16" s="27"/>
       <c r="H16" s="27"/>

</xml_diff>

<commit_message>
sell media buy PuBang
</commit_message>
<xml_diff>
--- a/stock.xlsx
+++ b/stock.xlsx
@@ -1,10 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="22416"/>
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="26405"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="2740" yWindow="0" windowWidth="25600" windowHeight="16060" tabRatio="996" activeTab="18"/>
+    <workbookView xWindow="2740" yWindow="0" windowWidth="25600" windowHeight="16060" tabRatio="996" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="民生银行" sheetId="13" r:id="rId1"/>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="304" uniqueCount="79">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="307" uniqueCount="81">
   <si>
     <t>达华智能</t>
   </si>
@@ -336,6 +336,12 @@
   </si>
   <si>
     <t>质押平仓，停牌</t>
+  </si>
+  <si>
+    <t>buy</t>
+  </si>
+  <si>
+    <t>亏2k多，当断则断</t>
   </si>
 </sst>
 </file>
@@ -1116,11 +1122,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="2116138216"/>
-        <c:axId val="2107332088"/>
+        <c:axId val="1780846152"/>
+        <c:axId val="1780849160"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="2116138216"/>
+        <c:axId val="1780846152"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1129,7 +1135,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="2107332088"/>
+        <c:crossAx val="1780849160"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -1137,7 +1143,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="2107332088"/>
+        <c:axId val="1780849160"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1148,14 +1154,13 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="2116138216"/>
+        <c:crossAx val="1780846152"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
     </c:plotArea>
     <c:legend>
       <c:legendPos val="r"/>
-      <c:layout/>
       <c:overlay val="0"/>
     </c:legend>
     <c:plotVisOnly val="1"/>
@@ -1454,11 +1459,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="-2018815896"/>
-        <c:axId val="-2018812888"/>
+        <c:axId val="-2089366248"/>
+        <c:axId val="-2089363240"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="-2018815896"/>
+        <c:axId val="-2089366248"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1467,7 +1472,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-2018812888"/>
+        <c:crossAx val="-2089363240"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -1475,7 +1480,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="-2018812888"/>
+        <c:axId val="-2089363240"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1486,7 +1491,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-2018815896"/>
+        <c:crossAx val="-2089366248"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -1797,11 +1802,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="-2018970856"/>
-        <c:axId val="-2018967848"/>
+        <c:axId val="1768478472"/>
+        <c:axId val="1768481480"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="-2018970856"/>
+        <c:axId val="1768478472"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1810,7 +1815,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-2018967848"/>
+        <c:crossAx val="1768481480"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -1818,7 +1823,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="-2018967848"/>
+        <c:axId val="1768481480"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:min val="4.3"/>
@@ -1830,7 +1835,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-2018970856"/>
+        <c:crossAx val="1768478472"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -2128,11 +2133,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:gapWidth val="150"/>
-        <c:axId val="-2019041832"/>
-        <c:axId val="-2019038824"/>
+        <c:axId val="1768376824"/>
+        <c:axId val="1768247880"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="-2019041832"/>
+        <c:axId val="1768376824"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2141,7 +2146,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-2019038824"/>
+        <c:crossAx val="1768247880"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -2149,7 +2154,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="-2019038824"/>
+        <c:axId val="1768247880"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2160,7 +2165,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-2019041832"/>
+        <c:crossAx val="1768376824"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -2422,11 +2427,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="-2018999304"/>
-        <c:axId val="-2018996296"/>
+        <c:axId val="-1998983960"/>
+        <c:axId val="-1998982552"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="-2018999304"/>
+        <c:axId val="-1998983960"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2435,7 +2440,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-2018996296"/>
+        <c:crossAx val="-1998982552"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -2443,7 +2448,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="-2018996296"/>
+        <c:axId val="-1998982552"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2454,7 +2459,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-2018999304"/>
+        <c:crossAx val="-1998983960"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -2726,11 +2731,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="-2019066648"/>
-        <c:axId val="-2019230264"/>
+        <c:axId val="-1998701160"/>
+        <c:axId val="-1999191480"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="-2019066648"/>
+        <c:axId val="-1998701160"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2739,7 +2744,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-2019230264"/>
+        <c:crossAx val="-1999191480"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -2747,7 +2752,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="-2019230264"/>
+        <c:axId val="-1999191480"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2758,7 +2763,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-2019066648"/>
+        <c:crossAx val="-1998701160"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -3017,11 +3022,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:gapWidth val="150"/>
-        <c:axId val="-2019209000"/>
-        <c:axId val="-2019205992"/>
+        <c:axId val="-1999189224"/>
+        <c:axId val="-1999070904"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="-2019209000"/>
+        <c:axId val="-1999189224"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3030,7 +3035,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-2019205992"/>
+        <c:crossAx val="-1999070904"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -3038,7 +3043,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="-2019205992"/>
+        <c:axId val="-1999070904"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3049,7 +3054,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-2019209000"/>
+        <c:crossAx val="-1999189224"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -3350,11 +3355,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="-2019163496"/>
-        <c:axId val="-2019160488"/>
+        <c:axId val="-1999120728"/>
+        <c:axId val="-1999098728"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="-2019163496"/>
+        <c:axId val="-1999120728"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3363,7 +3368,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-2019160488"/>
+        <c:crossAx val="-1999098728"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -3371,7 +3376,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="-2019160488"/>
+        <c:axId val="-1999098728"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3382,7 +3387,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-2019163496"/>
+        <c:crossAx val="-1999120728"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -3693,11 +3698,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="-2019114408"/>
-        <c:axId val="-2019111400"/>
+        <c:axId val="-1998782952"/>
+        <c:axId val="-1998881768"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="-2019114408"/>
+        <c:axId val="-1998782952"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3706,7 +3711,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-2019111400"/>
+        <c:crossAx val="-1998881768"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -3714,7 +3719,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="-2019111400"/>
+        <c:axId val="-1998881768"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3725,7 +3730,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-2019114408"/>
+        <c:crossAx val="-1998782952"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -4023,11 +4028,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:gapWidth val="150"/>
-        <c:axId val="-2019089512"/>
-        <c:axId val="-2019086504"/>
+        <c:axId val="-1998891048"/>
+        <c:axId val="-1998900872"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="-2019089512"/>
+        <c:axId val="-1998891048"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -4036,7 +4041,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-2019086504"/>
+        <c:crossAx val="-1998900872"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -4044,7 +4049,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="-2019086504"/>
+        <c:axId val="-1998900872"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -4055,7 +4060,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-2019089512"/>
+        <c:crossAx val="-1998891048"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -4356,11 +4361,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="-2020097368"/>
-        <c:axId val="-2020094360"/>
+        <c:axId val="-1998977512"/>
+        <c:axId val="-1998974504"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="-2020097368"/>
+        <c:axId val="-1998977512"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -4369,7 +4374,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-2020094360"/>
+        <c:crossAx val="-1998974504"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -4377,7 +4382,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="-2020094360"/>
+        <c:axId val="-1998974504"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -4388,7 +4393,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-2020097368"/>
+        <c:crossAx val="-1998977512"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -4699,11 +4704,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="-2020380488"/>
-        <c:axId val="-2020377544"/>
+        <c:axId val="1780933832"/>
+        <c:axId val="1781294424"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="-2020380488"/>
+        <c:axId val="1780933832"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -4712,7 +4717,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-2020377544"/>
+        <c:crossAx val="1781294424"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -4720,7 +4725,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="-2020377544"/>
+        <c:axId val="1781294424"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -4731,14 +4736,13 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-2020380488"/>
+        <c:crossAx val="1780933832"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
     </c:plotArea>
     <c:legend>
       <c:legendPos val="r"/>
-      <c:layout/>
       <c:overlay val="0"/>
     </c:legend>
     <c:plotVisOnly val="1"/>
@@ -5047,11 +5051,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="-2020049496"/>
-        <c:axId val="-2020046488"/>
+        <c:axId val="-2092867064"/>
+        <c:axId val="-2092864056"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="-2020049496"/>
+        <c:axId val="-2092867064"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -5060,7 +5064,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-2020046488"/>
+        <c:crossAx val="-2092864056"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -5068,7 +5072,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="-2020046488"/>
+        <c:axId val="-2092864056"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:min val="6.5"/>
@@ -5080,7 +5084,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-2020049496"/>
+        <c:crossAx val="-2092867064"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -5378,11 +5382,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:gapWidth val="150"/>
-        <c:axId val="-2020024952"/>
-        <c:axId val="-2020021928"/>
+        <c:axId val="-2092842616"/>
+        <c:axId val="-2092839608"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="-2020024952"/>
+        <c:axId val="-2092842616"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -5391,7 +5395,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-2020021928"/>
+        <c:crossAx val="-2092839608"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -5399,7 +5403,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="-2020021928"/>
+        <c:axId val="-2092839608"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -5410,7 +5414,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-2020024952"/>
+        <c:crossAx val="-2092842616"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -5711,11 +5715,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="-2019980328"/>
-        <c:axId val="-2019977320"/>
+        <c:axId val="-2092797944"/>
+        <c:axId val="-2092794936"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="-2019980328"/>
+        <c:axId val="-2092797944"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -5724,7 +5728,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-2019977320"/>
+        <c:crossAx val="-2092794936"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -5732,7 +5736,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="-2019977320"/>
+        <c:axId val="-2092794936"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -5743,7 +5747,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-2019980328"/>
+        <c:crossAx val="-2092797944"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -6054,11 +6058,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="-2019932456"/>
-        <c:axId val="-2019929448"/>
+        <c:axId val="-2092674328"/>
+        <c:axId val="-2092671352"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="-2019932456"/>
+        <c:axId val="-2092674328"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -6067,7 +6071,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-2019929448"/>
+        <c:crossAx val="-2092671352"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -6075,7 +6079,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="-2019929448"/>
+        <c:axId val="-2092671352"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:min val="9.0"/>
@@ -6087,7 +6091,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-2019932456"/>
+        <c:crossAx val="-2092674328"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -6385,11 +6389,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:gapWidth val="150"/>
-        <c:axId val="-2019908024"/>
-        <c:axId val="-2019905000"/>
+        <c:axId val="-2092653496"/>
+        <c:axId val="-2092650488"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="-2019908024"/>
+        <c:axId val="-2092653496"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -6398,7 +6402,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-2019905000"/>
+        <c:crossAx val="-2092650488"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -6406,7 +6410,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="-2019905000"/>
+        <c:axId val="-2092650488"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -6417,7 +6421,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-2019908024"/>
+        <c:crossAx val="-2092653496"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -6718,11 +6722,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="-2019863736"/>
-        <c:axId val="-2019860728"/>
+        <c:axId val="-1999571752"/>
+        <c:axId val="-1999623960"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="-2019863736"/>
+        <c:axId val="-1999571752"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -6731,7 +6735,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-2019860728"/>
+        <c:crossAx val="-1999623960"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -6739,7 +6743,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="-2019860728"/>
+        <c:axId val="-1999623960"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -6750,7 +6754,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-2019863736"/>
+        <c:crossAx val="-1999571752"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -7061,11 +7065,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="-2019815864"/>
-        <c:axId val="-2019812856"/>
+        <c:axId val="-2092735016"/>
+        <c:axId val="-2092762296"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="-2019815864"/>
+        <c:axId val="-2092735016"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -7074,7 +7078,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-2019812856"/>
+        <c:crossAx val="-2092762296"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -7082,7 +7086,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="-2019812856"/>
+        <c:axId val="-2092762296"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:min val="10.0"/>
@@ -7094,7 +7098,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-2019815864"/>
+        <c:crossAx val="-2092735016"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -7392,11 +7396,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:gapWidth val="150"/>
-        <c:axId val="-2019791432"/>
-        <c:axId val="-2019788408"/>
+        <c:axId val="-2092731432"/>
+        <c:axId val="-2092728424"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="-2019791432"/>
+        <c:axId val="-2092731432"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -7405,7 +7409,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-2019788408"/>
+        <c:crossAx val="-2092728424"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -7413,7 +7417,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="-2019788408"/>
+        <c:axId val="-2092728424"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -7424,7 +7428,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-2019791432"/>
+        <c:crossAx val="-2092731432"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -7725,11 +7729,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="-2019747000"/>
-        <c:axId val="-2019743992"/>
+        <c:axId val="1768118440"/>
+        <c:axId val="1768121192"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="-2019747000"/>
+        <c:axId val="1768118440"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -7738,7 +7742,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-2019743992"/>
+        <c:crossAx val="1768121192"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -7746,7 +7750,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="-2019743992"/>
+        <c:axId val="1768121192"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -7757,7 +7761,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-2019747000"/>
+        <c:crossAx val="1768118440"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -8068,11 +8072,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="-2019698680"/>
-        <c:axId val="-2019695656"/>
+        <c:axId val="2139033688"/>
+        <c:axId val="2139036696"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="-2019698680"/>
+        <c:axId val="2139033688"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -8081,7 +8085,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-2019695656"/>
+        <c:crossAx val="2139036696"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -8089,7 +8093,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="-2019695656"/>
+        <c:axId val="2139036696"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -8100,7 +8104,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-2019698680"/>
+        <c:crossAx val="2139033688"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -8398,11 +8402,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:gapWidth val="150"/>
-        <c:axId val="-2020355208"/>
-        <c:axId val="-2020352264"/>
+        <c:axId val="1781221176"/>
+        <c:axId val="1781224120"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="-2020355208"/>
+        <c:axId val="1781221176"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -8411,7 +8415,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-2020352264"/>
+        <c:crossAx val="1781224120"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -8419,7 +8423,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="-2020352264"/>
+        <c:axId val="1781224120"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -8430,14 +8434,13 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-2020355208"/>
+        <c:crossAx val="1781221176"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
     </c:plotArea>
     <c:legend>
       <c:legendPos val="r"/>
-      <c:layout/>
       <c:overlay val="0"/>
     </c:legend>
     <c:plotVisOnly val="1"/>
@@ -8733,11 +8736,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:gapWidth val="150"/>
-        <c:axId val="-2019674136"/>
-        <c:axId val="-2019671112"/>
+        <c:axId val="1768660504"/>
+        <c:axId val="2060507544"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="-2019674136"/>
+        <c:axId val="1768660504"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -8746,7 +8749,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-2019671112"/>
+        <c:crossAx val="2060507544"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -8754,7 +8757,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="-2019671112"/>
+        <c:axId val="2060507544"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -8765,7 +8768,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-2019674136"/>
+        <c:crossAx val="1768660504"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -9066,11 +9069,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="-2019296392"/>
-        <c:axId val="-2019293384"/>
+        <c:axId val="-2089545656"/>
+        <c:axId val="1768264632"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="-2019296392"/>
+        <c:axId val="-2089545656"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -9079,7 +9082,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-2019293384"/>
+        <c:crossAx val="1768264632"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -9087,7 +9090,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="-2019293384"/>
+        <c:axId val="1768264632"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -9098,7 +9101,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-2019296392"/>
+        <c:crossAx val="-2089545656"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -9409,11 +9412,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="-2019665608"/>
-        <c:axId val="-2019662552"/>
+        <c:axId val="-2089563832"/>
+        <c:axId val="-2089405048"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="-2019665608"/>
+        <c:axId val="-2089563832"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -9422,7 +9425,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-2019662552"/>
+        <c:crossAx val="-2089405048"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -9430,7 +9433,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="-2019662552"/>
+        <c:axId val="-2089405048"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:min val="5.0"/>
@@ -9442,7 +9445,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-2019665608"/>
+        <c:crossAx val="-2089563832"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -9740,11 +9743,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:gapWidth val="150"/>
-        <c:axId val="-2019636808"/>
-        <c:axId val="-2019633784"/>
+        <c:axId val="-2101213128"/>
+        <c:axId val="2058087176"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="-2019636808"/>
+        <c:axId val="-2101213128"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -9753,7 +9756,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-2019633784"/>
+        <c:crossAx val="2058087176"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -9761,7 +9764,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="-2019633784"/>
+        <c:axId val="2058087176"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -9772,7 +9775,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-2019636808"/>
+        <c:crossAx val="-2101213128"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -10073,11 +10076,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="2111065000"/>
-        <c:axId val="2111147048"/>
+        <c:axId val="-2092689496"/>
+        <c:axId val="-2092024424"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="2111065000"/>
+        <c:axId val="-2092689496"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -10086,7 +10089,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="2111147048"/>
+        <c:crossAx val="-2092024424"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -10094,7 +10097,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="2111147048"/>
+        <c:axId val="-2092024424"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -10105,7 +10108,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="2111065000"/>
+        <c:crossAx val="-2092689496"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -10416,11 +10419,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="2081733816"/>
-        <c:axId val="-2064679864"/>
+        <c:axId val="-2091982456"/>
+        <c:axId val="-2091979448"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="2081733816"/>
+        <c:axId val="-2091982456"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -10429,7 +10432,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-2064679864"/>
+        <c:crossAx val="-2091979448"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -10437,7 +10440,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="-2064679864"/>
+        <c:axId val="-2091979448"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -10448,7 +10451,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="2081733816"/>
+        <c:crossAx val="-2091982456"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -10746,11 +10749,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:gapWidth val="150"/>
-        <c:axId val="-2064664808"/>
-        <c:axId val="2111156664"/>
+        <c:axId val="-2092663560"/>
+        <c:axId val="-2091960824"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="-2064664808"/>
+        <c:axId val="-2092663560"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -10759,7 +10762,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="2111156664"/>
+        <c:crossAx val="-2091960824"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -10767,7 +10770,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="2111156664"/>
+        <c:axId val="-2091960824"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -10778,7 +10781,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-2064664808"/>
+        <c:crossAx val="-2092663560"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -11079,11 +11082,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="2087654904"/>
-        <c:axId val="2111057640"/>
+        <c:axId val="-2092392712"/>
+        <c:axId val="-2092373784"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="2087654904"/>
+        <c:axId val="-2092392712"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -11092,7 +11095,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="2111057640"/>
+        <c:crossAx val="-2092373784"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -11100,7 +11103,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="2111057640"/>
+        <c:axId val="-2092373784"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -11111,7 +11114,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="2087654904"/>
+        <c:crossAx val="-2092392712"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -11422,11 +11425,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="-2018729912"/>
-        <c:axId val="-2018726888"/>
+        <c:axId val="-2092383528"/>
+        <c:axId val="-2092380520"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="-2018729912"/>
+        <c:axId val="-2092383528"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -11435,7 +11438,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-2018726888"/>
+        <c:crossAx val="-2092380520"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -11443,7 +11446,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="-2018726888"/>
+        <c:axId val="-2092380520"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:min val="3.0"/>
@@ -11455,7 +11458,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-2018729912"/>
+        <c:crossAx val="-2092383528"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -11753,11 +11756,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:gapWidth val="150"/>
-        <c:axId val="-2018705448"/>
-        <c:axId val="-2018702424"/>
+        <c:axId val="-2092904616"/>
+        <c:axId val="-2092912536"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="-2018705448"/>
+        <c:axId val="-2092904616"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -11766,7 +11769,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-2018702424"/>
+        <c:crossAx val="-2092912536"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -11774,7 +11777,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="-2018702424"/>
+        <c:axId val="-2092912536"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -11785,7 +11788,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-2018705448"/>
+        <c:crossAx val="-2092904616"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -11978,11 +11981,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="-2020317304"/>
-        <c:axId val="-2020314360"/>
+        <c:axId val="1780521992"/>
+        <c:axId val="1780524936"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="-2020317304"/>
+        <c:axId val="1780521992"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -11991,7 +11994,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-2020314360"/>
+        <c:crossAx val="1780524936"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -12000,7 +12003,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="-2020314360"/>
+        <c:axId val="1780524936"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -12011,7 +12014,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-2020317304"/>
+        <c:crossAx val="1780521992"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -12312,11 +12315,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="-2018661192"/>
-        <c:axId val="-2018658184"/>
+        <c:axId val="2136105784"/>
+        <c:axId val="1768032072"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="-2018661192"/>
+        <c:axId val="2136105784"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -12325,7 +12328,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-2018658184"/>
+        <c:crossAx val="1768032072"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -12333,7 +12336,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="-2018658184"/>
+        <c:axId val="1768032072"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -12344,7 +12347,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-2018661192"/>
+        <c:crossAx val="2136105784"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -12655,11 +12658,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="-2018613320"/>
-        <c:axId val="-2018610312"/>
+        <c:axId val="2136102520"/>
+        <c:axId val="-2089361144"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="-2018613320"/>
+        <c:axId val="2136102520"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -12668,7 +12671,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-2018610312"/>
+        <c:crossAx val="-2089361144"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -12676,7 +12679,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="-2018610312"/>
+        <c:axId val="-2089361144"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -12687,7 +12690,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-2018613320"/>
+        <c:crossAx val="2136102520"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -12985,11 +12988,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:gapWidth val="150"/>
-        <c:axId val="-2018588888"/>
-        <c:axId val="-2018585864"/>
+        <c:axId val="-2089378536"/>
+        <c:axId val="2060615032"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="-2018588888"/>
+        <c:axId val="-2089378536"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -12998,7 +13001,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-2018585864"/>
+        <c:crossAx val="2060615032"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -13006,7 +13009,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="-2018585864"/>
+        <c:axId val="2060615032"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -13017,7 +13020,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-2018588888"/>
+        <c:crossAx val="-2089378536"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -13318,11 +13321,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="-2018544456"/>
-        <c:axId val="-2018541448"/>
+        <c:axId val="-2101260584"/>
+        <c:axId val="-2101257576"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="-2018544456"/>
+        <c:axId val="-2101260584"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -13331,7 +13334,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-2018541448"/>
+        <c:crossAx val="-2101257576"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -13339,7 +13342,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="-2018541448"/>
+        <c:axId val="-2101257576"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -13350,7 +13353,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-2018544456"/>
+        <c:crossAx val="-2101260584"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -13661,11 +13664,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="-2019355800"/>
-        <c:axId val="-2019364664"/>
+        <c:axId val="-2101205992"/>
+        <c:axId val="2058110584"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="-2019355800"/>
+        <c:axId val="-2101205992"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -13674,7 +13677,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-2019364664"/>
+        <c:crossAx val="2058110584"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -13682,7 +13685,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="-2019364664"/>
+        <c:axId val="2058110584"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:min val="8.0"/>
@@ -13694,7 +13697,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-2019355800"/>
+        <c:crossAx val="-2101205992"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -13992,11 +13995,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:gapWidth val="150"/>
-        <c:axId val="-2019380424"/>
-        <c:axId val="-2019389080"/>
+        <c:axId val="-2104825704"/>
+        <c:axId val="2037332264"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="-2019380424"/>
+        <c:axId val="-2104825704"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -14005,7 +14008,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-2019389080"/>
+        <c:crossAx val="2037332264"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -14013,7 +14016,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="-2019389080"/>
+        <c:axId val="2037332264"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -14024,7 +14027,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-2019380424"/>
+        <c:crossAx val="-2104825704"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -14325,11 +14328,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="-2019425080"/>
-        <c:axId val="-2019433896"/>
+        <c:axId val="-2089409880"/>
+        <c:axId val="-2089317160"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="-2019425080"/>
+        <c:axId val="-2089409880"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -14338,7 +14341,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-2019433896"/>
+        <c:crossAx val="-2089317160"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -14346,7 +14349,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="-2019433896"/>
+        <c:axId val="-2089317160"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -14357,7 +14360,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-2019425080"/>
+        <c:crossAx val="-2089409880"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -14668,11 +14671,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="-2019472888"/>
-        <c:axId val="-2019481752"/>
+        <c:axId val="1768267816"/>
+        <c:axId val="1768270824"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="-2019472888"/>
+        <c:axId val="1768267816"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -14681,7 +14684,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-2019481752"/>
+        <c:crossAx val="1768270824"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -14689,7 +14692,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="-2019481752"/>
+        <c:axId val="1768270824"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -14700,7 +14703,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-2019472888"/>
+        <c:crossAx val="1768267816"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -14998,11 +15001,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:gapWidth val="150"/>
-        <c:axId val="-2019497512"/>
-        <c:axId val="-2019506168"/>
+        <c:axId val="1768163656"/>
+        <c:axId val="1768166632"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="-2019497512"/>
+        <c:axId val="1768163656"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -15011,7 +15014,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-2019506168"/>
+        <c:crossAx val="1768166632"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -15019,7 +15022,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="-2019506168"/>
+        <c:axId val="1768166632"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -15030,7 +15033,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-2019497512"/>
+        <c:crossAx val="1768163656"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -15331,11 +15334,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="-2019541608"/>
-        <c:axId val="-2019550424"/>
+        <c:axId val="1767933864"/>
+        <c:axId val="1768067928"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="-2019541608"/>
+        <c:axId val="1767933864"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -15344,7 +15347,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-2019550424"/>
+        <c:crossAx val="1768067928"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -15352,7 +15355,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="-2019550424"/>
+        <c:axId val="1768067928"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -15363,7 +15366,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-2019541608"/>
+        <c:crossAx val="1767933864"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -15566,11 +15569,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="-2020269384"/>
-        <c:axId val="-2020266440"/>
+        <c:axId val="1781504968"/>
+        <c:axId val="1781440152"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="-2020269384"/>
+        <c:axId val="1781504968"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -15579,7 +15582,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-2020266440"/>
+        <c:crossAx val="1781440152"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -15588,7 +15591,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="-2020266440"/>
+        <c:axId val="1781440152"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:min val="40.0"/>
@@ -15600,7 +15603,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-2020269384"/>
+        <c:crossAx val="1781504968"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -15911,11 +15914,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="-2033785784"/>
-        <c:axId val="-2033243432"/>
+        <c:axId val="2138851816"/>
+        <c:axId val="2138854824"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="-2033785784"/>
+        <c:axId val="2138851816"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -15924,7 +15927,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-2033243432"/>
+        <c:crossAx val="2138854824"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -15932,7 +15935,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="-2033243432"/>
+        <c:axId val="2138854824"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:min val="4.5"/>
@@ -15944,7 +15947,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-2033785784"/>
+        <c:crossAx val="2138851816"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -16242,11 +16245,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:gapWidth val="150"/>
-        <c:axId val="-2033222376"/>
-        <c:axId val="-2033219368"/>
+        <c:axId val="2060454680"/>
+        <c:axId val="2061022568"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="-2033222376"/>
+        <c:axId val="2060454680"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -16255,7 +16258,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-2033219368"/>
+        <c:crossAx val="2061022568"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -16263,7 +16266,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="-2033219368"/>
+        <c:axId val="2061022568"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -16274,7 +16277,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-2033222376"/>
+        <c:crossAx val="2060454680"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -16533,11 +16536,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="-2033280344"/>
-        <c:axId val="-2033284056"/>
+        <c:axId val="1768091992"/>
+        <c:axId val="1767909240"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="-2033280344"/>
+        <c:axId val="1768091992"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -16546,7 +16549,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-2033284056"/>
+        <c:crossAx val="1767909240"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -16554,7 +16557,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="-2033284056"/>
+        <c:axId val="1767909240"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -16565,7 +16568,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-2033280344"/>
+        <c:crossAx val="1768091992"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -16834,11 +16837,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="-2033336200"/>
-        <c:axId val="-2033342968"/>
+        <c:axId val="1768014328"/>
+        <c:axId val="1767900984"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="-2033336200"/>
+        <c:axId val="1768014328"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -16847,7 +16850,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-2033342968"/>
+        <c:crossAx val="1767900984"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -16855,7 +16858,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="-2033342968"/>
+        <c:axId val="1767900984"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:min val="450.0"/>
@@ -16867,7 +16870,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-2033336200"/>
+        <c:crossAx val="1768014328"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -17123,11 +17126,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:gapWidth val="150"/>
-        <c:axId val="-2033383272"/>
-        <c:axId val="-2033380264"/>
+        <c:axId val="1768276072"/>
+        <c:axId val="1768279080"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="-2033383272"/>
+        <c:axId val="1768276072"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -17136,7 +17139,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-2033380264"/>
+        <c:crossAx val="1768279080"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -17144,7 +17147,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="-2033380264"/>
+        <c:axId val="1768279080"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -17155,7 +17158,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-2033383272"/>
+        <c:crossAx val="1768276072"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -17399,11 +17402,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="-2033411048"/>
-        <c:axId val="-2033417048"/>
+        <c:axId val="1768624072"/>
+        <c:axId val="1768627080"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="-2033411048"/>
+        <c:axId val="1768624072"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -17412,7 +17415,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-2033417048"/>
+        <c:crossAx val="1768627080"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -17420,7 +17423,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="-2033417048"/>
+        <c:axId val="1768627080"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -17431,7 +17434,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-2033411048"/>
+        <c:crossAx val="1768624072"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -17685,11 +17688,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="-2033475464"/>
-        <c:axId val="-2033472456"/>
+        <c:axId val="1768303256"/>
+        <c:axId val="1768261320"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="-2033475464"/>
+        <c:axId val="1768303256"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -17698,7 +17701,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-2033472456"/>
+        <c:crossAx val="1768261320"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -17706,7 +17709,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="-2033472456"/>
+        <c:axId val="1768261320"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:min val="15.0"/>
@@ -17718,7 +17721,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-2033475464"/>
+        <c:crossAx val="1768303256"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -17959,11 +17962,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:gapWidth val="150"/>
-        <c:axId val="-2033492168"/>
-        <c:axId val="-2033496120"/>
+        <c:axId val="1768099464"/>
+        <c:axId val="1768102472"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="-2033492168"/>
+        <c:axId val="1768099464"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -17972,7 +17975,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-2033496120"/>
+        <c:crossAx val="1768102472"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -17980,7 +17983,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="-2033496120"/>
+        <c:axId val="1768102472"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -17991,7 +17994,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-2033492168"/>
+        <c:crossAx val="1768099464"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -18289,11 +18292,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="-2019586056"/>
-        <c:axId val="-2019583048"/>
+        <c:axId val="1768546488"/>
+        <c:axId val="1768549496"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="-2019586056"/>
+        <c:axId val="1768546488"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -18302,7 +18305,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-2019583048"/>
+        <c:crossAx val="1768549496"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -18310,7 +18313,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="-2019583048"/>
+        <c:axId val="1768549496"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -18321,7 +18324,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-2019586056"/>
+        <c:crossAx val="1768546488"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -18629,11 +18632,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="-2020411752"/>
-        <c:axId val="-2020420552"/>
+        <c:axId val="1768620504"/>
+        <c:axId val="1768613976"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="-2020411752"/>
+        <c:axId val="1768620504"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -18642,7 +18645,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-2020420552"/>
+        <c:crossAx val="1768613976"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -18650,7 +18653,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="-2020420552"/>
+        <c:axId val="1768613976"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:min val="6.0"/>
@@ -18662,7 +18665,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-2020411752"/>
+        <c:crossAx val="1768620504"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -18852,11 +18855,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:gapWidth val="150"/>
-        <c:axId val="-2020245016"/>
-        <c:axId val="-2020241992"/>
+        <c:axId val="1781489864"/>
+        <c:axId val="2055356680"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="-2020245016"/>
+        <c:axId val="1781489864"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -18865,7 +18868,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-2020241992"/>
+        <c:crossAx val="2055356680"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -18874,7 +18877,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="-2020241992"/>
+        <c:axId val="2055356680"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -18885,7 +18888,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-2020245016"/>
+        <c:crossAx val="1781489864"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -19180,11 +19183,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:gapWidth val="150"/>
-        <c:axId val="-2020436344"/>
-        <c:axId val="-2020445000"/>
+        <c:axId val="1768710088"/>
+        <c:axId val="1768713096"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="-2020436344"/>
+        <c:axId val="1768710088"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -19193,7 +19196,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-2020445000"/>
+        <c:crossAx val="1768713096"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -19201,7 +19204,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="-2020445000"/>
+        <c:axId val="1768713096"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -19212,7 +19215,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-2020436344"/>
+        <c:crossAx val="1768710088"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -19510,11 +19513,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="-2020200728"/>
-        <c:axId val="-2020197720"/>
+        <c:axId val="-2089348072"/>
+        <c:axId val="1768605912"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="-2020200728"/>
+        <c:axId val="-2089348072"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -19523,7 +19526,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-2020197720"/>
+        <c:crossAx val="1768605912"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -19531,7 +19534,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="-2020197720"/>
+        <c:axId val="1768605912"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -19542,7 +19545,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-2020200728"/>
+        <c:crossAx val="-2089348072"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -19850,11 +19853,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="-2020152968"/>
-        <c:axId val="-2020149944"/>
+        <c:axId val="1768649416"/>
+        <c:axId val="1768448936"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="-2020152968"/>
+        <c:axId val="1768649416"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -19863,7 +19866,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-2020149944"/>
+        <c:crossAx val="1768448936"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -19871,7 +19874,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="-2020149944"/>
+        <c:axId val="1768448936"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:min val="16.5"/>
@@ -19883,7 +19886,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-2020152968"/>
+        <c:crossAx val="1768649416"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -20178,11 +20181,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:gapWidth val="150"/>
-        <c:axId val="-2020127608"/>
-        <c:axId val="-2020124584"/>
+        <c:axId val="1768368488"/>
+        <c:axId val="1768424536"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="-2020127608"/>
+        <c:axId val="1768368488"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -20191,7 +20194,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-2020124584"/>
+        <c:crossAx val="1768424536"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -20199,7 +20202,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="-2020124584"/>
+        <c:axId val="1768424536"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -20210,7 +20213,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-2020127608"/>
+        <c:crossAx val="1768368488"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -39369,7 +39372,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A2:BK13"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="AV1" workbookViewId="0">
+    <sheetView topLeftCell="AV1" workbookViewId="0">
       <selection activeCell="BK7" sqref="BK7"/>
     </sheetView>
   </sheetViews>
@@ -40670,8 +40673,8 @@
   </sheetPr>
   <dimension ref="A1:AT45"/>
   <sheetViews>
-    <sheetView topLeftCell="A9" workbookViewId="0">
-      <selection activeCell="AT7" sqref="AT7"/>
+    <sheetView tabSelected="1" topLeftCell="A8" workbookViewId="0">
+      <selection activeCell="E18" sqref="E18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -41960,11 +41963,21 @@
       <c r="AE16" s="10"/>
     </row>
     <row r="17" spans="1:31">
-      <c r="A17" s="10"/>
-      <c r="B17" s="10"/>
-      <c r="C17" s="10"/>
-      <c r="D17" s="36"/>
-      <c r="E17" s="27"/>
+      <c r="A17" s="10" t="s">
+        <v>71</v>
+      </c>
+      <c r="B17" s="9">
+        <v>43076</v>
+      </c>
+      <c r="C17" s="10">
+        <v>300</v>
+      </c>
+      <c r="D17" s="36">
+        <v>49.59</v>
+      </c>
+      <c r="E17" s="29" t="s">
+        <v>80</v>
+      </c>
       <c r="F17" s="27"/>
       <c r="G17" s="27"/>
       <c r="H17" s="27"/>
@@ -48088,10 +48101,10 @@
   <sheetPr enableFormatConditionsCalculation="0">
     <tabColor rgb="FFFFFF00"/>
   </sheetPr>
-  <dimension ref="A2:BQ14"/>
+  <dimension ref="A2:BQ15"/>
   <sheetViews>
-    <sheetView topLeftCell="A16" workbookViewId="0">
-      <selection activeCell="BQ7" sqref="BQ7"/>
+    <sheetView topLeftCell="A2" workbookViewId="0">
+      <selection activeCell="B16" sqref="B16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -49517,6 +49530,20 @@
       </c>
       <c r="E14">
         <v>-7040</v>
+      </c>
+    </row>
+    <row r="15" spans="1:69">
+      <c r="A15" t="s">
+        <v>79</v>
+      </c>
+      <c r="B15" s="2">
+        <v>43076</v>
+      </c>
+      <c r="C15">
+        <v>4000</v>
+      </c>
+      <c r="D15">
+        <v>5.53</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
update stock marketing quantity
</commit_message>
<xml_diff>
--- a/stock.xlsx
+++ b/stock.xlsx
@@ -1210,11 +1210,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="-2011499976"/>
-        <c:axId val="-2011258600"/>
+        <c:axId val="2110447336"/>
+        <c:axId val="2110694968"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="-2011499976"/>
+        <c:axId val="2110447336"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1223,7 +1223,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-2011258600"/>
+        <c:crossAx val="2110694968"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -1231,7 +1231,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="-2011258600"/>
+        <c:axId val="2110694968"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1242,13 +1242,14 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-2011499976"/>
+        <c:crossAx val="2110447336"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
     </c:plotArea>
     <c:legend>
       <c:legendPos val="r"/>
+      <c:layout/>
       <c:overlay val="0"/>
     </c:legend>
     <c:plotVisOnly val="1"/>
@@ -1616,11 +1617,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="2100087272"/>
-        <c:axId val="2100052072"/>
+        <c:axId val="2109757960"/>
+        <c:axId val="2109760968"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="2100087272"/>
+        <c:axId val="2109757960"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1629,7 +1630,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="2100052072"/>
+        <c:crossAx val="2109760968"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -1637,7 +1638,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="2100052072"/>
+        <c:axId val="2109760968"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1648,7 +1649,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="2100087272"/>
+        <c:crossAx val="2109757960"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -2028,11 +2029,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="2100130056"/>
-        <c:axId val="2099651192"/>
+        <c:axId val="2109814776"/>
+        <c:axId val="2109793208"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="2100130056"/>
+        <c:axId val="2109814776"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2041,7 +2042,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="2099651192"/>
+        <c:crossAx val="2109793208"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -2049,7 +2050,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="2099651192"/>
+        <c:axId val="2109793208"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:min val="4.3"/>
@@ -2061,7 +2062,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="2100130056"/>
+        <c:crossAx val="2109814776"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -2428,11 +2429,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:gapWidth val="150"/>
-        <c:axId val="2099860312"/>
-        <c:axId val="2099662904"/>
+        <c:axId val="2109837352"/>
+        <c:axId val="2109854808"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="2099860312"/>
+        <c:axId val="2109837352"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2441,7 +2442,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="2099662904"/>
+        <c:crossAx val="2109854808"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -2449,7 +2450,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="2099662904"/>
+        <c:axId val="2109854808"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2460,7 +2461,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="2099860312"/>
+        <c:crossAx val="2109837352"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -2791,11 +2792,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="-2072136232"/>
-        <c:axId val="-2072026008"/>
+        <c:axId val="2109832328"/>
+        <c:axId val="2110071720"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="-2072136232"/>
+        <c:axId val="2109832328"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2804,7 +2805,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-2072026008"/>
+        <c:crossAx val="2110071720"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -2812,7 +2813,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="-2072026008"/>
+        <c:axId val="2110071720"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2823,7 +2824,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-2072136232"/>
+        <c:crossAx val="2109832328"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -3164,11 +3165,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="-2072553160"/>
-        <c:axId val="-2072559352"/>
+        <c:axId val="2110047960"/>
+        <c:axId val="2109988920"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="-2072553160"/>
+        <c:axId val="2110047960"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3177,7 +3178,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-2072559352"/>
+        <c:crossAx val="2109988920"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -3185,7 +3186,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="-2072559352"/>
+        <c:axId val="2109988920"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3196,7 +3197,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-2072553160"/>
+        <c:crossAx val="2110047960"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -3524,11 +3525,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:gapWidth val="150"/>
-        <c:axId val="-2072930152"/>
-        <c:axId val="-2072316888"/>
+        <c:axId val="2109977416"/>
+        <c:axId val="2109938696"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="-2072930152"/>
+        <c:axId val="2109977416"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3537,7 +3538,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-2072316888"/>
+        <c:crossAx val="2109938696"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -3545,7 +3546,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="-2072316888"/>
+        <c:axId val="2109938696"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3556,7 +3557,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-2072930152"/>
+        <c:crossAx val="2109977416"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -3926,11 +3927,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="-2072979800"/>
-        <c:axId val="-2072993992"/>
+        <c:axId val="2110196760"/>
+        <c:axId val="2110166488"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="-2072979800"/>
+        <c:axId val="2110196760"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3939,7 +3940,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-2072993992"/>
+        <c:crossAx val="2110166488"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -3947,7 +3948,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="-2072993992"/>
+        <c:axId val="2110166488"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3958,7 +3959,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-2072979800"/>
+        <c:crossAx val="2110196760"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -4338,11 +4339,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="-2072084264"/>
-        <c:axId val="-2072107976"/>
+        <c:axId val="2110188968"/>
+        <c:axId val="2110255784"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="-2072084264"/>
+        <c:axId val="2110188968"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -4351,7 +4352,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-2072107976"/>
+        <c:crossAx val="2110255784"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -4359,9 +4360,10 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="-2072107976"/>
+        <c:axId val="2110255784"/>
         <c:scaling>
           <c:orientation val="minMax"/>
+          <c:min val="5.0"/>
         </c:scaling>
         <c:delete val="0"/>
         <c:axPos val="l"/>
@@ -4370,7 +4372,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-2072084264"/>
+        <c:crossAx val="2110188968"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -4737,11 +4739,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:gapWidth val="150"/>
-        <c:axId val="2067601608"/>
-        <c:axId val="-2072231752"/>
+        <c:axId val="2110363336"/>
+        <c:axId val="2110212504"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="2067601608"/>
+        <c:axId val="2110363336"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -4750,7 +4752,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-2072231752"/>
+        <c:crossAx val="2110212504"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -4758,7 +4760,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="-2072231752"/>
+        <c:axId val="2110212504"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -4769,7 +4771,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="2067601608"/>
+        <c:crossAx val="2110363336"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -5139,11 +5141,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="-2072899176"/>
-        <c:axId val="-2072636648"/>
+        <c:axId val="2110642152"/>
+        <c:axId val="2110497400"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="-2072899176"/>
+        <c:axId val="2110642152"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -5152,7 +5154,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-2072636648"/>
+        <c:crossAx val="2110497400"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -5160,7 +5162,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="-2072636648"/>
+        <c:axId val="2110497400"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -5171,7 +5173,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-2072899176"/>
+        <c:crossAx val="2110642152"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -5551,11 +5553,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="2099841064"/>
-        <c:axId val="2099997608"/>
+        <c:axId val="2110357240"/>
+        <c:axId val="-2073023992"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="2099841064"/>
+        <c:axId val="2110357240"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -5564,7 +5566,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="2099997608"/>
+        <c:crossAx val="-2073023992"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -5572,7 +5574,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="2099997608"/>
+        <c:axId val="-2073023992"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -5583,13 +5585,14 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="2099841064"/>
+        <c:crossAx val="2110357240"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
     </c:plotArea>
     <c:legend>
       <c:legendPos val="r"/>
+      <c:layout/>
       <c:overlay val="0"/>
     </c:legend>
     <c:plotVisOnly val="1"/>
@@ -5967,11 +5970,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="-2072569192"/>
-        <c:axId val="-2072412440"/>
+        <c:axId val="-2072023656"/>
+        <c:axId val="2110748552"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="-2072569192"/>
+        <c:axId val="-2072023656"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -5980,7 +5983,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-2072412440"/>
+        <c:crossAx val="2110748552"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -5988,7 +5991,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="-2072412440"/>
+        <c:axId val="2110748552"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:min val="6.5"/>
@@ -6000,7 +6003,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-2072569192"/>
+        <c:crossAx val="-2072023656"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -6367,11 +6370,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:gapWidth val="150"/>
-        <c:axId val="-2072507720"/>
-        <c:axId val="-2072907080"/>
+        <c:axId val="2110727000"/>
+        <c:axId val="2110743032"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="-2072507720"/>
+        <c:axId val="2110727000"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -6380,7 +6383,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-2072907080"/>
+        <c:crossAx val="2110743032"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -6388,7 +6391,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="-2072907080"/>
+        <c:axId val="2110743032"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -6399,7 +6402,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-2072507720"/>
+        <c:crossAx val="2110727000"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -6769,11 +6772,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="2099410584"/>
-        <c:axId val="2099413592"/>
+        <c:axId val="-2072289400"/>
+        <c:axId val="-2072077368"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="2099410584"/>
+        <c:axId val="-2072289400"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -6782,7 +6785,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="2099413592"/>
+        <c:crossAx val="-2072077368"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -6790,7 +6793,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="2099413592"/>
+        <c:axId val="-2072077368"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -6801,7 +6804,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="2099410584"/>
+        <c:crossAx val="-2072289400"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -7181,11 +7184,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="2099360968"/>
-        <c:axId val="2099363976"/>
+        <c:axId val="-2072009768"/>
+        <c:axId val="-2072963928"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="2099360968"/>
+        <c:axId val="-2072009768"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -7194,7 +7197,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="2099363976"/>
+        <c:crossAx val="-2072963928"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -7202,7 +7205,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="2099363976"/>
+        <c:axId val="-2072963928"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:min val="9.0"/>
@@ -7214,7 +7217,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="2099360968"/>
+        <c:crossAx val="-2072009768"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -7581,11 +7584,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:gapWidth val="150"/>
-        <c:axId val="2099820040"/>
-        <c:axId val="2099760248"/>
+        <c:axId val="-2072777720"/>
+        <c:axId val="-2072951896"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="2099820040"/>
+        <c:axId val="-2072777720"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -7594,7 +7597,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="2099760248"/>
+        <c:crossAx val="-2072951896"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -7602,7 +7605,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="2099760248"/>
+        <c:axId val="-2072951896"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -7613,7 +7616,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="2099820040"/>
+        <c:crossAx val="-2072777720"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -7983,11 +7986,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="-2072562792"/>
-        <c:axId val="-2072504040"/>
+        <c:axId val="-2072015080"/>
+        <c:axId val="-2073011592"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="-2072562792"/>
+        <c:axId val="-2072015080"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -7996,7 +7999,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-2072504040"/>
+        <c:crossAx val="-2073011592"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -8004,7 +8007,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="-2072504040"/>
+        <c:axId val="-2073011592"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -8015,7 +8018,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-2072562792"/>
+        <c:crossAx val="-2072015080"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -8395,11 +8398,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="-2072985896"/>
-        <c:axId val="-2072561480"/>
+        <c:axId val="-2072857256"/>
+        <c:axId val="-2072341768"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="-2072985896"/>
+        <c:axId val="-2072857256"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -8408,7 +8411,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-2072561480"/>
+        <c:crossAx val="-2072341768"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -8416,7 +8419,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="-2072561480"/>
+        <c:axId val="-2072341768"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:min val="10.0"/>
@@ -8428,7 +8431,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-2072985896"/>
+        <c:crossAx val="-2072857256"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -8795,11 +8798,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:gapWidth val="150"/>
-        <c:axId val="-2072206904"/>
-        <c:axId val="-2072863016"/>
+        <c:axId val="-2072594344"/>
+        <c:axId val="-2072683528"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="-2072206904"/>
+        <c:axId val="-2072594344"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -8808,7 +8811,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-2072863016"/>
+        <c:crossAx val="-2072683528"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -8816,7 +8819,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="-2072863016"/>
+        <c:axId val="-2072683528"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -8827,7 +8830,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-2072206904"/>
+        <c:crossAx val="-2072594344"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -9197,11 +9200,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="-2072641992"/>
-        <c:axId val="-2072808840"/>
+        <c:axId val="-2072340088"/>
+        <c:axId val="-2072938248"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="-2072641992"/>
+        <c:axId val="-2072340088"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -9210,7 +9213,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-2072808840"/>
+        <c:crossAx val="-2072938248"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -9218,7 +9221,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="-2072808840"/>
+        <c:axId val="-2072938248"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -9229,7 +9232,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-2072641992"/>
+        <c:crossAx val="-2072340088"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -9609,11 +9612,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="-2072883880"/>
-        <c:axId val="-2072008760"/>
+        <c:axId val="-2072251672"/>
+        <c:axId val="-2072227944"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="-2072883880"/>
+        <c:axId val="-2072251672"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -9622,7 +9625,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-2072008760"/>
+        <c:crossAx val="-2072227944"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -9630,10 +9633,10 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="-2072008760"/>
+        <c:axId val="-2072227944"/>
         <c:scaling>
           <c:orientation val="minMax"/>
-          <c:min val="2.0"/>
+          <c:min val="2.3"/>
         </c:scaling>
         <c:delete val="0"/>
         <c:axPos val="l"/>
@@ -9642,7 +9645,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-2072883880"/>
+        <c:crossAx val="-2072251672"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -10009,11 +10012,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:gapWidth val="150"/>
-        <c:axId val="-2014033464"/>
-        <c:axId val="-2013544088"/>
+        <c:axId val="2110339784"/>
+        <c:axId val="2110635672"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="-2014033464"/>
+        <c:axId val="2110339784"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -10022,7 +10025,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-2013544088"/>
+        <c:crossAx val="2110635672"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -10030,7 +10033,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="-2013544088"/>
+        <c:axId val="2110635672"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -10041,13 +10044,14 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-2014033464"/>
+        <c:crossAx val="2110339784"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
     </c:plotArea>
     <c:legend>
       <c:legendPos val="r"/>
+      <c:layout/>
       <c:overlay val="0"/>
     </c:legend>
     <c:plotVisOnly val="1"/>
@@ -10412,11 +10416,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:gapWidth val="150"/>
-        <c:axId val="-2072999176"/>
-        <c:axId val="-2072702984"/>
+        <c:axId val="-2072141528"/>
+        <c:axId val="-2072211432"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="-2072999176"/>
+        <c:axId val="-2072141528"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -10425,7 +10429,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-2072702984"/>
+        <c:crossAx val="-2072211432"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -10433,7 +10437,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="-2072702984"/>
+        <c:axId val="-2072211432"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -10444,7 +10448,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-2072999176"/>
+        <c:crossAx val="-2072141528"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -10814,11 +10818,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="-2072057576"/>
-        <c:axId val="-2072054568"/>
+        <c:axId val="-2073034696"/>
+        <c:axId val="-2072330952"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="-2072057576"/>
+        <c:axId val="-2073034696"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -10827,7 +10831,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-2072054568"/>
+        <c:crossAx val="-2072330952"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -10835,7 +10839,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="-2072054568"/>
+        <c:axId val="-2072330952"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -10846,7 +10850,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-2072057576"/>
+        <c:crossAx val="-2073034696"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -11226,11 +11230,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="2110541368"/>
-        <c:axId val="2110486664"/>
+        <c:axId val="-2072111416"/>
+        <c:axId val="-2072088008"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="2110541368"/>
+        <c:axId val="-2072111416"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -11239,7 +11243,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="2110486664"/>
+        <c:crossAx val="-2072088008"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -11247,7 +11251,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="2110486664"/>
+        <c:axId val="-2072088008"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:min val="5.0"/>
@@ -11259,7 +11263,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="2110541368"/>
+        <c:crossAx val="-2072111416"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -11626,11 +11630,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:gapWidth val="150"/>
-        <c:axId val="2110390536"/>
-        <c:axId val="2110429176"/>
+        <c:axId val="-2072627256"/>
+        <c:axId val="-2072669544"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="2110390536"/>
+        <c:axId val="-2072627256"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -11639,7 +11643,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="2110429176"/>
+        <c:crossAx val="-2072669544"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -11647,7 +11651,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="2110429176"/>
+        <c:axId val="-2072669544"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -11658,7 +11662,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="2110390536"/>
+        <c:crossAx val="-2072627256"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -11986,11 +11990,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="2109971656"/>
-        <c:axId val="2110359528"/>
+        <c:axId val="2092497848"/>
+        <c:axId val="2092823896"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="2109971656"/>
+        <c:axId val="2092497848"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -11999,7 +12003,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="2110359528"/>
+        <c:crossAx val="2092823896"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -12007,7 +12011,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="2110359528"/>
+        <c:axId val="2092823896"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -12018,7 +12022,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="2109971656"/>
+        <c:crossAx val="2092497848"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -12356,11 +12360,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="2110753992"/>
-        <c:axId val="2110739560"/>
+        <c:axId val="2092421016"/>
+        <c:axId val="2092364408"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="2110753992"/>
+        <c:axId val="2092421016"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -12369,7 +12373,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="2110739560"/>
+        <c:crossAx val="2092364408"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -12377,7 +12381,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="2110739560"/>
+        <c:axId val="2092364408"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:min val="6.0"/>
@@ -12389,7 +12393,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="2110753992"/>
+        <c:crossAx val="2092421016"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -12714,11 +12718,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:gapWidth val="150"/>
-        <c:axId val="2110723048"/>
-        <c:axId val="2110726056"/>
+        <c:axId val="2092926632"/>
+        <c:axId val="2092921352"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="2110723048"/>
+        <c:axId val="2092926632"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -12727,7 +12731,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="2110726056"/>
+        <c:crossAx val="2092921352"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -12735,7 +12739,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="2110726056"/>
+        <c:axId val="2092921352"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -12746,7 +12750,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="2110723048"/>
+        <c:crossAx val="2092926632"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -13116,11 +13120,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="2099848360"/>
-        <c:axId val="2099821624"/>
+        <c:axId val="2092865272"/>
+        <c:axId val="2092868248"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="2099848360"/>
+        <c:axId val="2092865272"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -13129,7 +13133,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="2099821624"/>
+        <c:crossAx val="2092868248"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -13137,7 +13141,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="2099821624"/>
+        <c:axId val="2092868248"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -13148,7 +13152,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="2099848360"/>
+        <c:crossAx val="2092865272"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -13528,11 +13532,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="2099971512"/>
-        <c:axId val="2099908104"/>
+        <c:axId val="2092817096"/>
+        <c:axId val="2092814968"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="2099971512"/>
+        <c:axId val="2092817096"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -13541,7 +13545,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="2099908104"/>
+        <c:crossAx val="2092814968"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -13549,7 +13553,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="2099908104"/>
+        <c:axId val="2092814968"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:min val="3.0"/>
@@ -13561,7 +13565,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="2099971512"/>
+        <c:crossAx val="2092817096"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -13928,11 +13932,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:gapWidth val="150"/>
-        <c:axId val="2099954888"/>
-        <c:axId val="2100021784"/>
+        <c:axId val="2092796792"/>
+        <c:axId val="2092785784"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="2099954888"/>
+        <c:axId val="2092796792"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -13941,7 +13945,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="2100021784"/>
+        <c:crossAx val="2092785784"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -13949,7 +13953,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="2100021784"/>
+        <c:axId val="2092785784"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -13960,7 +13964,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="2099954888"/>
+        <c:crossAx val="2092796792"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -14222,11 +14226,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="-2013807240"/>
-        <c:axId val="-2013804296"/>
+        <c:axId val="2109902472"/>
+        <c:axId val="2109868296"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="-2013807240"/>
+        <c:axId val="2109902472"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -14235,7 +14239,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-2013804296"/>
+        <c:crossAx val="2109868296"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -14244,7 +14248,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="-2013804296"/>
+        <c:axId val="2109868296"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -14255,7 +14259,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-2013807240"/>
+        <c:crossAx val="2109902472"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -14625,11 +14629,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="2110654536"/>
-        <c:axId val="2110651864"/>
+        <c:axId val="2092742072"/>
+        <c:axId val="2092745080"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="2110654536"/>
+        <c:axId val="2092742072"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -14638,7 +14642,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="2110651864"/>
+        <c:crossAx val="2092745080"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -14646,7 +14650,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="2110651864"/>
+        <c:axId val="2092745080"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -14657,7 +14661,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="2110654536"/>
+        <c:crossAx val="2092742072"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -15037,11 +15041,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="2110499208"/>
-        <c:axId val="2110489208"/>
+        <c:axId val="2092691560"/>
+        <c:axId val="2092687688"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="2110499208"/>
+        <c:axId val="2092691560"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -15050,7 +15054,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="2110489208"/>
+        <c:crossAx val="2092687688"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -15058,7 +15062,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="2110489208"/>
+        <c:axId val="2092687688"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:min val="3.0"/>
@@ -15070,7 +15074,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="2110499208"/>
+        <c:crossAx val="2092691560"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -15437,11 +15441,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:gapWidth val="150"/>
-        <c:axId val="2110427544"/>
-        <c:axId val="2110415688"/>
+        <c:axId val="2092662488"/>
+        <c:axId val="2092665496"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="2110427544"/>
+        <c:axId val="2092662488"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -15450,7 +15454,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="2110415688"/>
+        <c:crossAx val="2092665496"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -15458,7 +15462,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="2110415688"/>
+        <c:axId val="2092665496"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -15469,7 +15473,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="2110427544"/>
+        <c:crossAx val="2092662488"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -15839,11 +15843,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="2110255784"/>
-        <c:axId val="2110250888"/>
+        <c:axId val="2092624440"/>
+        <c:axId val="2092627448"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="2110255784"/>
+        <c:axId val="2092624440"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -15852,7 +15856,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="2110250888"/>
+        <c:crossAx val="2092627448"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -15860,7 +15864,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="2110250888"/>
+        <c:axId val="2092627448"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -15871,7 +15875,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="2110255784"/>
+        <c:crossAx val="2092624440"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -16251,11 +16255,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="2110165736"/>
-        <c:axId val="2110153720"/>
+        <c:axId val="2092565320"/>
+        <c:axId val="2092557256"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="2110165736"/>
+        <c:axId val="2092565320"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -16264,7 +16268,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="2110153720"/>
+        <c:crossAx val="2092557256"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -16272,9 +16276,10 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="2110153720"/>
+        <c:axId val="2092557256"/>
         <c:scaling>
           <c:orientation val="minMax"/>
+          <c:min val="4.0"/>
         </c:scaling>
         <c:delete val="0"/>
         <c:axPos val="l"/>
@@ -16283,7 +16288,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="2110165736"/>
+        <c:crossAx val="2092565320"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -16650,11 +16655,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:gapWidth val="150"/>
-        <c:axId val="2110117176"/>
-        <c:axId val="2110102920"/>
+        <c:axId val="2092538312"/>
+        <c:axId val="2092533672"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="2110117176"/>
+        <c:axId val="2092538312"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -16663,7 +16668,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="2110102920"/>
+        <c:crossAx val="2092533672"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -16671,7 +16676,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="2110102920"/>
+        <c:axId val="2092533672"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -16682,7 +16687,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="2110117176"/>
+        <c:crossAx val="2092538312"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -17052,11 +17057,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="2110025448"/>
-        <c:axId val="2110011064"/>
+        <c:axId val="2092484488"/>
+        <c:axId val="2092487496"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="2110025448"/>
+        <c:axId val="2092484488"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -17065,7 +17070,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="2110011064"/>
+        <c:crossAx val="2092487496"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -17073,7 +17078,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="2110011064"/>
+        <c:axId val="2092487496"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -17084,7 +17089,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="2110025448"/>
+        <c:crossAx val="2092484488"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -17464,11 +17469,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="2109928584"/>
-        <c:axId val="2109924728"/>
+        <c:axId val="2092432152"/>
+        <c:axId val="2092427192"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="2109928584"/>
+        <c:axId val="2092432152"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -17477,7 +17482,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="2109924728"/>
+        <c:crossAx val="2092427192"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -17485,7 +17490,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="2109924728"/>
+        <c:axId val="2092427192"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:min val="8.0"/>
@@ -17497,7 +17502,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="2109928584"/>
+        <c:crossAx val="2092432152"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -17864,11 +17869,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:gapWidth val="150"/>
-        <c:axId val="2109890168"/>
-        <c:axId val="2109893144"/>
+        <c:axId val="2092400024"/>
+        <c:axId val="2092394536"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="2109890168"/>
+        <c:axId val="2092400024"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -17877,7 +17882,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="2109893144"/>
+        <c:crossAx val="2092394536"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -17885,7 +17890,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="2109893144"/>
+        <c:axId val="2092394536"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -17896,7 +17901,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="2109890168"/>
+        <c:crossAx val="2092400024"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -18266,11 +18271,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="2100037112"/>
-        <c:axId val="2100119448"/>
+        <c:axId val="2092314632"/>
+        <c:axId val="2092313528"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="2100037112"/>
+        <c:axId val="2092314632"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -18279,7 +18284,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="2100119448"/>
+        <c:crossAx val="2092313528"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -18287,7 +18292,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="2100119448"/>
+        <c:axId val="2092313528"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -18298,7 +18303,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="2100037112"/>
+        <c:crossAx val="2092314632"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -18570,11 +18575,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="-2014218680"/>
-        <c:axId val="2099276568"/>
+        <c:axId val="2109878440"/>
+        <c:axId val="2110699720"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="-2014218680"/>
+        <c:axId val="2109878440"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -18583,7 +18588,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="2099276568"/>
+        <c:crossAx val="2110699720"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -18592,7 +18597,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="2099276568"/>
+        <c:axId val="2110699720"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:min val="40.0"/>
@@ -18604,7 +18609,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-2014218680"/>
+        <c:crossAx val="2109878440"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -18984,11 +18989,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="2100162200"/>
-        <c:axId val="2100123832"/>
+        <c:axId val="2092252904"/>
+        <c:axId val="2092247336"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="2100162200"/>
+        <c:axId val="2092252904"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -18997,7 +19002,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="2100123832"/>
+        <c:crossAx val="2092247336"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -19005,10 +19010,10 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="2100123832"/>
+        <c:axId val="2092247336"/>
         <c:scaling>
           <c:orientation val="minMax"/>
-          <c:min val="2.0"/>
+          <c:min val="2.6"/>
         </c:scaling>
         <c:delete val="0"/>
         <c:axPos val="l"/>
@@ -19017,7 +19022,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="2100162200"/>
+        <c:crossAx val="2092252904"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -19384,11 +19389,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:gapWidth val="150"/>
-        <c:axId val="2100276168"/>
-        <c:axId val="2100264808"/>
+        <c:axId val="2092215848"/>
+        <c:axId val="2092213672"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="2100276168"/>
+        <c:axId val="2092215848"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -19397,7 +19402,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="2100264808"/>
+        <c:crossAx val="2092213672"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -19405,7 +19410,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="2100264808"/>
+        <c:axId val="2092213672"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -19416,7 +19421,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="2100276168"/>
+        <c:crossAx val="2092215848"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -19786,11 +19791,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="2109848328"/>
-        <c:axId val="2109846040"/>
+        <c:axId val="2092160024"/>
+        <c:axId val="2092155688"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="2109848328"/>
+        <c:axId val="2092160024"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -19799,7 +19804,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="2109846040"/>
+        <c:crossAx val="2092155688"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -19807,7 +19812,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="2109846040"/>
+        <c:axId val="2092155688"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -19818,7 +19823,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="2109848328"/>
+        <c:crossAx val="2092160024"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -20198,11 +20203,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="2109821832"/>
-        <c:axId val="2109795112"/>
+        <c:axId val="2092103960"/>
+        <c:axId val="2092102120"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="2109821832"/>
+        <c:axId val="2092103960"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -20211,7 +20216,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="2109795112"/>
+        <c:crossAx val="2092102120"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -20219,7 +20224,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="2109795112"/>
+        <c:axId val="2092102120"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:min val="4.5"/>
@@ -20231,7 +20236,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="2109821832"/>
+        <c:crossAx val="2092103960"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -20598,11 +20603,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:gapWidth val="150"/>
-        <c:axId val="2109786008"/>
-        <c:axId val="2109773080"/>
+        <c:axId val="2092076440"/>
+        <c:axId val="2092072840"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="2109786008"/>
+        <c:axId val="2092076440"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -20611,7 +20616,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="2109773080"/>
+        <c:crossAx val="2092072840"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -20619,7 +20624,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="2109773080"/>
+        <c:axId val="2092072840"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -20630,7 +20635,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="2109786008"/>
+        <c:crossAx val="2092076440"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -20958,11 +20963,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="2092298424"/>
-        <c:axId val="2092389560"/>
+        <c:axId val="2092012088"/>
+        <c:axId val="2092015064"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="2092298424"/>
+        <c:axId val="2092012088"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -20971,7 +20976,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="2092389560"/>
+        <c:crossAx val="2092015064"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -20979,7 +20984,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="2092389560"/>
+        <c:axId val="2092015064"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -20990,7 +20995,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="2092298424"/>
+        <c:crossAx val="2092012088"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -21328,11 +21333,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="2092931608"/>
-        <c:axId val="2092921576"/>
+        <c:axId val="2091971176"/>
+        <c:axId val="2091964408"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="2092931608"/>
+        <c:axId val="2091971176"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -21341,7 +21346,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="2092921576"/>
+        <c:crossAx val="2091964408"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -21349,7 +21354,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="2092921576"/>
+        <c:axId val="2091964408"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:min val="450.0"/>
@@ -21361,7 +21366,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="2092931608"/>
+        <c:crossAx val="2091971176"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -21686,11 +21691,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:gapWidth val="150"/>
-        <c:axId val="2092900472"/>
-        <c:axId val="2092893960"/>
+        <c:axId val="2091956536"/>
+        <c:axId val="2091959544"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="2092900472"/>
+        <c:axId val="2091956536"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -21699,7 +21704,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="2092893960"/>
+        <c:crossAx val="2091959544"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -21707,7 +21712,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="2092893960"/>
+        <c:axId val="2091959544"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -21718,7 +21723,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="2092900472"/>
+        <c:crossAx val="2091956536"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -22031,11 +22036,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="2092848888"/>
-        <c:axId val="2092851896"/>
+        <c:axId val="2063909128"/>
+        <c:axId val="2063726504"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="2092848888"/>
+        <c:axId val="2063909128"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -22044,7 +22049,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="2092851896"/>
+        <c:crossAx val="2063726504"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -22052,7 +22057,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="2092851896"/>
+        <c:axId val="2063726504"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -22063,7 +22068,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="2092848888"/>
+        <c:crossAx val="2063909128"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -22386,11 +22391,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="2092798168"/>
-        <c:axId val="2092792440"/>
+        <c:axId val="2064586104"/>
+        <c:axId val="2064589112"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="2092798168"/>
+        <c:axId val="2064586104"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -22399,7 +22404,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="2092792440"/>
+        <c:crossAx val="2064589112"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -22407,7 +22412,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="2092792440"/>
+        <c:axId val="2064589112"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:min val="15.0"/>
@@ -22419,7 +22424,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="2092798168"/>
+        <c:crossAx val="2064586104"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -22678,11 +22683,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:gapWidth val="150"/>
-        <c:axId val="-2013667672"/>
-        <c:axId val="-2013664664"/>
+        <c:axId val="-2072063240"/>
+        <c:axId val="2110700616"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="-2013667672"/>
+        <c:axId val="-2072063240"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -22691,7 +22696,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-2013664664"/>
+        <c:crossAx val="2110700616"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -22700,7 +22705,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="-2013664664"/>
+        <c:axId val="2110700616"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -22711,7 +22716,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-2013667672"/>
+        <c:crossAx val="-2072063240"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -23021,11 +23026,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:gapWidth val="150"/>
-        <c:axId val="2092769016"/>
-        <c:axId val="2092764424"/>
+        <c:axId val="2064565992"/>
+        <c:axId val="2064556744"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="2092769016"/>
+        <c:axId val="2064565992"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -23034,7 +23039,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="2092764424"/>
+        <c:crossAx val="2064556744"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -23042,7 +23047,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="2092764424"/>
+        <c:axId val="2064556744"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -23053,7 +23058,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="2092769016"/>
+        <c:crossAx val="2064565992"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -23351,11 +23356,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="-2013102472"/>
-        <c:axId val="-2013834216"/>
+        <c:axId val="-2072019544"/>
+        <c:axId val="-2072264952"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="-2013102472"/>
+        <c:axId val="-2072019544"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -23364,7 +23369,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-2013834216"/>
+        <c:crossAx val="-2072264952"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -23372,7 +23377,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="-2013834216"/>
+        <c:axId val="-2072264952"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -23383,7 +23388,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-2013102472"/>
+        <c:crossAx val="-2072019544"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -23691,11 +23696,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="-2012268088"/>
-        <c:axId val="-2013128600"/>
+        <c:axId val="-2072638984"/>
+        <c:axId val="-2072949896"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="-2012268088"/>
+        <c:axId val="-2072638984"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -23704,7 +23709,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-2013128600"/>
+        <c:crossAx val="-2072949896"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -23712,7 +23717,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="-2013128600"/>
+        <c:axId val="-2072949896"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:min val="16.5"/>
@@ -23724,7 +23729,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-2012268088"/>
+        <c:crossAx val="-2072638984"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -24019,11 +24024,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:gapWidth val="150"/>
-        <c:axId val="-2012802568"/>
-        <c:axId val="-2097114536"/>
+        <c:axId val="2110452504"/>
+        <c:axId val="2110438632"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="-2012802568"/>
+        <c:axId val="2110452504"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -24032,7 +24037,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-2097114536"/>
+        <c:crossAx val="2110438632"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -24040,7 +24045,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="-2097114536"/>
+        <c:axId val="2110438632"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -24051,7 +24056,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-2012802568"/>
+        <c:crossAx val="2110452504"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -26333,7 +26338,7 @@
   </sheetPr>
   <dimension ref="A2:DA16"/>
   <sheetViews>
-    <sheetView topLeftCell="CS1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="DA7" sqref="DA7"/>
     </sheetView>
   </sheetViews>
@@ -28544,7 +28549,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A2:DA14"/>
   <sheetViews>
-    <sheetView topLeftCell="CO2" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="DA7" sqref="DA7"/>
     </sheetView>
   </sheetViews>
@@ -30708,7 +30713,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A2:DA15"/>
   <sheetViews>
-    <sheetView topLeftCell="CM1" workbookViewId="0">
+    <sheetView topLeftCell="A7" workbookViewId="0">
       <selection activeCell="DA7" sqref="DA7"/>
     </sheetView>
   </sheetViews>
@@ -32878,7 +32883,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A2:CM15"/>
   <sheetViews>
-    <sheetView topLeftCell="BW1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="CM7" sqref="CM7"/>
     </sheetView>
   </sheetViews>
@@ -34760,7 +34765,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A2:DA18"/>
   <sheetViews>
-    <sheetView topLeftCell="CM1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="DA7" sqref="DA7"/>
     </sheetView>
   </sheetViews>
@@ -36965,7 +36970,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A2:DA15"/>
   <sheetViews>
-    <sheetView topLeftCell="CM2" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="DA7" sqref="DA7"/>
     </sheetView>
   </sheetViews>
@@ -39170,8 +39175,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A2:DA14"/>
   <sheetViews>
-    <sheetView topLeftCell="CL1" workbookViewId="0">
-      <selection activeCell="DA7" sqref="DA7"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E3" sqref="E3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -39188,11 +39193,11 @@
         <v>7</v>
       </c>
       <c r="E2">
-        <v>162.38999999999999</v>
+        <v>178.53</v>
       </c>
       <c r="F2">
         <f>E2*10000</f>
-        <v>1623899.9999999998</v>
+        <v>1785300</v>
       </c>
     </row>
     <row r="3" spans="1:105">
@@ -40449,7 +40454,7 @@
     <row r="8" spans="1:105">
       <c r="A8" s="8">
         <f>B8/F2</f>
-        <v>1.6142059899173545E-3</v>
+        <v>1.4682737394425538E-3</v>
       </c>
       <c r="B8" s="7">
         <f>SUM(D8:MI8)</f>
@@ -41341,7 +41346,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A2:DA14"/>
   <sheetViews>
-    <sheetView topLeftCell="CN1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="DA7" sqref="DA7"/>
     </sheetView>
   </sheetViews>
@@ -43503,8 +43508,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A2:DA14"/>
   <sheetViews>
-    <sheetView topLeftCell="CL1" workbookViewId="0">
-      <selection activeCell="DA7" sqref="DA7"/>
+    <sheetView topLeftCell="A14" workbookViewId="0">
+      <selection activeCell="E3" sqref="E3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -43521,11 +43526,11 @@
         <v>7</v>
       </c>
       <c r="E2">
-        <v>18.72</v>
+        <v>19.34</v>
       </c>
       <c r="F2">
         <f>E2*10000</f>
-        <v>187200</v>
+        <v>193400</v>
       </c>
     </row>
     <row r="3" spans="1:105">
@@ -44782,7 +44787,7 @@
     <row r="8" spans="1:105">
       <c r="A8" s="8">
         <f>B8/F2</f>
-        <v>-2.7068938796662893E-2</v>
+        <v>-2.6201165164091485E-2</v>
       </c>
       <c r="B8" s="7">
         <f>SUM(D8:MI8)</f>
@@ -45662,7 +45667,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A2:DA14"/>
   <sheetViews>
-    <sheetView topLeftCell="CK1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="DA7" sqref="DA7"/>
     </sheetView>
   </sheetViews>
@@ -47821,7 +47826,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A2:CM13"/>
   <sheetViews>
-    <sheetView topLeftCell="BW1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="CM7" sqref="CM7"/>
     </sheetView>
   </sheetViews>
@@ -49689,7 +49694,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:BQ45"/>
   <sheetViews>
-    <sheetView topLeftCell="BG1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="BQ7" sqref="BQ7"/>
     </sheetView>
   </sheetViews>
@@ -52120,8 +52125,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A2:CH13"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="BW1" workbookViewId="0">
-      <selection activeCell="CH7" sqref="CH7"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E3" sqref="E3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -52138,11 +52143,11 @@
         <v>7</v>
       </c>
       <c r="E2">
-        <v>3.3</v>
+        <v>7.83</v>
       </c>
       <c r="F2">
         <f>E2*10000</f>
-        <v>33000</v>
+        <v>78300</v>
       </c>
     </row>
     <row r="3" spans="1:86">
@@ -53171,7 +53176,7 @@
     <row r="8" spans="1:86">
       <c r="A8" s="8">
         <f>B8/F2</f>
-        <v>2.5979252872820589E-3</v>
+        <v>1.0949110406169597E-3</v>
       </c>
       <c r="B8" s="7">
         <f>SUM(D8:MI8)</f>
@@ -54150,7 +54155,7 @@
   </sheetPr>
   <dimension ref="A2:CD15"/>
   <sheetViews>
-    <sheetView topLeftCell="BQ1" workbookViewId="0">
+    <sheetView topLeftCell="BP1" workbookViewId="0">
       <selection activeCell="CE5" sqref="CE5"/>
     </sheetView>
   </sheetViews>
@@ -55868,7 +55873,7 @@
   </sheetPr>
   <dimension ref="A2:DA19"/>
   <sheetViews>
-    <sheetView topLeftCell="CP1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="DA7" sqref="DA7"/>
     </sheetView>
   </sheetViews>
@@ -58115,8 +58120,8 @@
   </sheetPr>
   <dimension ref="A2:CN15"/>
   <sheetViews>
-    <sheetView topLeftCell="CC1" workbookViewId="0">
-      <selection activeCell="CN7" sqref="CN7"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E3" sqref="E3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -58133,11 +58138,11 @@
         <v>7</v>
       </c>
       <c r="E2">
-        <v>11.74</v>
+        <v>11.94</v>
       </c>
       <c r="F2">
         <f>E2*10000</f>
-        <v>117400</v>
+        <v>119400</v>
       </c>
     </row>
     <row r="3" spans="1:92">
@@ -59238,7 +59243,7 @@
     <row r="8" spans="1:92">
       <c r="A8" s="8">
         <f>B8/F2</f>
-        <v>1.6285423451739452E-2</v>
+        <v>1.6012635789231251E-2</v>
       </c>
       <c r="B8" s="7">
         <f>SUM(D8:MI8)</f>
@@ -60033,7 +60038,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A2:DA17"/>
   <sheetViews>
-    <sheetView topLeftCell="CP1" workbookViewId="0">
+    <sheetView topLeftCell="A11" workbookViewId="0">
       <selection activeCell="DA7" sqref="DA7"/>
     </sheetView>
   </sheetViews>
@@ -62237,7 +62242,7 @@
   </sheetPr>
   <dimension ref="A2:DA17"/>
   <sheetViews>
-    <sheetView topLeftCell="CN1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="DA7" sqref="DA7"/>
     </sheetView>
   </sheetViews>
@@ -64475,8 +64480,8 @@
   </sheetPr>
   <dimension ref="A2:DA20"/>
   <sheetViews>
-    <sheetView topLeftCell="CO1" workbookViewId="0">
-      <selection activeCell="DA7" sqref="DA7"/>
+    <sheetView topLeftCell="A8" workbookViewId="0">
+      <selection activeCell="E3" sqref="E3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -64493,11 +64498,11 @@
         <v>7</v>
       </c>
       <c r="E2">
-        <v>9.36</v>
+        <v>9.4700000000000006</v>
       </c>
       <c r="F2">
         <f>E2*10000</f>
-        <v>93600</v>
+        <v>94700</v>
       </c>
     </row>
     <row r="3" spans="1:105">
@@ -65754,7 +65759,7 @@
     <row r="8" spans="1:105">
       <c r="A8" s="8">
         <f>B8/F2</f>
-        <v>2.9297765156941054E-2</v>
+        <v>2.8957453206860429E-2</v>
       </c>
       <c r="B8" s="7">
         <f>SUM(D8:MI8)</f>
@@ -66683,7 +66688,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A2:DA14"/>
   <sheetViews>
-    <sheetView topLeftCell="CN1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="DA7" sqref="DA7"/>
     </sheetView>
   </sheetViews>

</xml_diff>